<commit_message>
Change names of Chart and Inter sheets in template to allow for charts of other billions to be included at a later stage
</commit_message>
<xml_diff>
--- a/inst/extdata/country_summary_template.xlsx
+++ b/inst/extdata/country_summary_template.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7399C187-00D2-41E1-AE45-755EE1FDF2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD0F3D1-26DB-4B80-B258-ACB64250A254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="17640" tabRatio="601" activeTab="4" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="17640" tabRatio="601" activeTab="3" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="11" r:id="rId1"/>
-    <sheet name="Chart" sheetId="6" r:id="rId2"/>
+    <sheet name="HPOP_Chart" sheetId="6" r:id="rId2"/>
     <sheet name="Time Series" sheetId="8" r:id="rId3"/>
-    <sheet name="Inter" sheetId="5" r:id="rId4"/>
+    <sheet name="HPOP_Inter" sheetId="5" r:id="rId4"/>
     <sheet name="Indicator List" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -310,7 +310,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,7 +705,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Inter!$E$2</c:f>
+              <c:f>HPOP_Inter!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -761,7 +761,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Inter!$G$3:$G$19</c:f>
+                <c:f>HPOP_Inter!$G$3:$G$19</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="17"/>
@@ -829,7 +829,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Inter!$B$3:$B$19</c:f>
+              <c:f>HPOP_Inter!$B$3:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -889,7 +889,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Inter!$E$3:$E$19</c:f>
+              <c:f>HPOP_Inter!$E$3:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -959,7 +959,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Inter!$F$2</c:f>
+              <c:f>HPOP_Inter!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -997,7 +997,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Inter!$H$3:$H$19</c:f>
+                <c:f>HPOP_Inter!$H$3:$H$19</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="17"/>
@@ -1057,7 +1057,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Inter!$H$3:$H$19</c:f>
+                <c:f>HPOP_Inter!$H$3:$H$19</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="17"/>
@@ -1125,7 +1125,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Inter!$B$3:$B$19</c:f>
+              <c:f>HPOP_Inter!$B$3:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1185,7 +1185,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Inter!$F$3:$F$19</c:f>
+              <c:f>HPOP_Inter!$F$3:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1255,7 +1255,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Inter!$I$2</c:f>
+              <c:f>HPOP_Inter!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1753,7 +1753,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F509903E-B556-4D14-89CC-FC17B1FAEEEC}" type="CELLRANGE">
+                    <a:fld id="{ADFF2E4B-3197-43E2-9DEF-B3CA1E7F780B}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1837,7 +1837,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Inter!$B$3:$B$19</c:f>
+              <c:f>HPOP_Inter!$B$3:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1897,7 +1897,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Inter!$I$3:$I$19</c:f>
+              <c:f>HPOP_Inter!$I$3:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1959,7 +1959,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Inter!$J$3:$J$19</c15:f>
+                <c15:f>HPOP_Inter!$J$3:$J$19</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="17"/>
                   <c:pt idx="0">
@@ -2530,7 +2530,7 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -2555,79 +2555,79 @@
     <col min="23" max="24" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
-    <row r="2" customFormat="1" ht="30" customHeight="1"/>
-    <row r="3" customFormat="1" ht="15" customHeight="1"/>
-    <row r="4" customFormat="1" ht="15" customHeight="1"/>
-    <row r="5" customFormat="1" ht="15" customHeight="1"/>
-    <row r="6" customFormat="1" ht="15" customHeight="1"/>
-    <row r="7" customFormat="1" ht="30" customHeight="1"/>
-    <row r="8" customFormat="1" ht="15" customHeight="1"/>
-    <row r="9" customFormat="1" ht="30" customHeight="1"/>
-    <row r="10" customFormat="1" ht="30" customHeight="1"/>
-    <row r="11" customFormat="1" ht="30" customHeight="1"/>
-    <row r="12" customFormat="1" ht="30" customHeight="1"/>
-    <row r="13" customFormat="1" ht="30" customHeight="1"/>
-    <row r="14" customFormat="1" ht="30" customHeight="1"/>
-    <row r="15" customFormat="1" ht="30" customHeight="1"/>
-    <row r="16" customFormat="1" ht="30" customHeight="1"/>
-    <row r="17" customFormat="1" ht="30" customHeight="1"/>
-    <row r="18" customFormat="1" ht="30" customHeight="1"/>
-    <row r="19" customFormat="1" ht="30" customHeight="1"/>
-    <row r="20" customFormat="1" ht="30" customHeight="1"/>
-    <row r="21" customFormat="1" ht="30" customHeight="1"/>
-    <row r="22" customFormat="1" ht="30" customHeight="1"/>
-    <row r="23" customFormat="1" ht="30" customHeight="1"/>
-    <row r="24" customFormat="1" ht="30" customHeight="1"/>
-    <row r="25" customFormat="1" ht="30" customHeight="1"/>
-    <row r="26" customFormat="1" ht="15" customHeight="1"/>
-    <row r="27" customFormat="1" ht="15" customHeight="1"/>
-    <row r="28" customFormat="1" ht="15" customHeight="1"/>
-    <row r="29" customFormat="1" ht="15" customHeight="1"/>
-    <row r="30" customFormat="1" ht="15" customHeight="1"/>
-    <row r="31" customFormat="1" ht="15" customHeight="1"/>
-    <row r="32" customFormat="1" ht="15" customHeight="1"/>
-    <row r="33" customFormat="1" ht="15" customHeight="1"/>
-    <row r="34" customFormat="1" ht="15" customHeight="1"/>
-    <row r="35" customFormat="1" ht="15" customHeight="1"/>
-    <row r="36" customFormat="1" ht="15" customHeight="1"/>
-    <row r="37" customFormat="1" ht="15" customHeight="1"/>
-    <row r="38" customFormat="1" ht="15" customHeight="1"/>
-    <row r="39" customFormat="1" ht="15" customHeight="1"/>
-    <row r="40" customFormat="1" ht="15" customHeight="1"/>
-    <row r="41" customFormat="1" ht="15" customHeight="1"/>
-    <row r="42" customFormat="1" ht="15" customHeight="1"/>
-    <row r="43" customFormat="1" ht="15" customHeight="1"/>
-    <row r="44" customFormat="1" ht="15" customHeight="1"/>
-    <row r="45" customFormat="1" ht="15" customHeight="1"/>
-    <row r="46" customFormat="1" ht="15" customHeight="1"/>
-    <row r="47" customFormat="1" ht="15" customHeight="1"/>
-    <row r="48" customFormat="1" ht="15" customHeight="1"/>
-    <row r="49" customFormat="1" ht="15" customHeight="1"/>
-    <row r="50" customFormat="1" ht="15" customHeight="1"/>
-    <row r="51" customFormat="1" ht="15" customHeight="1"/>
-    <row r="52" customFormat="1" ht="15" customHeight="1"/>
-    <row r="53" customFormat="1" ht="15" customHeight="1"/>
-    <row r="54" customFormat="1" ht="15" customHeight="1"/>
-    <row r="55" customFormat="1" ht="15" customHeight="1"/>
-    <row r="56" customFormat="1" ht="15" customHeight="1"/>
-    <row r="57" customFormat="1" ht="15" customHeight="1"/>
-    <row r="58" customFormat="1" ht="15" customHeight="1"/>
-    <row r="59" customFormat="1" ht="15" customHeight="1"/>
-    <row r="60" customFormat="1" ht="15" customHeight="1"/>
-    <row r="61" customFormat="1" ht="15" customHeight="1"/>
-    <row r="62" customFormat="1" ht="15" customHeight="1"/>
-    <row r="63" customFormat="1" ht="15" customHeight="1"/>
-    <row r="64" customFormat="1" ht="15" customHeight="1"/>
-    <row r="65" customFormat="1" ht="15" customHeight="1"/>
-    <row r="66" customFormat="1" ht="15" customHeight="1"/>
-    <row r="67" customFormat="1" ht="15" customHeight="1"/>
-    <row r="68" customFormat="1" ht="15" customHeight="1"/>
-    <row r="69" customFormat="1" ht="15" customHeight="1"/>
-    <row r="70" customFormat="1" ht="15" customHeight="1"/>
-    <row r="71" customFormat="1" ht="15" customHeight="1"/>
-    <row r="72" customFormat="1" ht="15" customHeight="1"/>
-    <row r="73" customFormat="1" ht="15" customHeight="1"/>
+    <row r="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="40" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2642,85 +2642,85 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="21" spans="2:20" ht="33.75" customHeight="1"/>
-    <row r="22" spans="2:20" ht="162" customHeight="1">
+    <row r="21" spans="2:20" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:20" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="6" t="str">
-        <f>Inter!A3</f>
+        <f>HPOP_Inter!A3</f>
         <v>Children not stunted</v>
       </c>
       <c r="D22" s="6" t="str">
-        <f>Inter!A4</f>
+        <f>HPOP_Inter!A4</f>
         <v>Children not wasted</v>
       </c>
       <c r="E22" s="6" t="str">
-        <f>Inter!A5</f>
+        <f>HPOP_Inter!A5</f>
         <v>Children not overweight</v>
       </c>
       <c r="F22" s="6" t="str">
-        <f>Inter!A6</f>
+        <f>HPOP_Inter!A6</f>
         <v>Developmentally on track under 5</v>
       </c>
       <c r="G22" s="6" t="str">
-        <f>Inter!A7</f>
+        <f>HPOP_Inter!A7</f>
         <v>Children not obese</v>
       </c>
       <c r="H22" s="6" t="str">
-        <f>Inter!A8</f>
+        <f>HPOP_Inter!A8</f>
         <v>Reduced partner violence</v>
       </c>
       <c r="I22" s="6" t="str">
-        <f>Inter!A9</f>
+        <f>HPOP_Inter!A9</f>
         <v>Reduced child violence</v>
       </c>
       <c r="J22" s="6" t="str">
-        <f>Inter!A10</f>
+        <f>HPOP_Inter!A10</f>
         <v>Reduced suicide attempts</v>
       </c>
       <c r="K22" s="6" t="str">
-        <f>Inter!A11</f>
+        <f>HPOP_Inter!A11</f>
         <v>Road safety</v>
       </c>
       <c r="L22" s="6" t="str">
-        <f>Inter!A12</f>
+        <f>HPOP_Inter!A12</f>
         <v>Safely managed water</v>
       </c>
       <c r="M22" s="6" t="str">
-        <f>Inter!A13</f>
+        <f>HPOP_Inter!A13</f>
         <v>Safely managed sanitation</v>
       </c>
       <c r="N22" s="6" t="str">
-        <f>Inter!A14</f>
+        <f>HPOP_Inter!A14</f>
         <v>Clean household fuels</v>
       </c>
       <c r="O22" s="6" t="str">
-        <f>Inter!A15</f>
+        <f>HPOP_Inter!A15</f>
         <v>Reduced alcohol use</v>
       </c>
       <c r="P22" s="6" t="str">
-        <f>Inter!A16</f>
+        <f>HPOP_Inter!A16</f>
         <v>Ambient air quality</v>
       </c>
       <c r="Q22" s="6" t="str">
-        <f>Inter!A17</f>
+        <f>HPOP_Inter!A17</f>
         <v>Tobacco non-use</v>
       </c>
       <c r="R22" s="6" t="str">
-        <f>Inter!A18</f>
+        <f>HPOP_Inter!A18</f>
         <v>Adults not obese</v>
       </c>
       <c r="S22" s="6" t="str">
-        <f>Inter!A19</f>
+        <f>HPOP_Inter!A19</f>
         <v>Healthy fats</v>
       </c>
       <c r="T22" s="7"/>
     </row>
-    <row r="23" spans="2:20">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:20">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -2739,13 +2739,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.85546875" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="18" customFormat="1">
+    <row r="1" spans="1:39" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
@@ -2772,7 +2772,7 @@
       <c r="Z1" s="21"/>
       <c r="AA1" s="22"/>
     </row>
-    <row r="2" spans="1:39" s="18" customFormat="1" ht="21">
+    <row r="2" spans="1:39" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>41</v>
       </c>
@@ -2801,7 +2801,7 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
     </row>
-    <row r="3" spans="1:39" s="18" customFormat="1">
+    <row r="3" spans="1:39" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="24"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
@@ -2828,7 +2828,7 @@
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="35" t="s">
         <v>40</v>
@@ -2873,7 +2873,7 @@
       <c r="AL4" s="18"/>
       <c r="AM4" s="18"/>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="36"/>
       <c r="C5" s="27">
@@ -2976,16 +2976,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B9ADA0-9FC1-425A-BF34-F0C669B1F93B}">
   <dimension ref="A2:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="23.25">
+    <row r="2" spans="1:12" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="2"/>
       <c r="C2" s="10">
@@ -3013,7 +3013,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>33</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="L4" s="33"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>23</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>26</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>28</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>29</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>30</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>31</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>32</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
     </row>
   </sheetData>
@@ -3707,11 +3707,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF07AF5-FD4F-4F8B-8ACA-4EDEF61AF714}">
   <dimension ref="A2:H23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
@@ -3723,7 +3723,7 @@
     <col min="8" max="8" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="30" customHeight="1">
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="17" t="s">
         <v>34</v>
       </c>
@@ -3734,7 +3734,7 @@
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
       <c r="C3" s="15"/>
       <c r="D3" s="9"/>
@@ -3743,7 +3743,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="32" t="s">
         <v>44</v>
@@ -3764,7 +3764,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" t="s">
         <v>50</v>
@@ -3785,7 +3785,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>53</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>55</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>57</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>59</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>61</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>63</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>65</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>68</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>70</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>72</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>74</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>77</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>80</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>82</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>57</v>
       </c>
@@ -4085,13 +4085,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21"/>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C22"/>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
         <v>42</v>
       </c>
@@ -4103,6 +4103,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -4319,22 +4328,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5668EAE9-BE2F-449B-83FE-5638B2ED2DF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B07A0A-C848-4FF7-A830-0D9B654DA189}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4353,7 +4361,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C5798F-31D9-455C-A266-3CF2A88C6872}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -4367,12 +4375,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5668EAE9-BE2F-449B-83FE-5638B2ED2DF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Write UHC RMNCH pillar
</commit_message>
<xml_diff>
--- a/inst/extdata/country_summary_template.xlsx
+++ b/inst/extdata/country_summary_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9099DC-DFD9-45C5-B8B3-71E0E3FE4520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F424A3E1-8E83-4DF0-98D7-62A450047148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="26136" windowHeight="16896" tabRatio="942" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="26136" windowHeight="16896" tabRatio="942" activeTab="2" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="12" r:id="rId1"/>
@@ -658,22 +658,6 @@
     <t>Malaria prevention</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">ITN use </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5</t>
-    </r>
-  </si>
-  <si>
     <t>Water and sanitation</t>
   </si>
   <si>
@@ -1707,9 +1691,6 @@
     <t>This indicator is slightly modified for the purpose of this exercise by the use of nested arithmetic means. See the Method Report for more details.</t>
   </si>
   <si>
-    <t>4 ITN use only applies to malaria endemic countries in sub-Saharan Africa for which data on ITN use are available.</t>
-  </si>
-  <si>
     <t>Direction of change</t>
   </si>
   <si>
@@ -1726,6 +1707,45 @@
   </si>
   <si>
     <t>- Type: type of data:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ITN use only applies to malaria endemic countries in sub-Saharan Africa for which data on ITN use are available.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ITN use </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3968,7 +3988,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72.525628659999995</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>96.093194519999997</c:v>
@@ -4337,7 +4357,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCDBAACD-B3C7-4503-9056-862180122333}" type="CELLRANGE">
+                    <a:fld id="{E07B57CD-6590-440E-9084-B6B0393F13F2}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4398,7 +4418,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{365D8202-920A-4749-AEE2-FA21DDEDB591}" type="CELLRANGE">
+                    <a:fld id="{69F94930-D0BD-4044-8C1D-E8D942E6BDFA}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4459,7 +4479,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4186C268-9880-4304-9446-7A8A3BC5D7A9}" type="CELLRANGE">
+                    <a:fld id="{69971402-75AE-4E22-9A30-9AEDB4C960A4}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4493,11 +4513,6 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7968A274-3CC3-427D-BA19-D37647F1E7F2}" type="CELLRANGE">
-                      <a:rPr lang="en-CH"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
                     <a:endParaRPr lang="en-CH"/>
                   </a:p>
                 </c:rich>
@@ -4511,7 +4526,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -4554,7 +4568,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02A25AC5-804A-495B-829D-C393F2D83896}" type="CELLRANGE">
+                    <a:fld id="{EF22AEBE-FF93-419A-ADBF-3D5CCF00EB66}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4588,7 +4602,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE6DBBB1-427A-49EC-A6B2-F165F2F37ED0}" type="CELLRANGE">
+                    <a:fld id="{FB442C29-6026-4175-BD42-9FD7C78542E7}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4622,7 +4636,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A2127B68-EA69-43F5-8852-38A6598CB8F0}" type="CELLRANGE">
+                    <a:fld id="{944D9DB4-2D29-4C34-977A-D88D3824780D}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4656,7 +4670,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DA492679-0EFC-4377-A369-421E7F7412F4}" type="CELLRANGE">
+                    <a:fld id="{5021FE3B-811D-4FC7-B2A3-7071F7BDFE19}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4690,7 +4704,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AFE84DC-4F45-48BA-90E2-8D5FC6490AC4}" type="CELLRANGE">
+                    <a:fld id="{0384E728-9EE1-499C-BA7F-01BD1C11EA24}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4724,7 +4738,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EDA226C4-19E0-4335-8A49-1DB0039D3F9E}" type="CELLRANGE">
+                    <a:fld id="{889FB31C-300B-43FB-ACCF-468D86221213}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4907,7 +4921,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -6535,7 +6549,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8579FA3E-EF4F-4C68-B37B-AEFD542EA0C3}" type="CELLRANGE">
+                    <a:fld id="{B54C23A3-9555-4577-848C-64E0A7B6AF29}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6596,7 +6610,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{372A21FE-2DB1-4F3B-B41B-A659DDF3546B}" type="CELLRANGE">
+                    <a:fld id="{CCDC4EA4-D849-4E34-9935-F8D4806478E8}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6657,7 +6671,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{66B7A643-F577-4EFB-8A0E-596A55857DCC}" type="CELLRANGE">
+                    <a:fld id="{D999897C-6BEB-46A0-A55A-BF6174CB7423}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6691,7 +6705,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{697A0FFD-A134-41B2-A27B-02B0BE81C1A7}" type="CELLRANGE">
+                    <a:fld id="{8B953A3A-F294-482B-BE57-3910FFF77454}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6752,7 +6766,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B5F8F16-7369-48BA-BA5E-C00C4CB22B3C}" type="CELLRANGE">
+                    <a:fld id="{7B2D33BF-11B9-4B94-A70E-6B092E37DD4E}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6786,7 +6800,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{20D20E06-A2EC-4D0F-8DE3-83A60800A260}" type="CELLRANGE">
+                    <a:fld id="{ED8DAC85-DD8B-48E1-B23F-D951873B1672}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6820,7 +6834,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FB4F350E-1E1F-44EC-87E7-5BE14831C5F7}" type="CELLRANGE">
+                    <a:fld id="{40E4DD50-5C1C-4F70-93FB-038394447B75}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6854,7 +6868,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D6814AC-3CA7-471D-9A07-9B37DC6B9D76}" type="CELLRANGE">
+                    <a:fld id="{48124EC9-6BFE-4524-AC41-EF4261DF36B4}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6888,7 +6902,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{446F1131-A54E-404B-B2B6-93C851F465D1}" type="CELLRANGE">
+                    <a:fld id="{D364C426-7FB5-4083-827A-9322CE0104A5}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6922,7 +6936,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6C2C7A3-B48C-4CCF-813B-747D1246A0C5}" type="CELLRANGE">
+                    <a:fld id="{5D461230-90CC-4C8F-9D2A-9DE8A736E086}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6956,7 +6970,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91260CD7-BBC5-47E5-8153-DC8A6F868884}" type="CELLRANGE">
+                    <a:fld id="{4093D5B9-A7B6-4DB5-A2A1-BD68E249CB2D}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6990,7 +7004,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5042931-CB04-4EAA-BC80-457C16A512E0}" type="CELLRANGE">
+                    <a:fld id="{71D75CFC-2647-4CDF-8436-083F2392E65D}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7024,7 +7038,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9572937B-19B3-4A1C-9C1E-03EE8BCF6A5F}" type="CELLRANGE">
+                    <a:fld id="{0CC48D71-2108-4CEF-B3FF-B9B6F645F80B}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7910,7 +7924,7 @@
   </sheetPr>
   <dimension ref="B1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C20" sqref="C20:M20"/>
     </sheetView>
   </sheetViews>
@@ -7925,7 +7939,7 @@
     <row r="1" spans="2:15" ht="10.5" customHeight="1"/>
     <row r="2" spans="2:15" ht="36" customHeight="1">
       <c r="B2" s="300" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C2" s="300"/>
       <c r="D2" s="300"/>
@@ -7943,7 +7957,7 @@
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1">
       <c r="B3" s="301" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C3" s="301"/>
       <c r="D3" s="301"/>
@@ -7961,7 +7975,7 @@
     </row>
     <row r="4" spans="2:15" ht="18.75" customHeight="1">
       <c r="B4" s="302" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C4" s="302"/>
       <c r="D4" s="302"/>
@@ -7979,7 +7993,7 @@
     </row>
     <row r="5" spans="2:15" ht="15" customHeight="1">
       <c r="B5" s="299" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C5" s="299"/>
       <c r="D5" s="299"/>
@@ -7997,7 +8011,7 @@
     </row>
     <row r="6" spans="2:15" ht="15" customHeight="1">
       <c r="B6" s="298" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C6" s="298"/>
       <c r="D6" s="298"/>
@@ -8015,7 +8029,7 @@
     </row>
     <row r="7" spans="2:15" ht="15" customHeight="1">
       <c r="B7" s="298" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C7" s="298"/>
       <c r="D7" s="298"/>
@@ -8033,7 +8047,7 @@
     </row>
     <row r="8" spans="2:15" ht="21.75" customHeight="1">
       <c r="B8" s="298" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C8" s="298"/>
       <c r="D8" s="298"/>
@@ -8051,7 +8065,7 @@
     </row>
     <row r="9" spans="2:15" ht="30" customHeight="1">
       <c r="B9" s="299" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C9" s="299"/>
       <c r="D9" s="299"/>
@@ -8066,7 +8080,7 @@
     </row>
     <row r="10" spans="2:15" ht="33.75" customHeight="1">
       <c r="B10" s="299" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C10" s="299"/>
       <c r="D10" s="299"/>
@@ -8081,7 +8095,7 @@
     </row>
     <row r="11" spans="2:15" ht="21" customHeight="1">
       <c r="B11" s="302" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C11" s="302"/>
       <c r="D11" s="302"/>
@@ -8099,7 +8113,7 @@
     </row>
     <row r="12" spans="2:15">
       <c r="B12" s="299" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C12" s="299"/>
       <c r="D12" s="299"/>
@@ -8115,7 +8129,7 @@
     </row>
     <row r="13" spans="2:15" ht="27" customHeight="1">
       <c r="B13" s="297" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C13" s="298"/>
       <c r="D13" s="298"/>
@@ -8131,7 +8145,7 @@
     </row>
     <row r="14" spans="2:15">
       <c r="B14" s="297" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C14" s="298"/>
       <c r="D14" s="298"/>
@@ -8147,7 +8161,7 @@
     </row>
     <row r="15" spans="2:15" ht="17.25" customHeight="1">
       <c r="B15" s="297" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C15" s="298"/>
       <c r="D15" s="298"/>
@@ -8163,7 +8177,7 @@
     </row>
     <row r="16" spans="2:15">
       <c r="B16" s="299" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C16" s="299"/>
       <c r="D16" s="299"/>
@@ -8179,7 +8193,7 @@
     </row>
     <row r="17" spans="2:13" ht="18">
       <c r="B17" s="302" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C17" s="302"/>
       <c r="D17" s="302"/>
@@ -8195,7 +8209,7 @@
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="299" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C18" s="299"/>
       <c r="D18" s="299"/>
@@ -8212,7 +8226,7 @@
     <row r="19" spans="2:13" ht="14.4" customHeight="1">
       <c r="B19" s="356"/>
       <c r="C19" s="355" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D19" s="355"/>
       <c r="E19" s="355"/>
@@ -8228,7 +8242,7 @@
     <row r="20" spans="2:13">
       <c r="B20" s="356"/>
       <c r="C20" s="355" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D20" s="355"/>
       <c r="E20" s="355"/>
@@ -8244,7 +8258,7 @@
     <row r="21" spans="2:13" ht="14.4" customHeight="1">
       <c r="B21" s="356"/>
       <c r="C21" s="355" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D21" s="355"/>
       <c r="E21" s="355"/>
@@ -8260,7 +8274,7 @@
     <row r="22" spans="2:13">
       <c r="B22" s="356"/>
       <c r="C22" s="355" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D22" s="355"/>
       <c r="E22" s="355"/>
@@ -8277,7 +8291,7 @@
       <c r="B23" s="356"/>
       <c r="C23" s="356"/>
       <c r="D23" s="355" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E23" s="355"/>
       <c r="F23" s="355"/>
@@ -8293,7 +8307,7 @@
       <c r="B24" s="356"/>
       <c r="C24" s="356"/>
       <c r="D24" s="355" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E24" s="355"/>
       <c r="F24" s="355"/>
@@ -8309,7 +8323,7 @@
       <c r="B25" s="294"/>
       <c r="C25" s="295"/>
       <c r="D25" s="299" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E25" s="299"/>
       <c r="F25" s="299"/>
@@ -8325,7 +8339,7 @@
       <c r="B26" s="294"/>
       <c r="C26" s="295"/>
       <c r="D26" s="355" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E26" s="355"/>
       <c r="F26" s="355"/>
@@ -8339,7 +8353,7 @@
     </row>
     <row r="27" spans="2:13" ht="15" customHeight="1">
       <c r="B27" s="297" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C27" s="298"/>
       <c r="D27" s="298"/>
@@ -8355,7 +8369,7 @@
     </row>
     <row r="28" spans="2:13" ht="15" customHeight="1">
       <c r="B28" s="297" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C28" s="298"/>
       <c r="D28" s="298"/>
@@ -8374,7 +8388,7 @@
     </row>
     <row r="30" spans="2:13" ht="18">
       <c r="B30" s="302" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C30" s="302"/>
       <c r="D30" s="302"/>
@@ -8390,7 +8404,7 @@
     </row>
     <row r="31" spans="2:13" ht="15" customHeight="1">
       <c r="B31" s="299" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C31" s="299"/>
       <c r="D31" s="299"/>
@@ -8406,7 +8420,7 @@
     </row>
     <row r="32" spans="2:13" ht="31.5" customHeight="1">
       <c r="B32" s="299" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C32" s="299"/>
       <c r="D32" s="299"/>
@@ -8422,7 +8436,7 @@
     </row>
     <row r="33" spans="2:13" ht="28.5" customHeight="1">
       <c r="B33" s="299" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C33" s="299"/>
       <c r="D33" s="299"/>
@@ -8438,7 +8452,7 @@
     </row>
     <row r="34" spans="2:13">
       <c r="B34" s="299" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C34" s="299"/>
       <c r="D34" s="299"/>
@@ -8454,7 +8468,7 @@
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="299" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C35" s="299"/>
       <c r="D35" s="299"/>
@@ -8470,7 +8484,7 @@
     </row>
     <row r="36" spans="2:13" ht="18">
       <c r="B36" s="302" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C36" s="302"/>
       <c r="D36" s="302"/>
@@ -8486,7 +8500,7 @@
     </row>
     <row r="37" spans="2:13" ht="30.75" customHeight="1">
       <c r="B37" s="299" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C37" s="299"/>
       <c r="D37" s="299"/>
@@ -8502,7 +8516,7 @@
     </row>
     <row r="38" spans="2:13">
       <c r="B38" s="299" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C38" s="299"/>
       <c r="D38" s="299"/>
@@ -8521,7 +8535,7 @@
     </row>
     <row r="40" spans="2:13" ht="18">
       <c r="B40" s="302" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C40" s="302"/>
       <c r="D40" s="302"/>
@@ -8537,7 +8551,7 @@
     </row>
     <row r="41" spans="2:13">
       <c r="B41" s="303" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C41" s="303"/>
       <c r="D41" s="303"/>
@@ -8553,7 +8567,7 @@
     </row>
     <row r="42" spans="2:13">
       <c r="B42" s="303" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C42" s="303"/>
       <c r="D42" s="303"/>
@@ -8569,7 +8583,7 @@
     </row>
     <row r="43" spans="2:13">
       <c r="B43" s="303" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C43" s="303"/>
       <c r="D43" s="303"/>
@@ -8585,7 +8599,7 @@
     </row>
     <row r="44" spans="2:13">
       <c r="B44" s="282" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C44" s="280"/>
       <c r="D44" s="280"/>
@@ -8601,7 +8615,7 @@
     </row>
     <row r="45" spans="2:13" ht="18">
       <c r="B45" s="302" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C45" s="302"/>
       <c r="D45" s="302"/>
@@ -8617,7 +8631,7 @@
     </row>
     <row r="46" spans="2:13">
       <c r="B46" s="299" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C46" s="299"/>
       <c r="D46" s="299"/>
@@ -8633,7 +8647,7 @@
     </row>
     <row r="47" spans="2:13">
       <c r="B47" s="304" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C47" s="304"/>
       <c r="D47" s="304"/>
@@ -8749,7 +8763,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="237" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B3" s="55">
         <v>1</v>
@@ -8785,7 +8799,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="237" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B4" s="55">
         <v>2</v>
@@ -8822,7 +8836,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="237" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B5" s="55">
         <v>3</v>
@@ -8858,7 +8872,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="237" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B6" s="55">
         <v>4</v>
@@ -9115,9 +9129,9 @@
   </sheetPr>
   <dimension ref="A1:AF76"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G16" sqref="G16"/>
+      <selection pane="topRight" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -9172,7 +9186,7 @@
     </row>
     <row r="2" spans="1:32" ht="30" customHeight="1">
       <c r="A2" s="175" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="13"/>
@@ -9293,7 +9307,7 @@
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
       <c r="A6" s="183" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B6" s="183"/>
       <c r="C6" s="183"/>
@@ -9328,7 +9342,7 @@
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1">
       <c r="A7" s="283" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -10856,7 +10870,7 @@
       <c r="T34" s="13"/>
       <c r="U34" s="13"/>
       <c r="W34" s="332" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="X34" s="333"/>
       <c r="Y34" s="267">
@@ -11445,7 +11459,7 @@
         <v>121</v>
       </c>
       <c r="C4" s="351" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D4" s="351"/>
       <c r="E4" s="351"/>
@@ -13542,7 +13556,7 @@
   <sheetData>
     <row r="2" spans="1:7" ht="30" customHeight="1">
       <c r="B2" s="12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="8"/>
@@ -13557,7 +13571,7 @@
     <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="236" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C4" s="236" t="s">
         <v>40</v>
@@ -13572,91 +13586,91 @@
         <v>43</v>
       </c>
       <c r="G4" s="236" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C5" s="244" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D5" s="244" t="s">
         <v>158</v>
       </c>
       <c r="E5" s="245" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F5" s="244" t="s">
         <v>158</v>
       </c>
       <c r="G5" s="246" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C6" s="244" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D6" s="244" t="s">
         <v>161</v>
       </c>
       <c r="E6" s="245" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F6" s="244" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G6" s="246" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="B7" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C7" s="244" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D7" s="244" t="s">
         <v>166</v>
       </c>
       <c r="E7" s="245" t="s">
+        <v>233</v>
+      </c>
+      <c r="F7" s="244" t="s">
         <v>234</v>
-      </c>
-      <c r="F7" s="244" t="s">
-        <v>235</v>
       </c>
       <c r="G7" s="246"/>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C8" s="244" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D8" s="244" t="s">
         <v>169</v>
       </c>
       <c r="E8" s="245" t="s">
+        <v>236</v>
+      </c>
+      <c r="F8" s="244" t="s">
         <v>237</v>
-      </c>
-      <c r="F8" s="244" t="s">
-        <v>238</v>
       </c>
       <c r="G8" s="246"/>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C9" s="244" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D9" s="244" t="s">
         <v>174</v>
@@ -13668,662 +13682,662 @@
         <v>175</v>
       </c>
       <c r="G9" s="246" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C10" s="244" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D10" s="244" t="s">
         <v>177</v>
       </c>
       <c r="E10" s="245" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F10" s="244" t="s">
         <v>177</v>
       </c>
       <c r="G10" s="246" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="B11" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C11" s="244" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D11" s="244" t="s">
         <v>180</v>
       </c>
       <c r="E11" s="245" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F11" s="244" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G11" s="246" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C12" s="244" t="s">
+        <v>242</v>
+      </c>
+      <c r="D12" s="244" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" s="245" t="s">
+        <v>182</v>
+      </c>
+      <c r="F12" s="244" t="s">
         <v>243</v>
-      </c>
-      <c r="D12" s="244" t="s">
-        <v>182</v>
-      </c>
-      <c r="E12" s="245" t="s">
-        <v>183</v>
-      </c>
-      <c r="F12" s="244" t="s">
-        <v>244</v>
       </c>
       <c r="G12" s="246"/>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C13" s="244" t="s">
+        <v>244</v>
+      </c>
+      <c r="D13" s="244" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" s="245" t="s">
+        <v>416</v>
+      </c>
+      <c r="F13" s="244" t="s">
         <v>245</v>
       </c>
-      <c r="D13" s="244" t="s">
-        <v>187</v>
-      </c>
-      <c r="E13" s="245" t="s">
-        <v>417</v>
-      </c>
-      <c r="F13" s="244" t="s">
-        <v>246</v>
-      </c>
       <c r="G13" s="285" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C14" s="244" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" s="244" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="245" t="s">
+        <v>417</v>
+      </c>
+      <c r="F14" s="244" t="s">
         <v>247</v>
       </c>
-      <c r="D14" s="244" t="s">
-        <v>190</v>
-      </c>
-      <c r="E14" s="245" t="s">
-        <v>418</v>
-      </c>
-      <c r="F14" s="244" t="s">
-        <v>248</v>
-      </c>
       <c r="G14" s="285" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C15" s="244" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D15" s="244" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E15" s="245" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F15" s="244" t="s">
         <v>29</v>
       </c>
       <c r="G15" s="246" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="B16" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C16" s="244" t="s">
+        <v>249</v>
+      </c>
+      <c r="D16" s="244" t="s">
+        <v>196</v>
+      </c>
+      <c r="E16" s="245" t="s">
+        <v>418</v>
+      </c>
+      <c r="F16" s="244" t="s">
         <v>250</v>
       </c>
-      <c r="D16" s="244" t="s">
-        <v>197</v>
-      </c>
-      <c r="E16" s="245" t="s">
-        <v>419</v>
-      </c>
-      <c r="F16" s="244" t="s">
-        <v>251</v>
-      </c>
       <c r="G16" s="285" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C17" s="244" t="s">
+        <v>251</v>
+      </c>
+      <c r="D17" s="244" t="s">
+        <v>199</v>
+      </c>
+      <c r="E17" s="245" t="s">
         <v>252</v>
       </c>
-      <c r="D17" s="244" t="s">
-        <v>200</v>
-      </c>
-      <c r="E17" s="245" t="s">
-        <v>253</v>
-      </c>
       <c r="F17" s="244" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G17" s="285" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C18" s="244" t="s">
+        <v>253</v>
+      </c>
+      <c r="D18" s="244" t="s">
         <v>254</v>
       </c>
-      <c r="D18" s="244" t="s">
+      <c r="E18" s="245" t="s">
+        <v>201</v>
+      </c>
+      <c r="F18" s="244" t="s">
         <v>255</v>
-      </c>
-      <c r="E18" s="245" t="s">
-        <v>202</v>
-      </c>
-      <c r="F18" s="244" t="s">
-        <v>256</v>
       </c>
       <c r="G18" s="285"/>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C19" s="244" t="s">
+        <v>256</v>
+      </c>
+      <c r="D19" s="244" t="s">
         <v>257</v>
       </c>
-      <c r="D19" s="244" t="s">
+      <c r="E19" s="245" t="s">
+        <v>204</v>
+      </c>
+      <c r="F19" s="244" t="s">
         <v>258</v>
-      </c>
-      <c r="E19" s="245" t="s">
-        <v>205</v>
-      </c>
-      <c r="F19" s="244" t="s">
-        <v>259</v>
       </c>
       <c r="G19" s="285"/>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C20" s="244" t="s">
+        <v>259</v>
+      </c>
+      <c r="D20" s="244" t="s">
+        <v>205</v>
+      </c>
+      <c r="E20" s="245" t="s">
+        <v>405</v>
+      </c>
+      <c r="F20" s="244" t="s">
         <v>260</v>
       </c>
-      <c r="D20" s="244" t="s">
-        <v>206</v>
-      </c>
-      <c r="E20" s="245" t="s">
-        <v>406</v>
-      </c>
-      <c r="F20" s="244" t="s">
-        <v>261</v>
-      </c>
       <c r="G20" s="285" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="21" spans="2:7">
       <c r="B21" s="244" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C21" s="245" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D21" s="244" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E21" s="245" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F21" s="244" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G21" s="246" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C22" s="241" t="s">
+        <v>259</v>
+      </c>
+      <c r="D22" s="241" t="s">
+        <v>404</v>
+      </c>
+      <c r="E22" s="242" t="s">
         <v>260</v>
-      </c>
-      <c r="D22" s="241" t="s">
-        <v>405</v>
-      </c>
-      <c r="E22" s="242" t="s">
-        <v>261</v>
       </c>
       <c r="F22" s="241"/>
       <c r="G22" s="243"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="241" t="s">
+        <v>378</v>
+      </c>
+      <c r="C23" s="241" t="s">
+        <v>420</v>
+      </c>
+      <c r="D23" s="241" t="s">
         <v>379</v>
       </c>
-      <c r="C23" s="241" t="s">
-        <v>421</v>
-      </c>
-      <c r="D23" s="241" t="s">
-        <v>380</v>
-      </c>
       <c r="E23" s="242" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F23" s="241"/>
       <c r="G23" s="243"/>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C24" s="241" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D24" s="241" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E24" s="242" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F24" s="241"/>
       <c r="G24" s="243"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C25" s="241" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D25" s="241" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E25" s="242" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F25" s="241"/>
       <c r="G25" s="243"/>
     </row>
     <row r="26" spans="2:7">
       <c r="B26" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C26" s="241" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D26" s="241" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E26" s="242" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F26" s="241"/>
       <c r="G26" s="243"/>
     </row>
     <row r="27" spans="2:7">
       <c r="B27" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C27" s="241" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D27" s="241" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E27" s="242" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F27" s="241"/>
       <c r="G27" s="243"/>
     </row>
     <row r="28" spans="2:7">
       <c r="B28" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C28" s="241" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D28" s="241" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E28" s="242" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F28" s="241"/>
       <c r="G28" s="243"/>
     </row>
     <row r="29" spans="2:7">
       <c r="B29" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C29" s="241" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D29" s="241" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E29" s="242" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F29" s="241"/>
       <c r="G29" s="243"/>
     </row>
     <row r="30" spans="2:7">
       <c r="B30" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C30" s="241" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D30" s="241" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E30" s="242" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F30" s="241"/>
       <c r="G30" s="243"/>
     </row>
     <row r="31" spans="2:7">
       <c r="B31" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C31" s="241" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D31" s="241" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E31" s="242" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F31" s="241"/>
       <c r="G31" s="243"/>
     </row>
     <row r="32" spans="2:7">
       <c r="B32" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C32" s="241" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D32" s="241" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E32" s="242" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F32" s="241"/>
       <c r="G32" s="243"/>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C33" s="241" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D33" s="241" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E33" s="242" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F33" s="241"/>
       <c r="G33" s="243"/>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C34" s="241" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D34" s="241" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E34" s="242" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F34" s="241"/>
       <c r="G34" s="243"/>
     </row>
     <row r="35" spans="2:7">
       <c r="B35" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C35" s="241" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D35" s="241" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E35" s="242" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F35" s="241"/>
       <c r="G35" s="243"/>
     </row>
     <row r="36" spans="2:7">
       <c r="B36" s="242" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C36" s="242" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D36" s="242" t="s">
+        <v>443</v>
+      </c>
+      <c r="E36" s="242" t="s">
         <v>444</v>
-      </c>
-      <c r="E36" s="242" t="s">
-        <v>445</v>
       </c>
       <c r="F36" s="241"/>
       <c r="G36" s="243"/>
     </row>
     <row r="37" spans="2:7">
       <c r="B37" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C37" s="241" t="s">
+        <v>317</v>
+      </c>
+      <c r="D37" s="241" t="s">
         <v>318</v>
       </c>
-      <c r="D37" s="241" t="s">
-        <v>319</v>
-      </c>
       <c r="E37" s="242" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F37" s="241"/>
       <c r="G37" s="243"/>
     </row>
     <row r="38" spans="2:7">
       <c r="B38" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C38" s="241" t="s">
+        <v>319</v>
+      </c>
+      <c r="D38" s="241" t="s">
         <v>320</v>
       </c>
-      <c r="D38" s="241" t="s">
+      <c r="E38" s="242" t="s">
         <v>321</v>
-      </c>
-      <c r="E38" s="242" t="s">
-        <v>322</v>
       </c>
       <c r="F38" s="241"/>
       <c r="G38" s="243"/>
     </row>
     <row r="39" spans="2:7">
       <c r="B39" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C39" s="241" t="s">
+        <v>322</v>
+      </c>
+      <c r="D39" s="241" t="s">
         <v>323</v>
       </c>
-      <c r="D39" s="241" t="s">
-        <v>324</v>
-      </c>
       <c r="E39" s="242" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F39" s="241"/>
       <c r="G39" s="243"/>
     </row>
     <row r="40" spans="2:7">
       <c r="B40" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C40" s="241" t="s">
+        <v>324</v>
+      </c>
+      <c r="D40" s="241" t="s">
         <v>325</v>
       </c>
-      <c r="D40" s="241" t="s">
-        <v>326</v>
-      </c>
       <c r="E40" s="242" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F40" s="241"/>
       <c r="G40" s="243"/>
     </row>
     <row r="41" spans="2:7">
       <c r="B41" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C41" s="241" t="s">
+        <v>326</v>
+      </c>
+      <c r="D41" s="241" t="s">
         <v>327</v>
       </c>
-      <c r="D41" s="241" t="s">
-        <v>328</v>
-      </c>
       <c r="E41" s="242" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F41" s="241"/>
       <c r="G41" s="243"/>
     </row>
     <row r="42" spans="2:7">
       <c r="B42" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C42" s="241" t="s">
+        <v>328</v>
+      </c>
+      <c r="D42" s="241" t="s">
         <v>329</v>
       </c>
-      <c r="D42" s="241" t="s">
-        <v>330</v>
-      </c>
       <c r="E42" s="242" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F42" s="241"/>
       <c r="G42" s="243"/>
     </row>
     <row r="43" spans="2:7">
       <c r="B43" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C43" s="241" t="s">
+        <v>330</v>
+      </c>
+      <c r="D43" s="241" t="s">
         <v>331</v>
       </c>
-      <c r="D43" s="241" t="s">
-        <v>332</v>
-      </c>
       <c r="E43" s="242" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F43" s="241"/>
       <c r="G43" s="243"/>
     </row>
     <row r="44" spans="2:7">
       <c r="B44" s="242" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C44" s="242" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D44" s="242" t="s">
+        <v>440</v>
+      </c>
+      <c r="E44" s="242" t="s">
         <v>441</v>
-      </c>
-      <c r="E44" s="242" t="s">
-        <v>442</v>
       </c>
       <c r="F44" s="241"/>
       <c r="G44" s="243"/>
     </row>
     <row r="45" spans="2:7">
       <c r="B45" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C45" s="241" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D45" s="241" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E45" s="242" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F45" s="241"/>
       <c r="G45" s="243"/>
     </row>
     <row r="46" spans="2:7">
       <c r="B46" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C46" s="241" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D46" s="241" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E46" s="242" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F46" s="241"/>
       <c r="G46" s="243"/>
     </row>
     <row r="47" spans="2:7">
       <c r="B47" s="241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C47" s="241" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D47" s="241" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E47" s="242" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F47" s="241"/>
       <c r="G47" s="243"/>
     </row>
     <row r="48" spans="2:7">
       <c r="B48" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C48" s="238" t="s">
         <v>44</v>
@@ -14341,7 +14355,7 @@
     </row>
     <row r="49" spans="2:7">
       <c r="B49" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C49" s="238" t="s">
         <v>47</v>
@@ -14359,7 +14373,7 @@
     </row>
     <row r="50" spans="2:7">
       <c r="B50" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C50" s="238" t="s">
         <v>49</v>
@@ -14377,7 +14391,7 @@
     </row>
     <row r="51" spans="2:7">
       <c r="B51" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C51" s="238" t="s">
         <v>123</v>
@@ -14395,7 +14409,7 @@
     </row>
     <row r="52" spans="2:7">
       <c r="B52" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C52" s="238" t="s">
         <v>51</v>
@@ -14413,7 +14427,7 @@
     </row>
     <row r="53" spans="2:7">
       <c r="B53" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C53" s="238" t="s">
         <v>53</v>
@@ -14431,7 +14445,7 @@
     </row>
     <row r="54" spans="2:7">
       <c r="B54" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C54" s="238" t="s">
         <v>55</v>
@@ -14449,7 +14463,7 @@
     </row>
     <row r="55" spans="2:7">
       <c r="B55" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C55" s="238" t="s">
         <v>57</v>
@@ -14467,7 +14481,7 @@
     </row>
     <row r="56" spans="2:7">
       <c r="B56" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C56" s="238" t="s">
         <v>59</v>
@@ -14485,13 +14499,13 @@
     </row>
     <row r="57" spans="2:7">
       <c r="B57" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C57" s="238" t="s">
         <v>61</v>
       </c>
       <c r="D57" s="239" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E57" s="239" t="s">
         <v>62</v>
@@ -14500,12 +14514,12 @@
         <v>24</v>
       </c>
       <c r="G57" s="240" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="58" spans="2:7">
       <c r="B58" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C58" s="238" t="s">
         <v>63</v>
@@ -14520,12 +14534,12 @@
         <v>25</v>
       </c>
       <c r="G58" s="240" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="59" spans="2:7">
       <c r="B59" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C59" s="238" t="s">
         <v>65</v>
@@ -14543,7 +14557,7 @@
     </row>
     <row r="60" spans="2:7">
       <c r="B60" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C60" s="238" t="s">
         <v>67</v>
@@ -14561,7 +14575,7 @@
     </row>
     <row r="61" spans="2:7">
       <c r="B61" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C61" s="238" t="s">
         <v>69</v>
@@ -14579,7 +14593,7 @@
     </row>
     <row r="62" spans="2:7">
       <c r="B62" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C62" s="238" t="s">
         <v>71</v>
@@ -14597,7 +14611,7 @@
     </row>
     <row r="63" spans="2:7">
       <c r="B63" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C63" s="238" t="s">
         <v>73</v>
@@ -14615,7 +14629,7 @@
     </row>
     <row r="64" spans="2:7">
       <c r="B64" s="238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C64" s="238" t="s">
         <v>51</v>
@@ -14646,9 +14660,9 @@
   </sheetPr>
   <dimension ref="A1:AE78"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+      <selection pane="topRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -14706,7 +14720,7 @@
     </row>
     <row r="2" spans="1:31" ht="23.25" customHeight="1">
       <c r="A2" s="68" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -14808,7 +14822,7 @@
     </row>
     <row r="5" spans="1:31" ht="18">
       <c r="A5" s="146" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B5" s="146"/>
       <c r="C5" s="146"/>
@@ -14847,7 +14861,7 @@
     </row>
     <row r="6" spans="1:31" ht="18">
       <c r="A6" s="146" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B6" s="146"/>
       <c r="C6" s="146"/>
@@ -14886,7 +14900,7 @@
     </row>
     <row r="7" spans="1:31" ht="18">
       <c r="A7" s="283" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B7" s="146"/>
       <c r="C7" s="146"/>
@@ -15015,12 +15029,12 @@
       <c r="J10" s="305"/>
       <c r="K10" s="296"/>
       <c r="L10" s="305" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M10" s="305"/>
       <c r="N10" s="296"/>
       <c r="O10" s="314" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="P10" s="296"/>
       <c r="Q10" s="305" t="s">
@@ -15163,7 +15177,7 @@
       <c r="M13" s="129"/>
       <c r="N13" s="96"/>
       <c r="O13" s="291">
-        <f>J13-I13</f>
+        <f>IF(OR(ISBLANK(I13),ISBLANK(J13)),"",J13-I13)</f>
         <v>1</v>
       </c>
       <c r="P13" s="96"/>
@@ -15223,7 +15237,7 @@
       <c r="M14" s="121"/>
       <c r="N14" s="89"/>
       <c r="O14" s="291">
-        <f t="shared" ref="O14:O16" si="0">J14-I14</f>
+        <f t="shared" ref="O14:O16" si="0">IF(OR(ISBLANK(I14),ISBLANK(J14)),"",J14-I14)</f>
         <v>-9.7765399999900637E-3</v>
       </c>
       <c r="P14" s="89"/>
@@ -15479,7 +15493,7 @@
       <c r="M19" s="129"/>
       <c r="N19" s="96"/>
       <c r="O19" s="291">
-        <f t="shared" ref="O19:O22" si="1">J19-I19</f>
+        <f>IF(OR(ISBLANK(I19),ISBLANK(J19)),"",J19-I19)</f>
         <v>0</v>
       </c>
       <c r="P19" s="96"/>
@@ -15512,7 +15526,7 @@
         <v>177</v>
       </c>
       <c r="B20" s="88" t="s">
-        <v>178</v>
+        <v>412</v>
       </c>
       <c r="C20" s="120">
         <v>64.595253999999997</v>
@@ -15539,7 +15553,7 @@
       <c r="M20" s="121"/>
       <c r="N20" s="89"/>
       <c r="O20" s="291">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="O20:O22" si="1">IF(OR(ISBLANK(I20),ISBLANK(J20)),"",J20-I20)</f>
         <v>7.9303746599999982</v>
       </c>
       <c r="P20" s="89"/>
@@ -15572,7 +15586,7 @@
         <v>180</v>
       </c>
       <c r="B21" s="91" t="s">
-        <v>181</v>
+        <v>464</v>
       </c>
       <c r="C21" s="122"/>
       <c r="D21" s="122"/>
@@ -15586,9 +15600,9 @@
       <c r="L21" s="123"/>
       <c r="M21" s="123"/>
       <c r="N21" s="92"/>
-      <c r="O21" s="291">
+      <c r="O21" s="291" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="P21" s="92"/>
       <c r="Q21" s="93"/>
@@ -15609,10 +15623,10 @@
     </row>
     <row r="22" spans="1:31" ht="25.5" customHeight="1">
       <c r="A22" s="91" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" s="91" t="s">
         <v>182</v>
-      </c>
-      <c r="B22" s="91" t="s">
-        <v>183</v>
       </c>
       <c r="C22" s="122">
         <v>94.258510000000001</v>
@@ -15625,7 +15639,7 @@
         <v>90</v>
       </c>
       <c r="G22" s="99" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H22" s="41"/>
       <c r="I22" s="122">
@@ -15670,7 +15684,7 @@
     <row r="23" spans="1:31" ht="15" customHeight="1">
       <c r="A23" s="199"/>
       <c r="B23" s="229" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C23" s="200"/>
       <c r="D23" s="201"/>
@@ -15710,7 +15724,7 @@
     </row>
     <row r="24" spans="1:31" ht="15" customHeight="1">
       <c r="A24" s="207" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B24" s="106"/>
       <c r="C24" s="124"/>
@@ -15745,10 +15759,10 @@
     </row>
     <row r="25" spans="1:31" ht="25.5" customHeight="1">
       <c r="A25" s="108" t="s">
+        <v>186</v>
+      </c>
+      <c r="B25" s="108" t="s">
         <v>187</v>
-      </c>
-      <c r="B25" s="108" t="s">
-        <v>188</v>
       </c>
       <c r="C25" s="126">
         <v>22.47</v>
@@ -15764,7 +15778,7 @@
         <v>90</v>
       </c>
       <c r="G25" s="98" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H25" s="109"/>
       <c r="I25" s="126">
@@ -15784,7 +15798,7 @@
       </c>
       <c r="N25" s="110"/>
       <c r="O25" s="291">
-        <f t="shared" ref="O25:O27" si="2">J25-I25</f>
+        <f t="shared" ref="O25:O27" si="2">IF(OR(ISBLANK(I25),ISBLANK(J25)),"",J25-I25)</f>
         <v>-0.96218870000000223</v>
       </c>
       <c r="P25" s="110"/>
@@ -15814,10 +15828,10 @@
     </row>
     <row r="26" spans="1:31" ht="25.5" customHeight="1">
       <c r="A26" s="91" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" s="91" t="s">
         <v>190</v>
-      </c>
-      <c r="B26" s="91" t="s">
-        <v>191</v>
       </c>
       <c r="C26" s="122">
         <v>5.43</v>
@@ -15833,7 +15847,7 @@
         <v>90</v>
       </c>
       <c r="G26" s="99" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H26" s="112"/>
       <c r="I26" s="122">
@@ -15883,10 +15897,10 @@
     </row>
     <row r="27" spans="1:31" ht="25.5" customHeight="1">
       <c r="A27" s="88" t="s">
+        <v>191</v>
+      </c>
+      <c r="B27" s="88" t="s">
         <v>192</v>
-      </c>
-      <c r="B27" s="88" t="s">
-        <v>193</v>
       </c>
       <c r="C27" s="120">
         <v>21.8</v>
@@ -15930,7 +15944,7 @@
         <v>90</v>
       </c>
       <c r="R27" s="90" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S27" s="89"/>
       <c r="T27" s="114" t="s">
@@ -15953,7 +15967,7 @@
     <row r="28" spans="1:31" ht="15" customHeight="1">
       <c r="A28" s="199"/>
       <c r="B28" s="229" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C28" s="200"/>
       <c r="D28" s="201"/>
@@ -15993,7 +16007,7 @@
     </row>
     <row r="29" spans="1:31" ht="15" customHeight="1">
       <c r="A29" s="107" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B29" s="106"/>
       <c r="C29" s="124"/>
@@ -16028,10 +16042,10 @@
     </row>
     <row r="30" spans="1:31" ht="25.5" customHeight="1">
       <c r="A30" s="108" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="108" t="s">
         <v>197</v>
-      </c>
-      <c r="B30" s="108" t="s">
-        <v>198</v>
       </c>
       <c r="C30" s="126">
         <v>49.92</v>
@@ -16047,7 +16061,7 @@
         <v>163</v>
       </c>
       <c r="G30" s="98" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H30" s="109"/>
       <c r="I30" s="126">
@@ -16067,7 +16081,7 @@
       </c>
       <c r="N30" s="110"/>
       <c r="O30" s="291">
-        <f t="shared" ref="O30:O34" si="3">J30-I30</f>
+        <f>IF(OR(ISBLANK(I30),ISBLANK(J30)),"",J30-I30)</f>
         <v>3.9624349300000006</v>
       </c>
       <c r="P30" s="110"/>
@@ -16097,10 +16111,10 @@
     </row>
     <row r="31" spans="1:31" ht="25.5" customHeight="1">
       <c r="A31" s="307" t="s">
+        <v>199</v>
+      </c>
+      <c r="B31" s="91" t="s">
         <v>200</v>
-      </c>
-      <c r="B31" s="91" t="s">
-        <v>201</v>
       </c>
       <c r="C31" s="122">
         <f>IF(AND(C32&lt;&gt;"",C33&lt;&gt;""),C32+C33,"")</f>
@@ -16136,7 +16150,7 @@
       </c>
       <c r="N31" s="92"/>
       <c r="O31" s="291">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="O31:O34" si="3">IF(OR(ISBLANK(I31),ISBLANK(J31)),"",J31-I31)</f>
         <v>5.3628150000000119</v>
       </c>
       <c r="P31" s="92"/>
@@ -16159,7 +16173,7 @@
     <row r="32" spans="1:31" ht="25.5" customHeight="1">
       <c r="A32" s="308"/>
       <c r="B32" s="91" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C32" s="122">
         <v>39.934623999999999</v>
@@ -16172,7 +16186,7 @@
         <v>163</v>
       </c>
       <c r="G32" s="99" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H32" s="112"/>
       <c r="I32" s="122">
@@ -16198,10 +16212,10 @@
       </c>
       <c r="S32" s="92"/>
       <c r="T32" s="99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U32" s="99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="V32" s="51"/>
       <c r="W32" s="51"/>
@@ -16217,7 +16231,7 @@
     <row r="33" spans="1:31" ht="25.5" customHeight="1">
       <c r="A33" s="309"/>
       <c r="B33" s="91" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C33" s="122">
         <v>26.017996</v>
@@ -16230,7 +16244,7 @@
         <v>163</v>
       </c>
       <c r="G33" s="99" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H33" s="112"/>
       <c r="I33" s="122">
@@ -16256,10 +16270,10 @@
       </c>
       <c r="S33" s="92"/>
       <c r="T33" s="99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U33" s="99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="V33" s="51"/>
       <c r="W33" s="51"/>
@@ -16274,10 +16288,10 @@
     </row>
     <row r="34" spans="1:31" ht="25.5" customHeight="1">
       <c r="A34" s="88" t="s">
+        <v>205</v>
+      </c>
+      <c r="B34" s="88" t="s">
         <v>206</v>
-      </c>
-      <c r="B34" s="88" t="s">
-        <v>207</v>
       </c>
       <c r="C34" s="120">
         <v>64</v>
@@ -16290,7 +16304,7 @@
         <v>163</v>
       </c>
       <c r="G34" s="114" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H34" s="113"/>
       <c r="I34" s="120">
@@ -16312,11 +16326,11 @@
         <v>163</v>
       </c>
       <c r="R34" s="90" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S34" s="89"/>
       <c r="T34" s="114" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="U34" s="114" t="s">
         <v>165</v>
@@ -16335,7 +16349,7 @@
     <row r="35" spans="1:31" ht="15" customHeight="1">
       <c r="A35" s="199"/>
       <c r="B35" s="229" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C35" s="200"/>
       <c r="D35" s="201"/>
@@ -16375,7 +16389,7 @@
     </row>
     <row r="36" spans="1:31" ht="15" customHeight="1">
       <c r="A36" s="107" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B36" s="107"/>
       <c r="C36" s="124"/>
@@ -16416,10 +16430,10 @@
     </row>
     <row r="37" spans="1:31" ht="37.049999999999997" customHeight="1">
       <c r="A37" s="88" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B37" s="88" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C37" s="120">
         <v>16.899999999999999</v>
@@ -16432,7 +16446,7 @@
         <v>163</v>
       </c>
       <c r="G37" s="114" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H37" s="113"/>
       <c r="I37" s="120">
@@ -16452,7 +16466,7 @@
       </c>
       <c r="N37" s="89"/>
       <c r="O37" s="291">
-        <f t="shared" ref="O37" si="4">J37-I37</f>
+        <f>IF(OR(ISBLANK(I37),ISBLANK(J37)),"",J37-I37)</f>
         <v>-0.87999999999999901</v>
       </c>
       <c r="P37" s="89"/>
@@ -16464,10 +16478,10 @@
       </c>
       <c r="S37" s="89"/>
       <c r="T37" s="114" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="U37" s="114" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="V37" s="51"/>
       <c r="W37" s="51"/>
@@ -16483,7 +16497,7 @@
     <row r="38" spans="1:31" ht="15" customHeight="1">
       <c r="A38" s="100"/>
       <c r="B38" s="100" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C38" s="101"/>
       <c r="D38" s="101"/>
@@ -16523,7 +16537,7 @@
     <row r="39" spans="1:31" ht="15" customHeight="1">
       <c r="A39" s="103"/>
       <c r="B39" s="83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C39" s="83"/>
       <c r="D39" s="83"/>
@@ -16560,7 +16574,7 @@
     <row r="40" spans="1:31" ht="15" customHeight="1">
       <c r="A40" s="103"/>
       <c r="B40" s="103" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C40" s="83"/>
       <c r="D40" s="83"/>
@@ -16596,7 +16610,7 @@
     <row r="41" spans="1:31" ht="15" customHeight="1">
       <c r="A41" s="116"/>
       <c r="B41" s="116" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C41" s="86"/>
       <c r="D41" s="86"/>
@@ -16633,7 +16647,7 @@
     <row r="42" spans="1:31" ht="15" customHeight="1">
       <c r="A42" s="116"/>
       <c r="B42" s="116" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C42" s="86"/>
       <c r="D42" s="86"/>
@@ -16701,7 +16715,7 @@
     </row>
     <row r="44" spans="1:31" ht="15" customHeight="1">
       <c r="A44" s="76" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B44" s="76"/>
       <c r="C44" s="51"/>
@@ -16735,7 +16749,7 @@
     </row>
     <row r="45" spans="1:31" ht="15" customHeight="1">
       <c r="A45" s="77" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B45" s="77"/>
       <c r="C45" s="13"/>
@@ -16769,7 +16783,7 @@
     </row>
     <row r="46" spans="1:31" ht="15" customHeight="1">
       <c r="A46" s="77" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B46" s="77"/>
       <c r="C46" s="13"/>
@@ -16803,7 +16817,7 @@
     </row>
     <row r="47" spans="1:31" ht="15" customHeight="1">
       <c r="A47" s="77" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B47" s="77"/>
       <c r="C47" s="13"/>
@@ -16837,7 +16851,7 @@
     </row>
     <row r="48" spans="1:31" ht="15" customHeight="1">
       <c r="A48" s="77" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="B48" s="77"/>
       <c r="C48" s="13"/>
@@ -16871,7 +16885,7 @@
     </row>
     <row r="49" spans="1:31" ht="15" customHeight="1">
       <c r="A49" s="306" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B49" s="306"/>
       <c r="C49" s="306"/>
@@ -17004,7 +17018,7 @@
     </row>
     <row r="53" spans="1:31" ht="15" customHeight="1">
       <c r="A53" s="78" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B53" s="77"/>
       <c r="C53" s="13"/>
@@ -17038,7 +17052,7 @@
     </row>
     <row r="54" spans="1:31" ht="15" customHeight="1">
       <c r="A54" s="77" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B54" s="77"/>
       <c r="C54" s="13"/>
@@ -17072,7 +17086,7 @@
     </row>
     <row r="55" spans="1:31" ht="15" customHeight="1">
       <c r="A55" s="77" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B55" s="77"/>
       <c r="C55" s="13"/>
@@ -17106,7 +17120,7 @@
     </row>
     <row r="56" spans="1:31" ht="15" customHeight="1">
       <c r="A56" s="77" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B56" s="77"/>
       <c r="C56" s="13"/>
@@ -17140,7 +17154,7 @@
     </row>
     <row r="57" spans="1:31" ht="15" customHeight="1">
       <c r="A57" s="77" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B57" s="77"/>
       <c r="C57" s="13"/>
@@ -17174,7 +17188,7 @@
     </row>
     <row r="58" spans="1:31" ht="15" customHeight="1">
       <c r="A58" s="77" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
@@ -17208,7 +17222,7 @@
     </row>
     <row r="59" spans="1:31" ht="15" customHeight="1">
       <c r="A59" s="77" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B59" s="77"/>
       <c r="C59" s="13"/>
@@ -17274,7 +17288,7 @@
     </row>
     <row r="61" spans="1:31" ht="15" customHeight="1">
       <c r="A61" s="77" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
@@ -17308,7 +17322,7 @@
     </row>
     <row r="62" spans="1:31" ht="15" customHeight="1">
       <c r="A62" s="79" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B62" s="80"/>
       <c r="C62" s="13"/>
@@ -17608,99 +17622,23 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="5" id="{13E72558-9E1F-4FE2-AEBD-91E812E652F5}">
-            <x14:iconSet showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>-100</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>O13:O16</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="4" id="{EAFDFEA2-7E28-42E2-B792-CBF43C344CF6}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
               </x14:cfvo>
               <x14:cfvo type="num">
-                <xm:f>-100</xm:f>
+                <xm:f>0</xm:f>
               </x14:cfvo>
               <x14:cfvo type="num">
-                <xm:f>0</xm:f>
+                <xm:f>9.9999999999999996E-24</xm:f>
               </x14:cfvo>
+              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
               <x14:cfIcon iconSet="3Arrows" iconId="1"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
               <x14:cfIcon iconSet="3Arrows" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>O19:O22</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{1C147B90-31F0-432B-BAE8-7033175F5FE1}">
-            <x14:iconSet showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>-100</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>O25:O27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{3B786A4F-F49A-47BA-8740-5FC88F779DCE}">
-            <x14:iconSet showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>-100</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>O30:O34</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{D89AAE43-83F0-42F6-A847-63B116565B3D}">
-            <x14:iconSet showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>-100</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>O37</xm:sqref>
+          <xm:sqref>O13:O37</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -17814,7 +17752,7 @@
         <v>121</v>
       </c>
       <c r="C4" s="318" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D4" s="318"/>
       <c r="E4" s="318"/>
@@ -18293,7 +18231,7 @@
     </row>
     <row r="13" spans="1:39">
       <c r="B13" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C13" s="210">
         <v>12.7003</v>
@@ -18370,7 +18308,7 @@
     </row>
     <row r="14" spans="1:39">
       <c r="B14" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C14" s="210">
         <v>9.8623410000000007</v>
@@ -18447,7 +18385,7 @@
     </row>
     <row r="15" spans="1:39">
       <c r="B15" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C15" s="210">
         <v>98.166569999999993</v>
@@ -18524,7 +18462,7 @@
     </row>
     <row r="16" spans="1:39">
       <c r="B16" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C16" s="212">
         <v>64.212990000000005</v>
@@ -18601,7 +18539,7 @@
     </row>
     <row r="17" spans="2:26">
       <c r="B17" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C17" s="210">
         <v>100</v>
@@ -18678,7 +18616,7 @@
     </row>
     <row r="18" spans="2:26">
       <c r="B18" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C18" s="210">
         <v>11.74239843</v>
@@ -18755,7 +18693,7 @@
     </row>
     <row r="19" spans="2:26">
       <c r="B19" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="210"/>
@@ -18812,7 +18750,7 @@
     </row>
     <row r="20" spans="2:26" ht="21.6">
       <c r="B20" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C20" s="210">
         <v>27.2</v>
@@ -18889,7 +18827,7 @@
     </row>
     <row r="21" spans="2:26">
       <c r="B21" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C21" s="210">
         <v>21</v>
@@ -18966,7 +18904,7 @@
     </row>
     <row r="22" spans="2:26" ht="15" thickBot="1">
       <c r="B22" s="213" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C22" s="214"/>
       <c r="D22" s="214"/>
@@ -18995,7 +18933,7 @@
     </row>
     <row r="23" spans="2:26">
       <c r="B23" s="215" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C23" s="216">
         <v>1</v>
@@ -19072,7 +19010,7 @@
     </row>
     <row r="24" spans="2:26">
       <c r="B24" s="217" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C24" s="210">
         <v>1</v>
@@ -19555,42 +19493,42 @@
       <c r="B8" s="55">
         <v>6</v>
       </c>
-      <c r="C8" s="56">
+      <c r="C8" s="56" t="e">
         <f>IF(INDEX(UHC_summary!I$1:I$100,MATCH(UHC_Inter!$A8,UHC_summary!$B$1:$B$100,0))=0,"",INDEX(UHC_summary!I$1:I$100,MATCH(UHC_Inter!$A8,UHC_summary!$B$1:$B$100,0)))</f>
-        <v>64.595253999999997</v>
-      </c>
-      <c r="D8" s="56">
+        <v>#N/A</v>
+      </c>
+      <c r="D8" s="56" t="e">
         <f>IF(INDEX(UHC_summary!J$1:J$100,MATCH(UHC_Inter!$A8,UHC_summary!$B$1:$B$100,0))=0,"",INDEX(UHC_summary!J$1:J$100,MATCH(UHC_Inter!$A8,UHC_summary!$B$1:$B$100,0)))</f>
-        <v>72.525628659999995</v>
-      </c>
-      <c r="E8" s="56">
+        <v>#N/A</v>
+      </c>
+      <c r="E8" s="56" t="e">
         <f t="shared" si="0"/>
-        <v>72.525628659999995</v>
+        <v>#N/A</v>
       </c>
       <c r="F8" s="56" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G8" s="56">
+      <c r="G8" s="56" t="e">
         <f t="shared" si="2"/>
-        <v>7.9303746599999982</v>
+        <v>#N/A</v>
       </c>
       <c r="H8" s="56" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="I8" s="56" t="str">
+      <c r="I8" s="56" t="e">
         <f>IF(INDEX(UHC_summary!D$1:D$100,MATCH(UHC_Inter!$A8,UHC_summary!$B$1:$B$100,0))=0,"",INDEX(UHC_summary!D$1:D$100,MATCH(UHC_Inter!$A8,UHC_summary!$B$1:$B$100,0)))</f>
-        <v/>
-      </c>
-      <c r="J8" s="220">
+        <v>#N/A</v>
+      </c>
+      <c r="J8" s="220" t="e">
         <f>IF(INDEX(UHC_summary!E$1:E$100,MATCH(UHC_Inter!$A8,UHC_summary!$B$1:$B$100,0))=0,"",INDEX(UHC_summary!E$1:E$100,MATCH(UHC_Inter!$A8,UHC_summary!$B$1:$B$100,0)))</f>
-        <v>2018</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="91" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B9" s="55">
         <v>7</v>
@@ -19630,7 +19568,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="108" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B10" s="55">
         <v>8</v>
@@ -19670,7 +19608,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="91" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B11" s="55">
         <v>9</v>
@@ -19710,7 +19648,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="88" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B12" s="55">
         <v>10</v>
@@ -19750,7 +19688,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="108" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B13" s="55">
         <v>11</v>
@@ -19790,7 +19728,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="91" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B14" s="55">
         <v>12</v>
@@ -19830,7 +19768,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="88" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B15" s="55">
         <v>13</v>
@@ -20071,7 +20009,7 @@
     </row>
     <row r="2" spans="1:31" ht="23.25" customHeight="1">
       <c r="A2" s="68" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -20166,7 +20104,7 @@
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="183" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B5" s="183"/>
       <c r="C5" s="13"/>
@@ -20206,7 +20144,7 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="183" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B6" s="183"/>
       <c r="C6" s="13"/>
@@ -20319,13 +20257,13 @@
         <v>121</v>
       </c>
       <c r="B9" s="324" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C9" s="327" t="s">
+        <v>268</v>
+      </c>
+      <c r="D9" s="324" t="s">
         <v>269</v>
-      </c>
-      <c r="D9" s="324" t="s">
-        <v>270</v>
       </c>
       <c r="E9" s="327" t="s">
         <v>87</v>
@@ -20338,12 +20276,12 @@
       </c>
       <c r="H9" s="148"/>
       <c r="I9" s="326" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J9" s="326"/>
       <c r="K9" s="153"/>
       <c r="L9" s="326" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="M9" s="326"/>
       <c r="N9" s="153"/>
@@ -20413,7 +20351,7 @@
     </row>
     <row r="11" spans="1:31">
       <c r="A11" s="137" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B11" s="137"/>
       <c r="C11" s="138"/>
@@ -20446,7 +20384,7 @@
     </row>
     <row r="12" spans="1:31" ht="15" customHeight="1">
       <c r="A12" s="156" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B12" s="156"/>
       <c r="C12" s="225">
@@ -20462,7 +20400,7 @@
         <v>163</v>
       </c>
       <c r="G12" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H12" s="156"/>
       <c r="I12" s="225">
@@ -20489,7 +20427,7 @@
       </c>
       <c r="Q12" s="158"/>
       <c r="R12" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S12" s="160" t="s">
         <v>165</v>
@@ -20507,7 +20445,7 @@
     </row>
     <row r="13" spans="1:31" ht="20.399999999999999">
       <c r="A13" s="161" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B13" s="161"/>
       <c r="C13" s="226">
@@ -20523,7 +20461,7 @@
         <v>163</v>
       </c>
       <c r="G13" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H13" s="161"/>
       <c r="I13" s="226">
@@ -20550,7 +20488,7 @@
       </c>
       <c r="Q13" s="163"/>
       <c r="R13" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S13" s="160" t="s">
         <v>165</v>
@@ -20568,7 +20506,7 @@
     </row>
     <row r="14" spans="1:31" ht="20.399999999999999">
       <c r="A14" s="161" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B14" s="161"/>
       <c r="C14" s="226">
@@ -20584,7 +20522,7 @@
         <v>163</v>
       </c>
       <c r="G14" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H14" s="161"/>
       <c r="I14" s="226">
@@ -20611,7 +20549,7 @@
       </c>
       <c r="Q14" s="163"/>
       <c r="R14" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S14" s="160" t="s">
         <v>165</v>
@@ -20629,7 +20567,7 @@
     </row>
     <row r="15" spans="1:31">
       <c r="A15" s="161" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B15" s="161"/>
       <c r="C15" s="226">
@@ -20645,7 +20583,7 @@
         <v>163</v>
       </c>
       <c r="G15" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H15" s="161"/>
       <c r="I15" s="226">
@@ -20672,7 +20610,7 @@
       </c>
       <c r="Q15" s="163"/>
       <c r="R15" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S15" s="160" t="s">
         <v>165</v>
@@ -20690,7 +20628,7 @@
     </row>
     <row r="16" spans="1:31">
       <c r="A16" s="161" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B16" s="161"/>
       <c r="C16" s="226">
@@ -20706,7 +20644,7 @@
         <v>163</v>
       </c>
       <c r="G16" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H16" s="161"/>
       <c r="I16" s="226">
@@ -20733,7 +20671,7 @@
       </c>
       <c r="Q16" s="163"/>
       <c r="R16" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S16" s="160" t="s">
         <v>165</v>
@@ -20751,7 +20689,7 @@
     </row>
     <row r="17" spans="1:31" ht="15" customHeight="1">
       <c r="A17" s="161" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B17" s="161"/>
       <c r="C17" s="226">
@@ -20767,7 +20705,7 @@
         <v>163</v>
       </c>
       <c r="G17" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H17" s="161"/>
       <c r="I17" s="226">
@@ -20794,7 +20732,7 @@
       </c>
       <c r="Q17" s="163"/>
       <c r="R17" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S17" s="160" t="s">
         <v>165</v>
@@ -20812,7 +20750,7 @@
     </row>
     <row r="18" spans="1:31" ht="15" customHeight="1">
       <c r="A18" s="161" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B18" s="161"/>
       <c r="C18" s="226">
@@ -20828,7 +20766,7 @@
         <v>163</v>
       </c>
       <c r="G18" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H18" s="161"/>
       <c r="I18" s="226">
@@ -20855,7 +20793,7 @@
       </c>
       <c r="Q18" s="163"/>
       <c r="R18" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S18" s="160" t="s">
         <v>165</v>
@@ -20873,7 +20811,7 @@
     </row>
     <row r="19" spans="1:31">
       <c r="A19" s="161" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B19" s="161"/>
       <c r="C19" s="226">
@@ -20889,7 +20827,7 @@
         <v>163</v>
       </c>
       <c r="G19" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H19" s="161"/>
       <c r="I19" s="226">
@@ -20916,7 +20854,7 @@
       </c>
       <c r="Q19" s="163"/>
       <c r="R19" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S19" s="160" t="s">
         <v>165</v>
@@ -20934,7 +20872,7 @@
     </row>
     <row r="20" spans="1:31">
       <c r="A20" s="161" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B20" s="161"/>
       <c r="C20" s="226">
@@ -20950,7 +20888,7 @@
         <v>163</v>
       </c>
       <c r="G20" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H20" s="161"/>
       <c r="I20" s="226">
@@ -20977,7 +20915,7 @@
       </c>
       <c r="Q20" s="163"/>
       <c r="R20" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S20" s="160" t="s">
         <v>165</v>
@@ -20995,7 +20933,7 @@
     </row>
     <row r="21" spans="1:31">
       <c r="A21" s="161" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B21" s="161"/>
       <c r="C21" s="226">
@@ -21011,7 +20949,7 @@
         <v>163</v>
       </c>
       <c r="G21" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H21" s="161"/>
       <c r="I21" s="226">
@@ -21038,7 +20976,7 @@
       </c>
       <c r="Q21" s="163"/>
       <c r="R21" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S21" s="160" t="s">
         <v>165</v>
@@ -21056,7 +20994,7 @@
     </row>
     <row r="22" spans="1:31">
       <c r="A22" s="161" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B22" s="161"/>
       <c r="C22" s="226">
@@ -21072,7 +21010,7 @@
         <v>163</v>
       </c>
       <c r="G22" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H22" s="161"/>
       <c r="I22" s="226">
@@ -21099,7 +21037,7 @@
       </c>
       <c r="Q22" s="163"/>
       <c r="R22" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S22" s="160" t="s">
         <v>165</v>
@@ -21117,7 +21055,7 @@
     </row>
     <row r="23" spans="1:31" ht="15" customHeight="1">
       <c r="A23" s="161" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B23" s="161"/>
       <c r="C23" s="226">
@@ -21133,7 +21071,7 @@
         <v>163</v>
       </c>
       <c r="G23" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H23" s="161"/>
       <c r="I23" s="226">
@@ -21160,7 +21098,7 @@
       </c>
       <c r="Q23" s="163"/>
       <c r="R23" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S23" s="160" t="s">
         <v>165</v>
@@ -21178,7 +21116,7 @@
     </row>
     <row r="24" spans="1:31" ht="15" customHeight="1">
       <c r="A24" s="161" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B24" s="161"/>
       <c r="C24" s="226">
@@ -21194,7 +21132,7 @@
         <v>163</v>
       </c>
       <c r="G24" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H24" s="165"/>
       <c r="I24" s="226">
@@ -21221,7 +21159,7 @@
       </c>
       <c r="Q24" s="163"/>
       <c r="R24" s="160" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S24" s="160" t="s">
         <v>165</v>
@@ -21240,7 +21178,7 @@
     <row r="25" spans="1:31">
       <c r="A25" s="141"/>
       <c r="B25" s="228" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C25" s="142">
         <f>AVERAGE(C12:C24)</f>
@@ -21290,7 +21228,7 @@
     </row>
     <row r="26" spans="1:31">
       <c r="A26" s="137" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B26" s="137"/>
       <c r="C26" s="138"/>
@@ -21323,10 +21261,10 @@
     </row>
     <row r="27" spans="1:31">
       <c r="A27" s="161" t="s">
+        <v>273</v>
+      </c>
+      <c r="B27" s="161" t="s">
         <v>274</v>
-      </c>
-      <c r="B27" s="161" t="s">
-        <v>275</v>
       </c>
       <c r="C27" s="226">
         <v>96</v>
@@ -21339,7 +21277,7 @@
         <v>90</v>
       </c>
       <c r="G27" s="160" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H27" s="161"/>
       <c r="I27" s="226">
@@ -21361,7 +21299,7 @@
       </c>
       <c r="Q27" s="163"/>
       <c r="R27" s="160" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S27" s="160"/>
       <c r="V27" s="51"/>
@@ -21377,10 +21315,10 @@
     </row>
     <row r="28" spans="1:31">
       <c r="A28" s="161" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B28" s="161" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C28" s="226">
         <v>98</v>
@@ -21393,7 +21331,7 @@
         <v>90</v>
       </c>
       <c r="G28" s="160" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H28" s="161"/>
       <c r="I28" s="226">
@@ -21415,7 +21353,7 @@
       </c>
       <c r="Q28" s="163"/>
       <c r="R28" s="160" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S28" s="160" t="s">
         <v>165</v>
@@ -21433,13 +21371,13 @@
     </row>
     <row r="29" spans="1:31" s="174" customFormat="1">
       <c r="A29" s="168" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B29" s="168" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C29" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D29" s="169"/>
       <c r="E29" s="170"/>
@@ -21447,10 +21385,10 @@
       <c r="G29" s="171"/>
       <c r="H29" s="168"/>
       <c r="I29" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J29" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K29" s="169"/>
       <c r="L29" s="169"/>
@@ -21476,13 +21414,13 @@
     </row>
     <row r="30" spans="1:31" s="174" customFormat="1">
       <c r="A30" s="168" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B30" s="168" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C30" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D30" s="169"/>
       <c r="E30" s="170"/>
@@ -21490,10 +21428,10 @@
       <c r="G30" s="171"/>
       <c r="H30" s="168"/>
       <c r="I30" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J30" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K30" s="169"/>
       <c r="L30" s="169"/>
@@ -21519,13 +21457,13 @@
     </row>
     <row r="31" spans="1:31" s="174" customFormat="1">
       <c r="A31" s="168" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B31" s="168" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C31" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D31" s="169"/>
       <c r="E31" s="170"/>
@@ -21533,10 +21471,10 @@
       <c r="G31" s="171"/>
       <c r="H31" s="168"/>
       <c r="I31" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J31" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K31" s="169"/>
       <c r="L31" s="169"/>
@@ -21562,13 +21500,13 @@
     </row>
     <row r="32" spans="1:31" s="174" customFormat="1">
       <c r="A32" s="168" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B32" s="168" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C32" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D32" s="169"/>
       <c r="E32" s="170"/>
@@ -21576,10 +21514,10 @@
       <c r="G32" s="171"/>
       <c r="H32" s="168"/>
       <c r="I32" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J32" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K32" s="169"/>
       <c r="L32" s="169"/>
@@ -21605,13 +21543,13 @@
     </row>
     <row r="33" spans="1:31" s="174" customFormat="1">
       <c r="A33" s="168" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B33" s="168" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C33" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D33" s="169"/>
       <c r="E33" s="170"/>
@@ -21619,10 +21557,10 @@
       <c r="G33" s="171"/>
       <c r="H33" s="168"/>
       <c r="I33" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J33" s="227" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K33" s="169"/>
       <c r="L33" s="169"/>
@@ -21648,10 +21586,10 @@
     </row>
     <row r="34" spans="1:31">
       <c r="A34" s="161" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B34" s="161" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C34" s="162"/>
       <c r="D34" s="162"/>
@@ -21683,10 +21621,10 @@
     </row>
     <row r="35" spans="1:31">
       <c r="A35" s="161" t="s">
+        <v>280</v>
+      </c>
+      <c r="B35" s="161" t="s">
         <v>281</v>
-      </c>
-      <c r="B35" s="161" t="s">
-        <v>282</v>
       </c>
       <c r="C35" s="162"/>
       <c r="D35" s="162"/>
@@ -21718,10 +21656,10 @@
     </row>
     <row r="36" spans="1:31">
       <c r="A36" s="161" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B36" s="161" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C36" s="162"/>
       <c r="D36" s="162"/>
@@ -21754,7 +21692,7 @@
     <row r="37" spans="1:31">
       <c r="A37" s="141"/>
       <c r="B37" s="228" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C37" s="188">
         <f>AVERAGE(C27:C36)</f>
@@ -21798,7 +21736,7 @@
     </row>
     <row r="38" spans="1:31" ht="40.049999999999997" customHeight="1">
       <c r="A38" s="137" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B38" s="137"/>
       <c r="C38" s="138"/>
@@ -21831,13 +21769,13 @@
     </row>
     <row r="39" spans="1:31" ht="20.399999999999999">
       <c r="A39" s="161" t="s">
+        <v>284</v>
+      </c>
+      <c r="B39" s="161" t="s">
         <v>285</v>
       </c>
-      <c r="B39" s="161" t="s">
-        <v>286</v>
-      </c>
       <c r="C39" s="162" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D39" s="162"/>
       <c r="E39" s="163">
@@ -21847,7 +21785,7 @@
         <v>163</v>
       </c>
       <c r="G39" s="160" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H39" s="161"/>
       <c r="I39" s="162">
@@ -21866,7 +21804,7 @@
       </c>
       <c r="Q39" s="163"/>
       <c r="R39" s="160" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S39" s="160" t="s">
         <v>165</v>
@@ -21884,13 +21822,13 @@
     </row>
     <row r="40" spans="1:31" ht="20.399999999999999">
       <c r="A40" s="161" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B40" s="161" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C40" s="162" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D40" s="162"/>
       <c r="E40" s="163">
@@ -21900,7 +21838,7 @@
         <v>163</v>
       </c>
       <c r="G40" s="160" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H40" s="161"/>
       <c r="I40" s="162">
@@ -21919,7 +21857,7 @@
       </c>
       <c r="Q40" s="163"/>
       <c r="R40" s="160" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S40" s="160" t="s">
         <v>165</v>
@@ -21937,13 +21875,13 @@
     </row>
     <row r="41" spans="1:31" ht="20.399999999999999">
       <c r="A41" s="161" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B41" s="161" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C41" s="162" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D41" s="162"/>
       <c r="E41" s="163">
@@ -21953,7 +21891,7 @@
         <v>163</v>
       </c>
       <c r="G41" s="160" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H41" s="161"/>
       <c r="I41" s="162">
@@ -21972,7 +21910,7 @@
       </c>
       <c r="Q41" s="163"/>
       <c r="R41" s="160" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S41" s="160" t="s">
         <v>165</v>
@@ -21991,7 +21929,7 @@
     <row r="42" spans="1:31">
       <c r="A42" s="141"/>
       <c r="B42" s="228" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C42" s="142" t="str">
         <f>IFERROR(AVERAGE(C39:C41),"")</f>
@@ -22036,7 +21974,7 @@
     <row r="43" spans="1:31" ht="15" customHeight="1">
       <c r="A43" s="137"/>
       <c r="B43" s="230" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C43" s="181"/>
       <c r="D43" s="181"/>
@@ -22078,7 +22016,7 @@
     <row r="44" spans="1:31" ht="15" customHeight="1">
       <c r="A44" s="137"/>
       <c r="B44" s="230" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C44" s="181"/>
       <c r="D44" s="181"/>
@@ -22114,7 +22052,7 @@
     <row r="45" spans="1:31" ht="15" customHeight="1">
       <c r="A45" s="137"/>
       <c r="B45" s="231" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C45" s="181"/>
       <c r="D45" s="138"/>
@@ -22150,7 +22088,7 @@
     <row r="46" spans="1:31" ht="15" customHeight="1">
       <c r="A46" s="137"/>
       <c r="B46" s="230" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C46" s="181"/>
       <c r="D46" s="138"/>
@@ -22186,7 +22124,7 @@
     <row r="47" spans="1:31" ht="15" customHeight="1">
       <c r="A47" s="137"/>
       <c r="B47" s="230" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C47" s="181"/>
       <c r="D47" s="138"/>
@@ -22221,7 +22159,7 @@
     </row>
     <row r="48" spans="1:31" ht="15" customHeight="1">
       <c r="A48" s="67" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B48" s="66"/>
       <c r="C48" s="134"/>
@@ -22251,7 +22189,7 @@
     </row>
     <row r="49" spans="1:31" ht="15" customHeight="1">
       <c r="A49" s="67" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B49" s="67"/>
       <c r="C49" s="134"/>
@@ -22281,7 +22219,7 @@
     </row>
     <row r="50" spans="1:31" ht="15" customHeight="1">
       <c r="A50" s="135" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B50" s="135"/>
       <c r="C50" s="134"/>
@@ -22673,7 +22611,7 @@
         <v>121</v>
       </c>
       <c r="C4" s="330" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D4" s="330"/>
       <c r="E4" s="330"/>
@@ -22803,7 +22741,7 @@
     </row>
     <row r="6" spans="1:39">
       <c r="B6" s="217" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" s="198">
         <v>1.3</v>
@@ -22880,7 +22818,7 @@
     </row>
     <row r="7" spans="1:39">
       <c r="B7" s="22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C7" s="23">
         <v>1.3</v>
@@ -22957,7 +22895,7 @@
     </row>
     <row r="8" spans="1:39">
       <c r="B8" s="22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
@@ -22986,7 +22924,7 @@
     </row>
     <row r="9" spans="1:39">
       <c r="B9" s="22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C9" s="23">
         <v>8.1999999999999993</v>
@@ -23063,7 +23001,7 @@
     </row>
     <row r="10" spans="1:39">
       <c r="B10" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C10" s="63"/>
       <c r="D10" s="63"/>
@@ -23092,7 +23030,7 @@
     </row>
     <row r="11" spans="1:39">
       <c r="B11" s="22" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C11" s="23">
         <v>9.4</v>
@@ -23169,7 +23107,7 @@
     </row>
     <row r="12" spans="1:39">
       <c r="B12" s="22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
@@ -23200,7 +23138,7 @@
     </row>
     <row r="13" spans="1:39">
       <c r="B13" s="22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
@@ -23229,7 +23167,7 @@
     </row>
     <row r="14" spans="1:39">
       <c r="B14" s="22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C14" s="23">
         <v>12.7003</v>
@@ -23306,7 +23244,7 @@
     </row>
     <row r="15" spans="1:39">
       <c r="B15" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C15" s="198">
         <v>9.8623410000000007</v>
@@ -23383,7 +23321,7 @@
     </row>
     <row r="16" spans="1:39">
       <c r="B16" s="22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C16" s="198">
         <v>98.166569999999993</v>
@@ -23460,7 +23398,7 @@
     </row>
     <row r="17" spans="2:26">
       <c r="B17" s="22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C17" s="198">
         <v>64.212990000000005</v>
@@ -23537,7 +23475,7 @@
     </row>
     <row r="18" spans="2:26">
       <c r="B18" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C18" s="198">
         <v>100</v>
@@ -23614,7 +23552,7 @@
     </row>
     <row r="19" spans="2:26">
       <c r="B19" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C19" s="198">
         <v>11.74239843</v>
@@ -23691,7 +23629,7 @@
     </row>
     <row r="20" spans="2:26">
       <c r="B20" s="22" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C20" s="198">
         <v>1</v>
@@ -23768,7 +23706,7 @@
     </row>
     <row r="21" spans="2:26">
       <c r="B21" s="22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C21" s="198"/>
       <c r="D21" s="198"/>
@@ -23825,7 +23763,7 @@
     </row>
     <row r="22" spans="2:26">
       <c r="B22" s="22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C22" s="198">
         <v>27.2</v>
@@ -23902,7 +23840,7 @@
     </row>
     <row r="23" spans="2:26">
       <c r="B23" s="22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C23" s="198">
         <v>21</v>
@@ -23979,7 +23917,7 @@
     </row>
     <row r="24" spans="2:26">
       <c r="B24" s="22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C24" s="198"/>
       <c r="D24" s="198"/>
@@ -24008,7 +23946,7 @@
     </row>
     <row r="25" spans="2:26">
       <c r="B25" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C25" s="198">
         <v>21</v>
@@ -24085,7 +24023,7 @@
     </row>
     <row r="26" spans="2:26">
       <c r="B26" s="22" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C26" s="198">
         <v>21</v>
@@ -24162,7 +24100,7 @@
     </row>
     <row r="27" spans="2:26">
       <c r="B27" s="22" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C27" s="198">
         <v>21</v>
@@ -24239,7 +24177,7 @@
     </row>
     <row r="28" spans="2:26">
       <c r="B28" s="22" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C28" s="198">
         <v>1</v>
@@ -24316,7 +24254,7 @@
     </row>
     <row r="29" spans="2:26">
       <c r="B29" s="22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C29" s="198">
         <v>21</v>
@@ -24393,7 +24331,7 @@
     </row>
     <row r="30" spans="2:26">
       <c r="B30" s="22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C30" s="198">
         <v>21</v>
@@ -24470,7 +24408,7 @@
     </row>
     <row r="31" spans="2:26">
       <c r="B31" s="22" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C31" s="198">
         <v>21</v>
@@ -24547,7 +24485,7 @@
     </row>
     <row r="32" spans="2:26">
       <c r="B32" s="22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C32" s="198">
         <v>1</v>

</xml_diff>

<commit_message>
Write and style UHC pillars
</commit_message>
<xml_diff>
--- a/inst/extdata/country_summary_template.xlsx
+++ b/inst/extdata/country_summary_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F424A3E1-8E83-4DF0-98D7-62A450047148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB73616-FAAC-4C3D-80F8-1F635DF46EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="26136" windowHeight="16896" tabRatio="942" activeTab="2" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
   </bookViews>
@@ -4357,7 +4357,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E07B57CD-6590-440E-9084-B6B0393F13F2}" type="CELLRANGE">
+                    <a:fld id="{FB4499A7-FB12-4D96-94A8-8BC0D32647AA}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4418,7 +4418,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69F94930-D0BD-4044-8C1D-E8D942E6BDFA}" type="CELLRANGE">
+                    <a:fld id="{F06C920E-7870-440F-A81E-B7E85ED1FADB}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4479,7 +4479,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69971402-75AE-4E22-9A30-9AEDB4C960A4}" type="CELLRANGE">
+                    <a:fld id="{73713997-4C78-4B97-B398-5EA863CD3862}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4568,7 +4568,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EF22AEBE-FF93-419A-ADBF-3D5CCF00EB66}" type="CELLRANGE">
+                    <a:fld id="{C9F80784-CF77-4651-BFEB-6988AFB2DB0C}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4602,7 +4602,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FB442C29-6026-4175-BD42-9FD7C78542E7}" type="CELLRANGE">
+                    <a:fld id="{044C5E24-3DAE-44BD-8373-19D55D88DFB2}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4636,7 +4636,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{944D9DB4-2D29-4C34-977A-D88D3824780D}" type="CELLRANGE">
+                    <a:fld id="{53E6927A-4697-4A73-8EA5-E0545B7AE294}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4670,7 +4670,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5021FE3B-811D-4FC7-B2A3-7071F7BDFE19}" type="CELLRANGE">
+                    <a:fld id="{C918974D-3B7F-4687-8346-F3684C17F695}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4704,7 +4704,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0384E728-9EE1-499C-BA7F-01BD1C11EA24}" type="CELLRANGE">
+                    <a:fld id="{FCE5C2FA-A7B4-4686-98F3-4F9E969BD975}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4738,7 +4738,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{889FB31C-300B-43FB-ACCF-468D86221213}" type="CELLRANGE">
+                    <a:fld id="{EA77688B-C903-49D7-96C9-E23BBE76D945}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6549,7 +6549,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B54C23A3-9555-4577-848C-64E0A7B6AF29}" type="CELLRANGE">
+                    <a:fld id="{822839EC-3AC3-46B8-B9C6-4A6E1AC76E76}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6610,7 +6610,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CCDC4EA4-D849-4E34-9935-F8D4806478E8}" type="CELLRANGE">
+                    <a:fld id="{FC5E985D-49BF-460B-B40C-7AD8E17AB9B6}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6671,7 +6671,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D999897C-6BEB-46A0-A55A-BF6174CB7423}" type="CELLRANGE">
+                    <a:fld id="{70A56CE7-CE7F-4105-878D-8BD7BDA9EB73}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6705,7 +6705,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B953A3A-F294-482B-BE57-3910FFF77454}" type="CELLRANGE">
+                    <a:fld id="{54F59819-F4D7-4520-8015-25FB355535F3}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6766,7 +6766,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7B2D33BF-11B9-4B94-A70E-6B092E37DD4E}" type="CELLRANGE">
+                    <a:fld id="{877B40D8-F53D-4DF7-9D53-93DB7BCDF2E3}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6800,7 +6800,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED8DAC85-DD8B-48E1-B23F-D951873B1672}" type="CELLRANGE">
+                    <a:fld id="{3D7F4118-8D5A-448F-AF81-15F9430D5BD3}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6834,7 +6834,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40E4DD50-5C1C-4F70-93FB-038394447B75}" type="CELLRANGE">
+                    <a:fld id="{7D5D75C4-E86B-49B2-B020-9CCFADFD4A81}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6868,7 +6868,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48124EC9-6BFE-4524-AC41-EF4261DF36B4}" type="CELLRANGE">
+                    <a:fld id="{206DF580-815E-4B1F-8305-4CA2784BF359}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6902,7 +6902,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D364C426-7FB5-4083-827A-9322CE0104A5}" type="CELLRANGE">
+                    <a:fld id="{C4937B9F-94D0-4DEE-BFBE-92CCF45166C8}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6936,7 +6936,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D461230-90CC-4C8F-9D2A-9DE8A736E086}" type="CELLRANGE">
+                    <a:fld id="{8D08DC29-E6F6-4EA7-8E62-E97383835DC1}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6970,7 +6970,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4093D5B9-A7B6-4DB5-A2A1-BD68E249CB2D}" type="CELLRANGE">
+                    <a:fld id="{EB7AD025-9B85-4661-8581-D4E7E99F6889}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7004,7 +7004,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71D75CFC-2647-4CDF-8436-083F2392E65D}" type="CELLRANGE">
+                    <a:fld id="{D9B84CAA-2538-4890-A06E-2165DE19E1B4}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7038,7 +7038,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0CC48D71-2108-4CEF-B3FF-B9B6F645F80B}" type="CELLRANGE">
+                    <a:fld id="{B13D521F-BC31-48CF-9E67-04E38A8733F3}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>

</xml_diff>

<commit_message>
Finalize writting UHC summary data boxes
</commit_message>
<xml_diff>
--- a/inst/extdata/country_summary_template.xlsx
+++ b/inst/extdata/country_summary_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB73616-FAAC-4C3D-80F8-1F635DF46EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F069CA86-A9B4-4D09-80C7-B8B518678BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="26136" windowHeight="16896" tabRatio="942" activeTab="2" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
   </bookViews>
@@ -1830,29 +1830,34 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1865,6 +1870,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -2105,6 +2111,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -2118,6 +2125,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="18">
@@ -2665,7 +2673,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="357">
+  <cellXfs count="364">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3469,27 +3477,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="31" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3638,12 +3680,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -4357,7 +4393,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FB4499A7-FB12-4D96-94A8-8BC0D32647AA}" type="CELLRANGE">
+                    <a:fld id="{52AF2E62-9BF9-4468-8D0A-E613A5E33556}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4418,7 +4454,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F06C920E-7870-440F-A81E-B7E85ED1FADB}" type="CELLRANGE">
+                    <a:fld id="{0925C3DF-D4F7-4DCE-80E7-601E580697CF}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4479,7 +4515,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73713997-4C78-4B97-B398-5EA863CD3862}" type="CELLRANGE">
+                    <a:fld id="{0EECFAF7-2AAF-40AA-8AAA-4C0A47FDD8DD}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4568,7 +4604,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C9F80784-CF77-4651-BFEB-6988AFB2DB0C}" type="CELLRANGE">
+                    <a:fld id="{8EA0A50E-1C82-4658-BF1C-7AFC1557C595}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4602,7 +4638,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{044C5E24-3DAE-44BD-8373-19D55D88DFB2}" type="CELLRANGE">
+                    <a:fld id="{773C19D4-F3C8-482E-86AF-B72E982ED125}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4636,7 +4672,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{53E6927A-4697-4A73-8EA5-E0545B7AE294}" type="CELLRANGE">
+                    <a:fld id="{AACAE9A2-2AA1-45E3-A204-BD6BB99BA8EC}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4670,7 +4706,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C918974D-3B7F-4687-8346-F3684C17F695}" type="CELLRANGE">
+                    <a:fld id="{73002424-144D-4A2F-8C81-D38E5F8487E7}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4704,7 +4740,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FCE5C2FA-A7B4-4686-98F3-4F9E969BD975}" type="CELLRANGE">
+                    <a:fld id="{E119BC76-0746-43AF-9950-349D17EF926D}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4738,7 +4774,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA77688B-C903-49D7-96C9-E23BBE76D945}" type="CELLRANGE">
+                    <a:fld id="{B8CD1D01-63C7-49E6-ABDC-C8C0761BAE80}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6549,7 +6585,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{822839EC-3AC3-46B8-B9C6-4A6E1AC76E76}" type="CELLRANGE">
+                    <a:fld id="{4C962DFD-7857-4700-8855-FC64C98AF4C6}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6610,7 +6646,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC5E985D-49BF-460B-B40C-7AD8E17AB9B6}" type="CELLRANGE">
+                    <a:fld id="{BD81AED7-E1BC-4547-ADE3-4C63DA4E7A47}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6671,7 +6707,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70A56CE7-CE7F-4105-878D-8BD7BDA9EB73}" type="CELLRANGE">
+                    <a:fld id="{03076614-7912-45CA-939E-42A4573DD4A9}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6705,7 +6741,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54F59819-F4D7-4520-8015-25FB355535F3}" type="CELLRANGE">
+                    <a:fld id="{67DDC2D6-2284-438F-86F6-037498C3EC55}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6766,7 +6802,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{877B40D8-F53D-4DF7-9D53-93DB7BCDF2E3}" type="CELLRANGE">
+                    <a:fld id="{AB965C57-6897-476D-88B5-DE461CBE2E3F}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6800,7 +6836,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D7F4118-8D5A-448F-AF81-15F9430D5BD3}" type="CELLRANGE">
+                    <a:fld id="{0F04B170-9610-46DD-87B3-6DAE2EACF803}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6834,7 +6870,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D5D75C4-E86B-49B2-B020-9CCFADFD4A81}" type="CELLRANGE">
+                    <a:fld id="{6AD1100D-BCE7-4670-A811-038041F97DAE}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6868,7 +6904,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{206DF580-815E-4B1F-8305-4CA2784BF359}" type="CELLRANGE">
+                    <a:fld id="{025AB3CD-C717-44FF-AE23-9AB09CF1842A}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6902,7 +6938,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C4937B9F-94D0-4DEE-BFBE-92CCF45166C8}" type="CELLRANGE">
+                    <a:fld id="{2525D601-D721-4E0A-9781-423DD625BE99}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6936,7 +6972,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D08DC29-E6F6-4EA7-8E62-E97383835DC1}" type="CELLRANGE">
+                    <a:fld id="{86F99699-1841-498E-A8E9-40F5D3743A54}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6970,7 +7006,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB7AD025-9B85-4661-8581-D4E7E99F6889}" type="CELLRANGE">
+                    <a:fld id="{7B7F344A-F667-44E4-8026-65AE861F2CC1}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7004,7 +7040,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D9B84CAA-2538-4890-A06E-2165DE19E1B4}" type="CELLRANGE">
+                    <a:fld id="{25158C50-781E-4716-8BE8-6CDA82B05A8F}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7038,7 +7074,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B13D521F-BC31-48CF-9E67-04E38A8733F3}" type="CELLRANGE">
+                    <a:fld id="{330EC238-B412-4A22-9226-887B495C9FAF}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7938,664 +7974,664 @@
   <sheetData>
     <row r="1" spans="2:15" ht="10.5" customHeight="1"/>
     <row r="2" spans="2:15" ht="36" customHeight="1">
-      <c r="B2" s="300" t="s">
+      <c r="B2" s="309" t="s">
         <v>339</v>
       </c>
-      <c r="C2" s="300"/>
-      <c r="D2" s="300"/>
-      <c r="E2" s="300"/>
-      <c r="F2" s="300"/>
-      <c r="G2" s="300"/>
-      <c r="H2" s="300"/>
-      <c r="I2" s="300"/>
-      <c r="J2" s="300"/>
-      <c r="K2" s="300"/>
-      <c r="L2" s="300"/>
-      <c r="M2" s="300"/>
+      <c r="C2" s="309"/>
+      <c r="D2" s="309"/>
+      <c r="E2" s="309"/>
+      <c r="F2" s="309"/>
+      <c r="G2" s="309"/>
+      <c r="H2" s="309"/>
+      <c r="I2" s="309"/>
+      <c r="J2" s="309"/>
+      <c r="K2" s="309"/>
+      <c r="L2" s="309"/>
+      <c r="M2" s="309"/>
       <c r="N2" s="68"/>
       <c r="O2" s="68"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1">
-      <c r="B3" s="301" t="s">
+      <c r="B3" s="310" t="s">
         <v>439</v>
       </c>
-      <c r="C3" s="301"/>
-      <c r="D3" s="301"/>
-      <c r="E3" s="301"/>
-      <c r="F3" s="301"/>
-      <c r="G3" s="301"/>
-      <c r="H3" s="301"/>
-      <c r="I3" s="301"/>
-      <c r="J3" s="301"/>
-      <c r="K3" s="301"/>
-      <c r="L3" s="301"/>
-      <c r="M3" s="301"/>
+      <c r="C3" s="310"/>
+      <c r="D3" s="310"/>
+      <c r="E3" s="310"/>
+      <c r="F3" s="310"/>
+      <c r="G3" s="310"/>
+      <c r="H3" s="310"/>
+      <c r="I3" s="310"/>
+      <c r="J3" s="310"/>
+      <c r="K3" s="310"/>
+      <c r="L3" s="310"/>
+      <c r="M3" s="310"/>
       <c r="N3" s="222"/>
       <c r="O3" s="222"/>
     </row>
     <row r="4" spans="2:15" ht="18.75" customHeight="1">
-      <c r="B4" s="302" t="s">
+      <c r="B4" s="306" t="s">
         <v>340</v>
       </c>
-      <c r="C4" s="302"/>
-      <c r="D4" s="302"/>
-      <c r="E4" s="302"/>
-      <c r="F4" s="302"/>
-      <c r="G4" s="302"/>
-      <c r="H4" s="302"/>
-      <c r="I4" s="302"/>
-      <c r="J4" s="302"/>
-      <c r="K4" s="302"/>
-      <c r="L4" s="302"/>
-      <c r="M4" s="302"/>
+      <c r="C4" s="306"/>
+      <c r="D4" s="306"/>
+      <c r="E4" s="306"/>
+      <c r="F4" s="306"/>
+      <c r="G4" s="306"/>
+      <c r="H4" s="306"/>
+      <c r="I4" s="306"/>
+      <c r="J4" s="306"/>
+      <c r="K4" s="306"/>
+      <c r="L4" s="306"/>
+      <c r="M4" s="306"/>
       <c r="N4" s="223"/>
       <c r="O4" s="223"/>
     </row>
     <row r="5" spans="2:15" ht="15" customHeight="1">
-      <c r="B5" s="299" t="s">
+      <c r="B5" s="307" t="s">
         <v>361</v>
       </c>
-      <c r="C5" s="299"/>
-      <c r="D5" s="299"/>
-      <c r="E5" s="299"/>
-      <c r="F5" s="299"/>
-      <c r="G5" s="299"/>
-      <c r="H5" s="299"/>
-      <c r="I5" s="299"/>
-      <c r="J5" s="299"/>
-      <c r="K5" s="299"/>
-      <c r="L5" s="299"/>
-      <c r="M5" s="299"/>
+      <c r="C5" s="307"/>
+      <c r="D5" s="307"/>
+      <c r="E5" s="307"/>
+      <c r="F5" s="307"/>
+      <c r="G5" s="307"/>
+      <c r="H5" s="307"/>
+      <c r="I5" s="307"/>
+      <c r="J5" s="307"/>
+      <c r="K5" s="307"/>
+      <c r="L5" s="307"/>
+      <c r="M5" s="307"/>
       <c r="N5" s="222"/>
       <c r="O5" s="222"/>
     </row>
     <row r="6" spans="2:15" ht="15" customHeight="1">
-      <c r="B6" s="298" t="s">
+      <c r="B6" s="305" t="s">
         <v>362</v>
       </c>
-      <c r="C6" s="298"/>
-      <c r="D6" s="298"/>
-      <c r="E6" s="298"/>
-      <c r="F6" s="298"/>
-      <c r="G6" s="298"/>
-      <c r="H6" s="298"/>
-      <c r="I6" s="298"/>
-      <c r="J6" s="298"/>
-      <c r="K6" s="298"/>
-      <c r="L6" s="298"/>
-      <c r="M6" s="298"/>
+      <c r="C6" s="305"/>
+      <c r="D6" s="305"/>
+      <c r="E6" s="305"/>
+      <c r="F6" s="305"/>
+      <c r="G6" s="305"/>
+      <c r="H6" s="305"/>
+      <c r="I6" s="305"/>
+      <c r="J6" s="305"/>
+      <c r="K6" s="305"/>
+      <c r="L6" s="305"/>
+      <c r="M6" s="305"/>
       <c r="N6" s="224"/>
       <c r="O6" s="224"/>
     </row>
     <row r="7" spans="2:15" ht="15" customHeight="1">
-      <c r="B7" s="298" t="s">
+      <c r="B7" s="305" t="s">
         <v>363</v>
       </c>
-      <c r="C7" s="298"/>
-      <c r="D7" s="298"/>
-      <c r="E7" s="298"/>
-      <c r="F7" s="298"/>
-      <c r="G7" s="298"/>
-      <c r="H7" s="298"/>
-      <c r="I7" s="298"/>
-      <c r="J7" s="298"/>
-      <c r="K7" s="298"/>
-      <c r="L7" s="298"/>
-      <c r="M7" s="298"/>
+      <c r="C7" s="305"/>
+      <c r="D7" s="305"/>
+      <c r="E7" s="305"/>
+      <c r="F7" s="305"/>
+      <c r="G7" s="305"/>
+      <c r="H7" s="305"/>
+      <c r="I7" s="305"/>
+      <c r="J7" s="305"/>
+      <c r="K7" s="305"/>
+      <c r="L7" s="305"/>
+      <c r="M7" s="305"/>
       <c r="N7" s="224"/>
       <c r="O7" s="224"/>
     </row>
     <row r="8" spans="2:15" ht="21.75" customHeight="1">
-      <c r="B8" s="298" t="s">
+      <c r="B8" s="305" t="s">
         <v>364</v>
       </c>
-      <c r="C8" s="298"/>
-      <c r="D8" s="298"/>
-      <c r="E8" s="298"/>
-      <c r="F8" s="298"/>
-      <c r="G8" s="298"/>
-      <c r="H8" s="298"/>
-      <c r="I8" s="298"/>
-      <c r="J8" s="298"/>
-      <c r="K8" s="298"/>
-      <c r="L8" s="298"/>
-      <c r="M8" s="298"/>
+      <c r="C8" s="305"/>
+      <c r="D8" s="305"/>
+      <c r="E8" s="305"/>
+      <c r="F8" s="305"/>
+      <c r="G8" s="305"/>
+      <c r="H8" s="305"/>
+      <c r="I8" s="305"/>
+      <c r="J8" s="305"/>
+      <c r="K8" s="305"/>
+      <c r="L8" s="305"/>
+      <c r="M8" s="305"/>
       <c r="N8" s="224"/>
       <c r="O8" s="224"/>
     </row>
     <row r="9" spans="2:15" ht="30" customHeight="1">
-      <c r="B9" s="299" t="s">
+      <c r="B9" s="307" t="s">
         <v>341</v>
       </c>
-      <c r="C9" s="299"/>
-      <c r="D9" s="299"/>
-      <c r="E9" s="299"/>
-      <c r="F9" s="299"/>
-      <c r="G9" s="299"/>
-      <c r="H9" s="299"/>
-      <c r="I9" s="299"/>
-      <c r="J9" s="299"/>
-      <c r="K9" s="299"/>
-      <c r="L9" s="299"/>
+      <c r="C9" s="307"/>
+      <c r="D9" s="307"/>
+      <c r="E9" s="307"/>
+      <c r="F9" s="307"/>
+      <c r="G9" s="307"/>
+      <c r="H9" s="307"/>
+      <c r="I9" s="307"/>
+      <c r="J9" s="307"/>
+      <c r="K9" s="307"/>
+      <c r="L9" s="307"/>
     </row>
     <row r="10" spans="2:15" ht="33.75" customHeight="1">
-      <c r="B10" s="299" t="s">
+      <c r="B10" s="307" t="s">
         <v>342</v>
       </c>
-      <c r="C10" s="299"/>
-      <c r="D10" s="299"/>
-      <c r="E10" s="299"/>
-      <c r="F10" s="299"/>
-      <c r="G10" s="299"/>
-      <c r="H10" s="299"/>
-      <c r="I10" s="299"/>
-      <c r="J10" s="299"/>
-      <c r="K10" s="299"/>
-      <c r="L10" s="299"/>
+      <c r="C10" s="307"/>
+      <c r="D10" s="307"/>
+      <c r="E10" s="307"/>
+      <c r="F10" s="307"/>
+      <c r="G10" s="307"/>
+      <c r="H10" s="307"/>
+      <c r="I10" s="307"/>
+      <c r="J10" s="307"/>
+      <c r="K10" s="307"/>
+      <c r="L10" s="307"/>
     </row>
     <row r="11" spans="2:15" ht="21" customHeight="1">
-      <c r="B11" s="302" t="s">
+      <c r="B11" s="306" t="s">
         <v>343</v>
       </c>
-      <c r="C11" s="302"/>
-      <c r="D11" s="302"/>
-      <c r="E11" s="302"/>
-      <c r="F11" s="302"/>
-      <c r="G11" s="302"/>
-      <c r="H11" s="302"/>
-      <c r="I11" s="302"/>
-      <c r="J11" s="302"/>
-      <c r="K11" s="302"/>
-      <c r="L11" s="302"/>
-      <c r="M11" s="302"/>
+      <c r="C11" s="306"/>
+      <c r="D11" s="306"/>
+      <c r="E11" s="306"/>
+      <c r="F11" s="306"/>
+      <c r="G11" s="306"/>
+      <c r="H11" s="306"/>
+      <c r="I11" s="306"/>
+      <c r="J11" s="306"/>
+      <c r="K11" s="306"/>
+      <c r="L11" s="306"/>
+      <c r="M11" s="306"/>
       <c r="N11" s="69"/>
       <c r="O11" s="69"/>
     </row>
     <row r="12" spans="2:15">
-      <c r="B12" s="299" t="s">
+      <c r="B12" s="307" t="s">
         <v>344</v>
       </c>
-      <c r="C12" s="299"/>
-      <c r="D12" s="299"/>
-      <c r="E12" s="299"/>
-      <c r="F12" s="299"/>
-      <c r="G12" s="299"/>
-      <c r="H12" s="299"/>
-      <c r="I12" s="299"/>
-      <c r="J12" s="299"/>
-      <c r="K12" s="299"/>
-      <c r="L12" s="299"/>
-      <c r="M12" s="299"/>
+      <c r="C12" s="307"/>
+      <c r="D12" s="307"/>
+      <c r="E12" s="307"/>
+      <c r="F12" s="307"/>
+      <c r="G12" s="307"/>
+      <c r="H12" s="307"/>
+      <c r="I12" s="307"/>
+      <c r="J12" s="307"/>
+      <c r="K12" s="307"/>
+      <c r="L12" s="307"/>
+      <c r="M12" s="307"/>
     </row>
     <row r="13" spans="2:15" ht="27" customHeight="1">
-      <c r="B13" s="297" t="s">
+      <c r="B13" s="308" t="s">
         <v>371</v>
       </c>
-      <c r="C13" s="298"/>
-      <c r="D13" s="298"/>
-      <c r="E13" s="298"/>
-      <c r="F13" s="298"/>
-      <c r="G13" s="298"/>
-      <c r="H13" s="298"/>
-      <c r="I13" s="298"/>
-      <c r="J13" s="298"/>
-      <c r="K13" s="298"/>
-      <c r="L13" s="298"/>
-      <c r="M13" s="298"/>
+      <c r="C13" s="305"/>
+      <c r="D13" s="305"/>
+      <c r="E13" s="305"/>
+      <c r="F13" s="305"/>
+      <c r="G13" s="305"/>
+      <c r="H13" s="305"/>
+      <c r="I13" s="305"/>
+      <c r="J13" s="305"/>
+      <c r="K13" s="305"/>
+      <c r="L13" s="305"/>
+      <c r="M13" s="305"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="B14" s="297" t="s">
+      <c r="B14" s="308" t="s">
         <v>372</v>
       </c>
-      <c r="C14" s="298"/>
-      <c r="D14" s="298"/>
-      <c r="E14" s="298"/>
-      <c r="F14" s="298"/>
-      <c r="G14" s="298"/>
-      <c r="H14" s="298"/>
-      <c r="I14" s="298"/>
-      <c r="J14" s="298"/>
-      <c r="K14" s="298"/>
-      <c r="L14" s="298"/>
-      <c r="M14" s="298"/>
+      <c r="C14" s="305"/>
+      <c r="D14" s="305"/>
+      <c r="E14" s="305"/>
+      <c r="F14" s="305"/>
+      <c r="G14" s="305"/>
+      <c r="H14" s="305"/>
+      <c r="I14" s="305"/>
+      <c r="J14" s="305"/>
+      <c r="K14" s="305"/>
+      <c r="L14" s="305"/>
+      <c r="M14" s="305"/>
     </row>
     <row r="15" spans="2:15" ht="17.25" customHeight="1">
-      <c r="B15" s="297" t="s">
+      <c r="B15" s="308" t="s">
         <v>373</v>
       </c>
-      <c r="C15" s="298"/>
-      <c r="D15" s="298"/>
-      <c r="E15" s="298"/>
-      <c r="F15" s="298"/>
-      <c r="G15" s="298"/>
-      <c r="H15" s="298"/>
-      <c r="I15" s="298"/>
-      <c r="J15" s="298"/>
-      <c r="K15" s="298"/>
-      <c r="L15" s="298"/>
-      <c r="M15" s="298"/>
+      <c r="C15" s="305"/>
+      <c r="D15" s="305"/>
+      <c r="E15" s="305"/>
+      <c r="F15" s="305"/>
+      <c r="G15" s="305"/>
+      <c r="H15" s="305"/>
+      <c r="I15" s="305"/>
+      <c r="J15" s="305"/>
+      <c r="K15" s="305"/>
+      <c r="L15" s="305"/>
+      <c r="M15" s="305"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="B16" s="299" t="s">
+      <c r="B16" s="307" t="s">
         <v>370</v>
       </c>
-      <c r="C16" s="299"/>
-      <c r="D16" s="299"/>
-      <c r="E16" s="299"/>
-      <c r="F16" s="299"/>
-      <c r="G16" s="299"/>
-      <c r="H16" s="299"/>
-      <c r="I16" s="299"/>
-      <c r="J16" s="299"/>
-      <c r="K16" s="299"/>
-      <c r="L16" s="299"/>
-      <c r="M16" s="299"/>
+      <c r="C16" s="307"/>
+      <c r="D16" s="307"/>
+      <c r="E16" s="307"/>
+      <c r="F16" s="307"/>
+      <c r="G16" s="307"/>
+      <c r="H16" s="307"/>
+      <c r="I16" s="307"/>
+      <c r="J16" s="307"/>
+      <c r="K16" s="307"/>
+      <c r="L16" s="307"/>
+      <c r="M16" s="307"/>
     </row>
     <row r="17" spans="2:13" ht="18">
-      <c r="B17" s="302" t="s">
+      <c r="B17" s="306" t="s">
         <v>345</v>
       </c>
-      <c r="C17" s="302"/>
-      <c r="D17" s="302"/>
-      <c r="E17" s="302"/>
-      <c r="F17" s="302"/>
-      <c r="G17" s="302"/>
-      <c r="H17" s="302"/>
-      <c r="I17" s="302"/>
-      <c r="J17" s="302"/>
-      <c r="K17" s="302"/>
-      <c r="L17" s="302"/>
-      <c r="M17" s="302"/>
+      <c r="C17" s="306"/>
+      <c r="D17" s="306"/>
+      <c r="E17" s="306"/>
+      <c r="F17" s="306"/>
+      <c r="G17" s="306"/>
+      <c r="H17" s="306"/>
+      <c r="I17" s="306"/>
+      <c r="J17" s="306"/>
+      <c r="K17" s="306"/>
+      <c r="L17" s="306"/>
+      <c r="M17" s="306"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="299" t="s">
+      <c r="B18" s="307" t="s">
         <v>346</v>
       </c>
-      <c r="C18" s="299"/>
-      <c r="D18" s="299"/>
-      <c r="E18" s="299"/>
-      <c r="F18" s="299"/>
-      <c r="G18" s="299"/>
-      <c r="H18" s="299"/>
-      <c r="I18" s="299"/>
-      <c r="J18" s="299"/>
-      <c r="K18" s="299"/>
-      <c r="L18" s="299"/>
-      <c r="M18" s="299"/>
+      <c r="C18" s="307"/>
+      <c r="D18" s="307"/>
+      <c r="E18" s="307"/>
+      <c r="F18" s="307"/>
+      <c r="G18" s="307"/>
+      <c r="H18" s="307"/>
+      <c r="I18" s="307"/>
+      <c r="J18" s="307"/>
+      <c r="K18" s="307"/>
+      <c r="L18" s="307"/>
+      <c r="M18" s="307"/>
     </row>
     <row r="19" spans="2:13" ht="14.4" customHeight="1">
-      <c r="B19" s="356"/>
-      <c r="C19" s="355" t="s">
+      <c r="B19" s="297"/>
+      <c r="C19" s="311" t="s">
         <v>365</v>
       </c>
-      <c r="D19" s="355"/>
-      <c r="E19" s="355"/>
-      <c r="F19" s="355"/>
-      <c r="G19" s="355"/>
-      <c r="H19" s="355"/>
-      <c r="I19" s="355"/>
-      <c r="J19" s="355"/>
-      <c r="K19" s="355"/>
-      <c r="L19" s="355"/>
-      <c r="M19" s="355"/>
+      <c r="D19" s="311"/>
+      <c r="E19" s="311"/>
+      <c r="F19" s="311"/>
+      <c r="G19" s="311"/>
+      <c r="H19" s="311"/>
+      <c r="I19" s="311"/>
+      <c r="J19" s="311"/>
+      <c r="K19" s="311"/>
+      <c r="L19" s="311"/>
+      <c r="M19" s="311"/>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="356"/>
-      <c r="C20" s="355" t="s">
+      <c r="B20" s="297"/>
+      <c r="C20" s="311" t="s">
         <v>366</v>
       </c>
-      <c r="D20" s="355"/>
-      <c r="E20" s="355"/>
-      <c r="F20" s="355"/>
-      <c r="G20" s="355"/>
-      <c r="H20" s="355"/>
-      <c r="I20" s="355"/>
-      <c r="J20" s="355"/>
-      <c r="K20" s="355"/>
-      <c r="L20" s="355"/>
-      <c r="M20" s="355"/>
+      <c r="D20" s="311"/>
+      <c r="E20" s="311"/>
+      <c r="F20" s="311"/>
+      <c r="G20" s="311"/>
+      <c r="H20" s="311"/>
+      <c r="I20" s="311"/>
+      <c r="J20" s="311"/>
+      <c r="K20" s="311"/>
+      <c r="L20" s="311"/>
+      <c r="M20" s="311"/>
     </row>
     <row r="21" spans="2:13" ht="14.4" customHeight="1">
-      <c r="B21" s="356"/>
-      <c r="C21" s="355" t="s">
+      <c r="B21" s="297"/>
+      <c r="C21" s="311" t="s">
         <v>367</v>
       </c>
-      <c r="D21" s="355"/>
-      <c r="E21" s="355"/>
-      <c r="F21" s="355"/>
-      <c r="G21" s="355"/>
-      <c r="H21" s="355"/>
-      <c r="I21" s="355"/>
-      <c r="J21" s="355"/>
-      <c r="K21" s="355"/>
-      <c r="L21" s="355"/>
-      <c r="M21" s="355"/>
+      <c r="D21" s="311"/>
+      <c r="E21" s="311"/>
+      <c r="F21" s="311"/>
+      <c r="G21" s="311"/>
+      <c r="H21" s="311"/>
+      <c r="I21" s="311"/>
+      <c r="J21" s="311"/>
+      <c r="K21" s="311"/>
+      <c r="L21" s="311"/>
+      <c r="M21" s="311"/>
     </row>
     <row r="22" spans="2:13">
-      <c r="B22" s="356"/>
-      <c r="C22" s="355" t="s">
+      <c r="B22" s="297"/>
+      <c r="C22" s="311" t="s">
         <v>462</v>
       </c>
-      <c r="D22" s="355"/>
-      <c r="E22" s="355"/>
-      <c r="F22" s="355"/>
-      <c r="G22" s="355"/>
-      <c r="H22" s="355"/>
-      <c r="I22" s="355"/>
-      <c r="J22" s="355"/>
-      <c r="K22" s="355"/>
-      <c r="L22" s="355"/>
-      <c r="M22" s="355"/>
+      <c r="D22" s="311"/>
+      <c r="E22" s="311"/>
+      <c r="F22" s="311"/>
+      <c r="G22" s="311"/>
+      <c r="H22" s="311"/>
+      <c r="I22" s="311"/>
+      <c r="J22" s="311"/>
+      <c r="K22" s="311"/>
+      <c r="L22" s="311"/>
+      <c r="M22" s="311"/>
     </row>
     <row r="23" spans="2:13" ht="14.4" customHeight="1">
-      <c r="B23" s="356"/>
-      <c r="C23" s="356"/>
-      <c r="D23" s="355" t="s">
+      <c r="B23" s="297"/>
+      <c r="C23" s="297"/>
+      <c r="D23" s="311" t="s">
         <v>458</v>
       </c>
-      <c r="E23" s="355"/>
-      <c r="F23" s="355"/>
-      <c r="G23" s="355"/>
-      <c r="H23" s="355"/>
-      <c r="I23" s="355"/>
-      <c r="J23" s="355"/>
-      <c r="K23" s="355"/>
-      <c r="L23" s="355"/>
-      <c r="M23" s="355"/>
+      <c r="E23" s="311"/>
+      <c r="F23" s="311"/>
+      <c r="G23" s="311"/>
+      <c r="H23" s="311"/>
+      <c r="I23" s="311"/>
+      <c r="J23" s="311"/>
+      <c r="K23" s="311"/>
+      <c r="L23" s="311"/>
+      <c r="M23" s="311"/>
     </row>
     <row r="24" spans="2:13" ht="14.4" customHeight="1">
-      <c r="B24" s="356"/>
-      <c r="C24" s="356"/>
-      <c r="D24" s="355" t="s">
+      <c r="B24" s="297"/>
+      <c r="C24" s="297"/>
+      <c r="D24" s="311" t="s">
         <v>459</v>
       </c>
-      <c r="E24" s="355"/>
-      <c r="F24" s="355"/>
-      <c r="G24" s="355"/>
-      <c r="H24" s="355"/>
-      <c r="I24" s="355"/>
-      <c r="J24" s="355"/>
-      <c r="K24" s="355"/>
-      <c r="L24" s="355"/>
-      <c r="M24" s="355"/>
+      <c r="E24" s="311"/>
+      <c r="F24" s="311"/>
+      <c r="G24" s="311"/>
+      <c r="H24" s="311"/>
+      <c r="I24" s="311"/>
+      <c r="J24" s="311"/>
+      <c r="K24" s="311"/>
+      <c r="L24" s="311"/>
+      <c r="M24" s="311"/>
     </row>
     <row r="25" spans="2:13">
       <c r="B25" s="294"/>
       <c r="C25" s="295"/>
-      <c r="D25" s="299" t="s">
+      <c r="D25" s="307" t="s">
         <v>460</v>
       </c>
-      <c r="E25" s="299"/>
-      <c r="F25" s="299"/>
-      <c r="G25" s="299"/>
-      <c r="H25" s="299"/>
-      <c r="I25" s="299"/>
-      <c r="J25" s="299"/>
-      <c r="K25" s="299"/>
-      <c r="L25" s="299"/>
-      <c r="M25" s="299"/>
+      <c r="E25" s="307"/>
+      <c r="F25" s="307"/>
+      <c r="G25" s="307"/>
+      <c r="H25" s="307"/>
+      <c r="I25" s="307"/>
+      <c r="J25" s="307"/>
+      <c r="K25" s="307"/>
+      <c r="L25" s="307"/>
+      <c r="M25" s="307"/>
     </row>
     <row r="26" spans="2:13">
       <c r="B26" s="294"/>
       <c r="C26" s="295"/>
-      <c r="D26" s="355" t="s">
+      <c r="D26" s="311" t="s">
         <v>461</v>
       </c>
-      <c r="E26" s="355"/>
-      <c r="F26" s="355"/>
-      <c r="G26" s="355"/>
-      <c r="H26" s="355"/>
-      <c r="I26" s="355"/>
-      <c r="J26" s="355"/>
-      <c r="K26" s="355"/>
-      <c r="L26" s="355"/>
-      <c r="M26" s="355"/>
+      <c r="E26" s="311"/>
+      <c r="F26" s="311"/>
+      <c r="G26" s="311"/>
+      <c r="H26" s="311"/>
+      <c r="I26" s="311"/>
+      <c r="J26" s="311"/>
+      <c r="K26" s="311"/>
+      <c r="L26" s="311"/>
+      <c r="M26" s="311"/>
     </row>
     <row r="27" spans="2:13" ht="15" customHeight="1">
-      <c r="B27" s="297" t="s">
+      <c r="B27" s="308" t="s">
         <v>368</v>
       </c>
-      <c r="C27" s="298"/>
-      <c r="D27" s="298"/>
-      <c r="E27" s="298"/>
-      <c r="F27" s="298"/>
-      <c r="G27" s="298"/>
-      <c r="H27" s="298"/>
-      <c r="I27" s="298"/>
-      <c r="J27" s="298"/>
-      <c r="K27" s="298"/>
-      <c r="L27" s="298"/>
-      <c r="M27" s="298"/>
+      <c r="C27" s="305"/>
+      <c r="D27" s="305"/>
+      <c r="E27" s="305"/>
+      <c r="F27" s="305"/>
+      <c r="G27" s="305"/>
+      <c r="H27" s="305"/>
+      <c r="I27" s="305"/>
+      <c r="J27" s="305"/>
+      <c r="K27" s="305"/>
+      <c r="L27" s="305"/>
+      <c r="M27" s="305"/>
     </row>
     <row r="28" spans="2:13" ht="15" customHeight="1">
-      <c r="B28" s="297" t="s">
+      <c r="B28" s="308" t="s">
         <v>369</v>
       </c>
-      <c r="C28" s="298"/>
-      <c r="D28" s="298"/>
-      <c r="E28" s="298"/>
-      <c r="F28" s="298"/>
-      <c r="G28" s="298"/>
-      <c r="H28" s="298"/>
-      <c r="I28" s="298"/>
-      <c r="J28" s="298"/>
-      <c r="K28" s="298"/>
-      <c r="L28" s="298"/>
-      <c r="M28" s="298"/>
+      <c r="C28" s="305"/>
+      <c r="D28" s="305"/>
+      <c r="E28" s="305"/>
+      <c r="F28" s="305"/>
+      <c r="G28" s="305"/>
+      <c r="H28" s="305"/>
+      <c r="I28" s="305"/>
+      <c r="J28" s="305"/>
+      <c r="K28" s="305"/>
+      <c r="L28" s="305"/>
+      <c r="M28" s="305"/>
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="221"/>
     </row>
     <row r="30" spans="2:13" ht="18">
-      <c r="B30" s="302" t="s">
+      <c r="B30" s="306" t="s">
         <v>347</v>
       </c>
-      <c r="C30" s="302"/>
-      <c r="D30" s="302"/>
-      <c r="E30" s="302"/>
-      <c r="F30" s="302"/>
-      <c r="G30" s="302"/>
-      <c r="H30" s="302"/>
-      <c r="I30" s="302"/>
-      <c r="J30" s="302"/>
-      <c r="K30" s="302"/>
-      <c r="L30" s="302"/>
-      <c r="M30" s="302"/>
+      <c r="C30" s="306"/>
+      <c r="D30" s="306"/>
+      <c r="E30" s="306"/>
+      <c r="F30" s="306"/>
+      <c r="G30" s="306"/>
+      <c r="H30" s="306"/>
+      <c r="I30" s="306"/>
+      <c r="J30" s="306"/>
+      <c r="K30" s="306"/>
+      <c r="L30" s="306"/>
+      <c r="M30" s="306"/>
     </row>
     <row r="31" spans="2:13" ht="15" customHeight="1">
-      <c r="B31" s="299" t="s">
+      <c r="B31" s="307" t="s">
         <v>374</v>
       </c>
-      <c r="C31" s="299"/>
-      <c r="D31" s="299"/>
-      <c r="E31" s="299"/>
-      <c r="F31" s="299"/>
-      <c r="G31" s="299"/>
-      <c r="H31" s="299"/>
-      <c r="I31" s="299"/>
-      <c r="J31" s="299"/>
-      <c r="K31" s="299"/>
-      <c r="L31" s="299"/>
-      <c r="M31" s="299"/>
+      <c r="C31" s="307"/>
+      <c r="D31" s="307"/>
+      <c r="E31" s="307"/>
+      <c r="F31" s="307"/>
+      <c r="G31" s="307"/>
+      <c r="H31" s="307"/>
+      <c r="I31" s="307"/>
+      <c r="J31" s="307"/>
+      <c r="K31" s="307"/>
+      <c r="L31" s="307"/>
+      <c r="M31" s="307"/>
     </row>
     <row r="32" spans="2:13" ht="31.5" customHeight="1">
-      <c r="B32" s="299" t="s">
+      <c r="B32" s="307" t="s">
         <v>348</v>
       </c>
-      <c r="C32" s="299"/>
-      <c r="D32" s="299"/>
-      <c r="E32" s="299"/>
-      <c r="F32" s="299"/>
-      <c r="G32" s="299"/>
-      <c r="H32" s="299"/>
-      <c r="I32" s="299"/>
-      <c r="J32" s="299"/>
-      <c r="K32" s="299"/>
-      <c r="L32" s="299"/>
-      <c r="M32" s="299"/>
+      <c r="C32" s="307"/>
+      <c r="D32" s="307"/>
+      <c r="E32" s="307"/>
+      <c r="F32" s="307"/>
+      <c r="G32" s="307"/>
+      <c r="H32" s="307"/>
+      <c r="I32" s="307"/>
+      <c r="J32" s="307"/>
+      <c r="K32" s="307"/>
+      <c r="L32" s="307"/>
+      <c r="M32" s="307"/>
     </row>
     <row r="33" spans="2:13" ht="28.5" customHeight="1">
-      <c r="B33" s="299" t="s">
+      <c r="B33" s="307" t="s">
         <v>349</v>
       </c>
-      <c r="C33" s="299"/>
-      <c r="D33" s="299"/>
-      <c r="E33" s="299"/>
-      <c r="F33" s="299"/>
-      <c r="G33" s="299"/>
-      <c r="H33" s="299"/>
-      <c r="I33" s="299"/>
-      <c r="J33" s="299"/>
-      <c r="K33" s="299"/>
-      <c r="L33" s="299"/>
-      <c r="M33" s="299"/>
+      <c r="C33" s="307"/>
+      <c r="D33" s="307"/>
+      <c r="E33" s="307"/>
+      <c r="F33" s="307"/>
+      <c r="G33" s="307"/>
+      <c r="H33" s="307"/>
+      <c r="I33" s="307"/>
+      <c r="J33" s="307"/>
+      <c r="K33" s="307"/>
+      <c r="L33" s="307"/>
+      <c r="M33" s="307"/>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="299" t="s">
+      <c r="B34" s="307" t="s">
         <v>350</v>
       </c>
-      <c r="C34" s="299"/>
-      <c r="D34" s="299"/>
-      <c r="E34" s="299"/>
-      <c r="F34" s="299"/>
-      <c r="G34" s="299"/>
-      <c r="H34" s="299"/>
-      <c r="I34" s="299"/>
-      <c r="J34" s="299"/>
-      <c r="K34" s="299"/>
-      <c r="L34" s="299"/>
-      <c r="M34" s="299"/>
+      <c r="C34" s="307"/>
+      <c r="D34" s="307"/>
+      <c r="E34" s="307"/>
+      <c r="F34" s="307"/>
+      <c r="G34" s="307"/>
+      <c r="H34" s="307"/>
+      <c r="I34" s="307"/>
+      <c r="J34" s="307"/>
+      <c r="K34" s="307"/>
+      <c r="L34" s="307"/>
+      <c r="M34" s="307"/>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="299" t="s">
+      <c r="B35" s="307" t="s">
         <v>351</v>
       </c>
-      <c r="C35" s="299"/>
-      <c r="D35" s="299"/>
-      <c r="E35" s="299"/>
-      <c r="F35" s="299"/>
-      <c r="G35" s="299"/>
-      <c r="H35" s="299"/>
-      <c r="I35" s="299"/>
-      <c r="J35" s="299"/>
-      <c r="K35" s="299"/>
-      <c r="L35" s="299"/>
-      <c r="M35" s="299"/>
+      <c r="C35" s="307"/>
+      <c r="D35" s="307"/>
+      <c r="E35" s="307"/>
+      <c r="F35" s="307"/>
+      <c r="G35" s="307"/>
+      <c r="H35" s="307"/>
+      <c r="I35" s="307"/>
+      <c r="J35" s="307"/>
+      <c r="K35" s="307"/>
+      <c r="L35" s="307"/>
+      <c r="M35" s="307"/>
     </row>
     <row r="36" spans="2:13" ht="18">
-      <c r="B36" s="302" t="s">
+      <c r="B36" s="306" t="s">
         <v>352</v>
       </c>
-      <c r="C36" s="302"/>
-      <c r="D36" s="302"/>
-      <c r="E36" s="302"/>
-      <c r="F36" s="302"/>
-      <c r="G36" s="302"/>
-      <c r="H36" s="302"/>
-      <c r="I36" s="302"/>
-      <c r="J36" s="302"/>
-      <c r="K36" s="302"/>
-      <c r="L36" s="302"/>
-      <c r="M36" s="302"/>
+      <c r="C36" s="306"/>
+      <c r="D36" s="306"/>
+      <c r="E36" s="306"/>
+      <c r="F36" s="306"/>
+      <c r="G36" s="306"/>
+      <c r="H36" s="306"/>
+      <c r="I36" s="306"/>
+      <c r="J36" s="306"/>
+      <c r="K36" s="306"/>
+      <c r="L36" s="306"/>
+      <c r="M36" s="306"/>
     </row>
     <row r="37" spans="2:13" ht="30.75" customHeight="1">
-      <c r="B37" s="299" t="s">
+      <c r="B37" s="307" t="s">
         <v>353</v>
       </c>
-      <c r="C37" s="299"/>
-      <c r="D37" s="299"/>
-      <c r="E37" s="299"/>
-      <c r="F37" s="299"/>
-      <c r="G37" s="299"/>
-      <c r="H37" s="299"/>
-      <c r="I37" s="299"/>
-      <c r="J37" s="299"/>
-      <c r="K37" s="299"/>
-      <c r="L37" s="299"/>
-      <c r="M37" s="299"/>
+      <c r="C37" s="307"/>
+      <c r="D37" s="307"/>
+      <c r="E37" s="307"/>
+      <c r="F37" s="307"/>
+      <c r="G37" s="307"/>
+      <c r="H37" s="307"/>
+      <c r="I37" s="307"/>
+      <c r="J37" s="307"/>
+      <c r="K37" s="307"/>
+      <c r="L37" s="307"/>
+      <c r="M37" s="307"/>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="299" t="s">
+      <c r="B38" s="307" t="s">
         <v>354</v>
       </c>
-      <c r="C38" s="299"/>
-      <c r="D38" s="299"/>
-      <c r="E38" s="299"/>
-      <c r="F38" s="299"/>
-      <c r="G38" s="299"/>
-      <c r="H38" s="299"/>
-      <c r="I38" s="299"/>
-      <c r="J38" s="299"/>
-      <c r="K38" s="299"/>
-      <c r="L38" s="299"/>
-      <c r="M38" s="299"/>
+      <c r="C38" s="307"/>
+      <c r="D38" s="307"/>
+      <c r="E38" s="307"/>
+      <c r="F38" s="307"/>
+      <c r="G38" s="307"/>
+      <c r="H38" s="307"/>
+      <c r="I38" s="307"/>
+      <c r="J38" s="307"/>
+      <c r="K38" s="307"/>
+      <c r="L38" s="307"/>
+      <c r="M38" s="307"/>
     </row>
     <row r="39" spans="2:13">
       <c r="B39" s="221"/>
     </row>
     <row r="40" spans="2:13" ht="18">
-      <c r="B40" s="302" t="s">
+      <c r="B40" s="306" t="s">
         <v>355</v>
       </c>
-      <c r="C40" s="302"/>
-      <c r="D40" s="302"/>
-      <c r="E40" s="302"/>
-      <c r="F40" s="302"/>
-      <c r="G40" s="302"/>
-      <c r="H40" s="302"/>
-      <c r="I40" s="302"/>
-      <c r="J40" s="302"/>
-      <c r="K40" s="302"/>
-      <c r="L40" s="302"/>
-      <c r="M40" s="302"/>
+      <c r="C40" s="306"/>
+      <c r="D40" s="306"/>
+      <c r="E40" s="306"/>
+      <c r="F40" s="306"/>
+      <c r="G40" s="306"/>
+      <c r="H40" s="306"/>
+      <c r="I40" s="306"/>
+      <c r="J40" s="306"/>
+      <c r="K40" s="306"/>
+      <c r="L40" s="306"/>
+      <c r="M40" s="306"/>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="303" t="s">
+      <c r="B41" s="313" t="s">
         <v>356</v>
       </c>
-      <c r="C41" s="303"/>
-      <c r="D41" s="303"/>
-      <c r="E41" s="303"/>
-      <c r="F41" s="303"/>
-      <c r="G41" s="303"/>
-      <c r="H41" s="303"/>
-      <c r="I41" s="303"/>
-      <c r="J41" s="303"/>
-      <c r="K41" s="303"/>
-      <c r="L41" s="303"/>
-      <c r="M41" s="303"/>
+      <c r="C41" s="313"/>
+      <c r="D41" s="313"/>
+      <c r="E41" s="313"/>
+      <c r="F41" s="313"/>
+      <c r="G41" s="313"/>
+      <c r="H41" s="313"/>
+      <c r="I41" s="313"/>
+      <c r="J41" s="313"/>
+      <c r="K41" s="313"/>
+      <c r="L41" s="313"/>
+      <c r="M41" s="313"/>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="303" t="s">
+      <c r="B42" s="313" t="s">
         <v>357</v>
       </c>
-      <c r="C42" s="303"/>
-      <c r="D42" s="303"/>
-      <c r="E42" s="303"/>
-      <c r="F42" s="303"/>
-      <c r="G42" s="303"/>
-      <c r="H42" s="303"/>
-      <c r="I42" s="303"/>
-      <c r="J42" s="303"/>
-      <c r="K42" s="303"/>
-      <c r="L42" s="303"/>
-      <c r="M42" s="303"/>
+      <c r="C42" s="313"/>
+      <c r="D42" s="313"/>
+      <c r="E42" s="313"/>
+      <c r="F42" s="313"/>
+      <c r="G42" s="313"/>
+      <c r="H42" s="313"/>
+      <c r="I42" s="313"/>
+      <c r="J42" s="313"/>
+      <c r="K42" s="313"/>
+      <c r="L42" s="313"/>
+      <c r="M42" s="313"/>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="303" t="s">
+      <c r="B43" s="313" t="s">
         <v>358</v>
       </c>
-      <c r="C43" s="303"/>
-      <c r="D43" s="303"/>
-      <c r="E43" s="303"/>
-      <c r="F43" s="303"/>
-      <c r="G43" s="303"/>
-      <c r="H43" s="303"/>
-      <c r="I43" s="303"/>
-      <c r="J43" s="303"/>
-      <c r="K43" s="303"/>
-      <c r="L43" s="303"/>
-      <c r="M43" s="303"/>
+      <c r="C43" s="313"/>
+      <c r="D43" s="313"/>
+      <c r="E43" s="313"/>
+      <c r="F43" s="313"/>
+      <c r="G43" s="313"/>
+      <c r="H43" s="313"/>
+      <c r="I43" s="313"/>
+      <c r="J43" s="313"/>
+      <c r="K43" s="313"/>
+      <c r="L43" s="313"/>
+      <c r="M43" s="313"/>
     </row>
     <row r="44" spans="2:13">
       <c r="B44" s="282" t="s">
@@ -8614,52 +8650,52 @@
       <c r="M44" s="280"/>
     </row>
     <row r="45" spans="2:13" ht="18">
-      <c r="B45" s="302" t="s">
+      <c r="B45" s="306" t="s">
         <v>359</v>
       </c>
-      <c r="C45" s="302"/>
-      <c r="D45" s="302"/>
-      <c r="E45" s="302"/>
-      <c r="F45" s="302"/>
-      <c r="G45" s="302"/>
-      <c r="H45" s="302"/>
-      <c r="I45" s="302"/>
-      <c r="J45" s="302"/>
-      <c r="K45" s="302"/>
-      <c r="L45" s="302"/>
-      <c r="M45" s="302"/>
+      <c r="C45" s="306"/>
+      <c r="D45" s="306"/>
+      <c r="E45" s="306"/>
+      <c r="F45" s="306"/>
+      <c r="G45" s="306"/>
+      <c r="H45" s="306"/>
+      <c r="I45" s="306"/>
+      <c r="J45" s="306"/>
+      <c r="K45" s="306"/>
+      <c r="L45" s="306"/>
+      <c r="M45" s="306"/>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="299" t="s">
+      <c r="B46" s="307" t="s">
         <v>360</v>
       </c>
-      <c r="C46" s="299"/>
-      <c r="D46" s="299"/>
-      <c r="E46" s="299"/>
-      <c r="F46" s="299"/>
-      <c r="G46" s="299"/>
-      <c r="H46" s="299"/>
-      <c r="I46" s="299"/>
-      <c r="J46" s="299"/>
-      <c r="K46" s="299"/>
-      <c r="L46" s="299"/>
-      <c r="M46" s="299"/>
+      <c r="C46" s="307"/>
+      <c r="D46" s="307"/>
+      <c r="E46" s="307"/>
+      <c r="F46" s="307"/>
+      <c r="G46" s="307"/>
+      <c r="H46" s="307"/>
+      <c r="I46" s="307"/>
+      <c r="J46" s="307"/>
+      <c r="K46" s="307"/>
+      <c r="L46" s="307"/>
+      <c r="M46" s="307"/>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="304" t="s">
+      <c r="B47" s="312" t="s">
         <v>451</v>
       </c>
-      <c r="C47" s="304"/>
-      <c r="D47" s="304"/>
-      <c r="E47" s="304"/>
-      <c r="F47" s="304"/>
-      <c r="G47" s="304"/>
-      <c r="H47" s="304"/>
-      <c r="I47" s="304"/>
-      <c r="J47" s="304"/>
-      <c r="K47" s="304"/>
-      <c r="L47" s="304"/>
-      <c r="M47" s="304"/>
+      <c r="C47" s="312"/>
+      <c r="D47" s="312"/>
+      <c r="E47" s="312"/>
+      <c r="F47" s="312"/>
+      <c r="G47" s="312"/>
+      <c r="H47" s="312"/>
+      <c r="I47" s="312"/>
+      <c r="J47" s="312"/>
+      <c r="K47" s="312"/>
+      <c r="L47" s="312"/>
+      <c r="M47" s="312"/>
     </row>
   </sheetData>
   <mergeCells count="43">
@@ -8685,16 +8721,17 @@
     <mergeCell ref="B27:M27"/>
     <mergeCell ref="B28:M28"/>
     <mergeCell ref="B30:M30"/>
+    <mergeCell ref="C21:M21"/>
+    <mergeCell ref="C22:M22"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B14:M14"/>
     <mergeCell ref="B16:M16"/>
     <mergeCell ref="B17:M17"/>
     <mergeCell ref="B18:M18"/>
     <mergeCell ref="C19:M19"/>
     <mergeCell ref="C20:M20"/>
-    <mergeCell ref="C21:M21"/>
-    <mergeCell ref="C22:M22"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="B10:L10"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="B4:M4"/>
@@ -8705,7 +8742,6 @@
     <mergeCell ref="B11:M11"/>
     <mergeCell ref="B12:M12"/>
     <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B14:M14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B41" r:id="rId1" display="https://cdn.who.int/media/docs/default-source/documents/about-us/thirteenth-general-programme/gpw13_methodology_nov9_online-version1b3170f8-98ea-4fcc-aa3a-059ede7e51ad.pdf?sfvrsn=12dfeb0d_1&amp;download=true" xr:uid="{5B1AD3AB-AC30-4E70-9D4E-7E9B49DF39DD}"/>
@@ -9397,121 +9433,121 @@
       <c r="Z8" s="13"/>
     </row>
     <row r="9" spans="1:32" ht="15" customHeight="1">
-      <c r="A9" s="350" t="s">
+      <c r="A9" s="359" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="350"/>
-      <c r="C9" s="348" t="s">
+      <c r="B9" s="359"/>
+      <c r="C9" s="357" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="348"/>
-      <c r="E9" s="348"/>
-      <c r="F9" s="348"/>
-      <c r="G9" s="348"/>
-      <c r="H9" s="348"/>
-      <c r="I9" s="348"/>
+      <c r="D9" s="357"/>
+      <c r="E9" s="357"/>
+      <c r="F9" s="357"/>
+      <c r="G9" s="357"/>
+      <c r="H9" s="357"/>
+      <c r="I9" s="357"/>
       <c r="J9" s="30"/>
-      <c r="K9" s="349" t="s">
+      <c r="K9" s="358" t="s">
         <v>78</v>
       </c>
-      <c r="L9" s="349"/>
-      <c r="M9" s="349"/>
-      <c r="N9" s="349"/>
-      <c r="O9" s="349"/>
-      <c r="P9" s="349"/>
-      <c r="Q9" s="349"/>
-      <c r="R9" s="349"/>
-      <c r="S9" s="349"/>
-      <c r="T9" s="349"/>
-      <c r="U9" s="349"/>
+      <c r="L9" s="358"/>
+      <c r="M9" s="358"/>
+      <c r="N9" s="358"/>
+      <c r="O9" s="358"/>
+      <c r="P9" s="358"/>
+      <c r="Q9" s="358"/>
+      <c r="R9" s="358"/>
+      <c r="S9" s="358"/>
+      <c r="T9" s="358"/>
+      <c r="U9" s="358"/>
       <c r="V9" s="30"/>
-      <c r="W9" s="345" t="s">
+      <c r="W9" s="354" t="s">
         <v>79</v>
       </c>
-      <c r="X9" s="346"/>
-      <c r="Y9" s="346"/>
-      <c r="Z9" s="347"/>
+      <c r="X9" s="355"/>
+      <c r="Y9" s="355"/>
+      <c r="Z9" s="356"/>
     </row>
     <row r="10" spans="1:32">
-      <c r="A10" s="334" t="s">
+      <c r="A10" s="343" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="334" t="s">
+      <c r="B10" s="343" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="334" t="s">
+      <c r="C10" s="343" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="334" t="s">
+      <c r="D10" s="343" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="334" t="s">
+      <c r="E10" s="343" t="s">
         <v>120</v>
       </c>
-      <c r="F10" s="334" t="s">
+      <c r="F10" s="343" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="334" t="s">
+      <c r="G10" s="343" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="336" t="s">
+      <c r="H10" s="345" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="336" t="s">
+      <c r="I10" s="345" t="s">
         <v>114</v>
       </c>
       <c r="J10" s="31"/>
-      <c r="K10" s="338" t="s">
+      <c r="K10" s="347" t="s">
         <v>81</v>
       </c>
-      <c r="L10" s="338" t="s">
+      <c r="L10" s="347" t="s">
         <v>82</v>
       </c>
       <c r="M10" s="87"/>
-      <c r="N10" s="338" t="s">
+      <c r="N10" s="347" t="s">
         <v>83</v>
       </c>
-      <c r="O10" s="338" t="s">
+      <c r="O10" s="347" t="s">
         <v>82</v>
       </c>
       <c r="P10" s="87"/>
-      <c r="Q10" s="338" t="s">
+      <c r="Q10" s="347" t="s">
         <v>84</v>
       </c>
-      <c r="R10" s="338" t="s">
+      <c r="R10" s="347" t="s">
         <v>82</v>
       </c>
       <c r="S10" s="87"/>
-      <c r="T10" s="338" t="s">
+      <c r="T10" s="347" t="s">
         <v>85</v>
       </c>
-      <c r="U10" s="338" t="s">
+      <c r="U10" s="347" t="s">
         <v>82</v>
       </c>
       <c r="V10" s="31"/>
-      <c r="W10" s="335" t="s">
+      <c r="W10" s="344" t="s">
         <v>118</v>
       </c>
-      <c r="X10" s="334" t="s">
+      <c r="X10" s="343" t="s">
         <v>115</v>
       </c>
-      <c r="Y10" s="334" t="s">
+      <c r="Y10" s="343" t="s">
         <v>116</v>
       </c>
-      <c r="Z10" s="334" t="s">
+      <c r="Z10" s="343" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="15" customHeight="1">
-      <c r="A11" s="334"/>
-      <c r="B11" s="334"/>
-      <c r="C11" s="337"/>
-      <c r="D11" s="337"/>
-      <c r="E11" s="337"/>
-      <c r="F11" s="337"/>
-      <c r="G11" s="337"/>
-      <c r="H11" s="337"/>
-      <c r="I11" s="337"/>
+      <c r="A11" s="343"/>
+      <c r="B11" s="343"/>
+      <c r="C11" s="346"/>
+      <c r="D11" s="346"/>
+      <c r="E11" s="346"/>
+      <c r="F11" s="346"/>
+      <c r="G11" s="346"/>
+      <c r="H11" s="346"/>
+      <c r="I11" s="346"/>
       <c r="J11" s="31"/>
       <c r="K11" s="27">
         <v>2018</v>
@@ -9541,10 +9577,10 @@
         <v>2023</v>
       </c>
       <c r="V11" s="31"/>
-      <c r="W11" s="335"/>
-      <c r="X11" s="334"/>
-      <c r="Y11" s="334"/>
-      <c r="Z11" s="334"/>
+      <c r="W11" s="344"/>
+      <c r="X11" s="343"/>
+      <c r="Y11" s="343"/>
+      <c r="Z11" s="343"/>
     </row>
     <row r="12" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
       <c r="A12" s="195" t="s">
@@ -10727,14 +10763,14 @@
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
       <c r="U30" s="13"/>
-      <c r="W30" s="339" t="s">
+      <c r="W30" s="348" t="s">
         <v>104</v>
       </c>
-      <c r="X30" s="340"/>
-      <c r="Y30" s="341" t="s">
+      <c r="X30" s="349"/>
+      <c r="Y30" s="350" t="s">
         <v>105</v>
       </c>
-      <c r="Z30" s="342"/>
+      <c r="Z30" s="351"/>
     </row>
     <row r="31" spans="1:32" ht="15" customHeight="1">
       <c r="A31" s="51" t="s">
@@ -10761,10 +10797,10 @@
       <c r="T31" s="13"/>
       <c r="U31" s="13"/>
       <c r="V31" s="26"/>
-      <c r="W31" s="343" t="s">
+      <c r="W31" s="352" t="s">
         <v>107</v>
       </c>
-      <c r="X31" s="344"/>
+      <c r="X31" s="353"/>
       <c r="Y31" s="40" t="s">
         <v>126</v>
       </c>
@@ -10797,10 +10833,10 @@
       <c r="T32" s="13"/>
       <c r="U32" s="13"/>
       <c r="V32" s="26"/>
-      <c r="W32" s="331" t="s">
+      <c r="W32" s="340" t="s">
         <v>109</v>
       </c>
-      <c r="X32" s="331"/>
+      <c r="X32" s="340"/>
       <c r="Y32" s="266">
         <v>1660448.0263009099</v>
       </c>
@@ -10834,10 +10870,10 @@
       <c r="T33" s="13"/>
       <c r="U33" s="13"/>
       <c r="V33" s="26"/>
-      <c r="W33" s="331" t="s">
+      <c r="W33" s="340" t="s">
         <v>111</v>
       </c>
-      <c r="X33" s="331"/>
+      <c r="X33" s="340"/>
       <c r="Y33" s="266">
         <v>-691434.53619569901</v>
       </c>
@@ -10869,10 +10905,10 @@
       <c r="S34" s="13"/>
       <c r="T34" s="13"/>
       <c r="U34" s="13"/>
-      <c r="W34" s="332" t="s">
+      <c r="W34" s="341" t="s">
         <v>446</v>
       </c>
-      <c r="X34" s="333"/>
+      <c r="X34" s="342"/>
       <c r="Y34" s="267">
         <f>Y32+Y33</f>
         <v>969013.49010521092</v>
@@ -10904,10 +10940,10 @@
       <c r="S35" s="13"/>
       <c r="T35" s="13"/>
       <c r="U35" s="13"/>
-      <c r="W35" s="331" t="s">
+      <c r="W35" s="340" t="s">
         <v>112</v>
       </c>
-      <c r="X35" s="331"/>
+      <c r="X35" s="340"/>
       <c r="Y35" s="266">
         <v>3.6784375539831999</v>
       </c>
@@ -11455,35 +11491,35 @@
     </row>
     <row r="4" spans="1:39" ht="15" customHeight="1">
       <c r="A4" s="13"/>
-      <c r="B4" s="352" t="s">
+      <c r="B4" s="361" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="351" t="s">
+      <c r="C4" s="360" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="351"/>
-      <c r="E4" s="351"/>
-      <c r="F4" s="351"/>
-      <c r="G4" s="351"/>
-      <c r="H4" s="351"/>
-      <c r="I4" s="351"/>
-      <c r="J4" s="351"/>
-      <c r="K4" s="351"/>
-      <c r="L4" s="351"/>
-      <c r="M4" s="351"/>
-      <c r="N4" s="351"/>
-      <c r="O4" s="351"/>
-      <c r="P4" s="351"/>
-      <c r="Q4" s="351"/>
-      <c r="R4" s="351"/>
-      <c r="S4" s="351"/>
-      <c r="T4" s="351"/>
-      <c r="U4" s="351"/>
-      <c r="V4" s="351"/>
-      <c r="W4" s="351"/>
-      <c r="X4" s="351"/>
-      <c r="Y4" s="351"/>
-      <c r="Z4" s="351"/>
+      <c r="D4" s="360"/>
+      <c r="E4" s="360"/>
+      <c r="F4" s="360"/>
+      <c r="G4" s="360"/>
+      <c r="H4" s="360"/>
+      <c r="I4" s="360"/>
+      <c r="J4" s="360"/>
+      <c r="K4" s="360"/>
+      <c r="L4" s="360"/>
+      <c r="M4" s="360"/>
+      <c r="N4" s="360"/>
+      <c r="O4" s="360"/>
+      <c r="P4" s="360"/>
+      <c r="Q4" s="360"/>
+      <c r="R4" s="360"/>
+      <c r="S4" s="360"/>
+      <c r="T4" s="360"/>
+      <c r="U4" s="360"/>
+      <c r="V4" s="360"/>
+      <c r="W4" s="360"/>
+      <c r="X4" s="360"/>
+      <c r="Y4" s="360"/>
+      <c r="Z4" s="360"/>
       <c r="AA4" s="13"/>
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
@@ -11500,7 +11536,7 @@
     </row>
     <row r="5" spans="1:39">
       <c r="A5" s="13"/>
-      <c r="B5" s="353"/>
+      <c r="B5" s="362"/>
       <c r="C5" s="273" t="s">
         <v>127</v>
       </c>
@@ -12639,28 +12675,28 @@
       <c r="Z22" s="274"/>
     </row>
     <row r="23" spans="2:26">
-      <c r="B23" s="354"/>
-      <c r="C23" s="354"/>
-      <c r="D23" s="354"/>
-      <c r="E23" s="354"/>
-      <c r="F23" s="354"/>
-      <c r="G23" s="354"/>
-      <c r="H23" s="354"/>
-      <c r="I23" s="354"/>
-      <c r="J23" s="354"/>
-      <c r="K23" s="354"/>
-      <c r="L23" s="354"/>
-      <c r="M23" s="354"/>
-      <c r="N23" s="354"/>
-      <c r="O23" s="354"/>
-      <c r="P23" s="354"/>
-      <c r="Q23" s="354"/>
-      <c r="R23" s="354"/>
-      <c r="S23" s="354"/>
-      <c r="T23" s="354"/>
-      <c r="U23" s="354"/>
-      <c r="V23" s="354"/>
-      <c r="W23" s="354"/>
+      <c r="B23" s="363"/>
+      <c r="C23" s="363"/>
+      <c r="D23" s="363"/>
+      <c r="E23" s="363"/>
+      <c r="F23" s="363"/>
+      <c r="G23" s="363"/>
+      <c r="H23" s="363"/>
+      <c r="I23" s="363"/>
+      <c r="J23" s="363"/>
+      <c r="K23" s="363"/>
+      <c r="L23" s="363"/>
+      <c r="M23" s="363"/>
+      <c r="N23" s="363"/>
+      <c r="O23" s="363"/>
+      <c r="P23" s="363"/>
+      <c r="Q23" s="363"/>
+      <c r="R23" s="363"/>
+      <c r="S23" s="363"/>
+      <c r="T23" s="363"/>
+      <c r="U23" s="363"/>
+      <c r="V23" s="363"/>
+      <c r="W23" s="363"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -14662,7 +14698,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B30" sqref="B30"/>
+      <selection pane="topRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -14970,29 +15006,29 @@
     <row r="9" spans="1:31" ht="18">
       <c r="A9" s="84"/>
       <c r="B9" s="84"/>
-      <c r="C9" s="310" t="s">
+      <c r="C9" s="319" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="310"/>
-      <c r="E9" s="310"/>
-      <c r="F9" s="310"/>
-      <c r="G9" s="310"/>
+      <c r="D9" s="319"/>
+      <c r="E9" s="319"/>
+      <c r="F9" s="319"/>
+      <c r="G9" s="319"/>
       <c r="H9" s="29"/>
-      <c r="I9" s="310" t="s">
+      <c r="I9" s="319" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="310"/>
-      <c r="K9" s="310"/>
-      <c r="L9" s="310"/>
-      <c r="M9" s="310"/>
-      <c r="N9" s="310"/>
-      <c r="O9" s="310"/>
-      <c r="P9" s="310"/>
-      <c r="Q9" s="310"/>
-      <c r="R9" s="310"/>
-      <c r="S9" s="310"/>
-      <c r="T9" s="310"/>
-      <c r="U9" s="310"/>
+      <c r="J9" s="319"/>
+      <c r="K9" s="319"/>
+      <c r="L9" s="319"/>
+      <c r="M9" s="319"/>
+      <c r="N9" s="319"/>
+      <c r="O9" s="319"/>
+      <c r="P9" s="319"/>
+      <c r="Q9" s="319"/>
+      <c r="R9" s="319"/>
+      <c r="S9" s="319"/>
+      <c r="T9" s="319"/>
+      <c r="U9" s="319"/>
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
       <c r="X9" s="13"/>
@@ -15007,45 +15043,45 @@
     <row r="10" spans="1:31" ht="14.55" customHeight="1">
       <c r="A10" s="85"/>
       <c r="B10" s="85"/>
-      <c r="C10" s="311" t="s">
+      <c r="C10" s="320" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="311" t="s">
+      <c r="D10" s="320" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="305" t="s">
+      <c r="E10" s="314" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="305" t="s">
+      <c r="F10" s="314" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="305" t="s">
+      <c r="G10" s="314" t="s">
         <v>85</v>
       </c>
       <c r="H10" s="60"/>
-      <c r="I10" s="305" t="s">
+      <c r="I10" s="314" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="305"/>
+      <c r="J10" s="314"/>
       <c r="K10" s="296"/>
-      <c r="L10" s="305" t="s">
+      <c r="L10" s="314" t="s">
         <v>228</v>
       </c>
-      <c r="M10" s="305"/>
+      <c r="M10" s="314"/>
       <c r="N10" s="296"/>
-      <c r="O10" s="314" t="s">
+      <c r="O10" s="323" t="s">
         <v>457</v>
       </c>
       <c r="P10" s="296"/>
-      <c r="Q10" s="305" t="s">
+      <c r="Q10" s="314" t="s">
         <v>84</v>
       </c>
-      <c r="R10" s="305"/>
+      <c r="R10" s="314"/>
       <c r="S10" s="296"/>
-      <c r="T10" s="305" t="s">
+      <c r="T10" s="314" t="s">
         <v>85</v>
       </c>
-      <c r="U10" s="305"/>
+      <c r="U10" s="314"/>
       <c r="V10" s="51"/>
       <c r="W10" s="51"/>
       <c r="X10" s="51"/>
@@ -15064,11 +15100,11 @@
       <c r="B11" s="85" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="312"/>
-      <c r="D11" s="312"/>
-      <c r="E11" s="313"/>
-      <c r="F11" s="313"/>
-      <c r="G11" s="313"/>
+      <c r="C11" s="321"/>
+      <c r="D11" s="321"/>
+      <c r="E11" s="322"/>
+      <c r="F11" s="322"/>
+      <c r="G11" s="322"/>
       <c r="H11" s="30"/>
       <c r="I11" s="117">
         <v>2018</v>
@@ -15084,7 +15120,7 @@
         <v>2023</v>
       </c>
       <c r="N11" s="118"/>
-      <c r="O11" s="315"/>
+      <c r="O11" s="324"/>
       <c r="P11" s="118"/>
       <c r="Q11" s="117">
         <v>2018</v>
@@ -15528,46 +15564,46 @@
       <c r="B20" s="88" t="s">
         <v>412</v>
       </c>
-      <c r="C20" s="120">
+      <c r="C20" s="298">
         <v>64.595253999999997</v>
       </c>
-      <c r="D20" s="120"/>
-      <c r="E20" s="90">
+      <c r="D20" s="298"/>
+      <c r="E20" s="299">
         <v>2018</v>
       </c>
-      <c r="F20" s="90" t="s">
+      <c r="F20" s="299" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="99" t="s">
+      <c r="G20" s="300" t="s">
         <v>179</v>
       </c>
-      <c r="H20" s="41"/>
-      <c r="I20" s="120">
+      <c r="H20" s="301"/>
+      <c r="I20" s="298">
         <v>64.595253999999997</v>
       </c>
-      <c r="J20" s="120">
+      <c r="J20" s="298">
         <v>72.525628659999995</v>
       </c>
-      <c r="K20" s="120"/>
-      <c r="L20" s="121"/>
-      <c r="M20" s="121"/>
-      <c r="N20" s="89"/>
-      <c r="O20" s="291">
+      <c r="K20" s="298"/>
+      <c r="L20" s="302"/>
+      <c r="M20" s="302"/>
+      <c r="N20" s="303"/>
+      <c r="O20" s="304">
         <f t="shared" ref="O20:O22" si="1">IF(OR(ISBLANK(I20),ISBLANK(J20)),"",J20-I20)</f>
         <v>7.9303746599999982</v>
       </c>
-      <c r="P20" s="89"/>
-      <c r="Q20" s="90" t="s">
+      <c r="P20" s="303"/>
+      <c r="Q20" s="299" t="s">
         <v>90</v>
       </c>
-      <c r="R20" s="90" t="s">
+      <c r="R20" s="299" t="s">
         <v>91</v>
       </c>
-      <c r="S20" s="89"/>
-      <c r="T20" s="99" t="s">
+      <c r="S20" s="303"/>
+      <c r="T20" s="300" t="s">
         <v>179</v>
       </c>
-      <c r="U20" s="99" t="s">
+      <c r="U20" s="300" t="s">
         <v>165</v>
       </c>
       <c r="V20" s="51"/>
@@ -16110,7 +16146,7 @@
       <c r="AE30" s="13"/>
     </row>
     <row r="31" spans="1:31" ht="25.5" customHeight="1">
-      <c r="A31" s="307" t="s">
+      <c r="A31" s="316" t="s">
         <v>199</v>
       </c>
       <c r="B31" s="91" t="s">
@@ -16171,7 +16207,7 @@
       <c r="AE31" s="13"/>
     </row>
     <row r="32" spans="1:31" ht="25.5" customHeight="1">
-      <c r="A32" s="308"/>
+      <c r="A32" s="317"/>
       <c r="B32" s="91" t="s">
         <v>201</v>
       </c>
@@ -16229,7 +16265,7 @@
       <c r="AE32" s="13"/>
     </row>
     <row r="33" spans="1:31" ht="25.5" customHeight="1">
-      <c r="A33" s="309"/>
+      <c r="A33" s="318"/>
       <c r="B33" s="91" t="s">
         <v>204</v>
       </c>
@@ -16884,29 +16920,29 @@
       <c r="AE48" s="13"/>
     </row>
     <row r="49" spans="1:31" ht="15" customHeight="1">
-      <c r="A49" s="306" t="s">
+      <c r="A49" s="315" t="s">
         <v>263</v>
       </c>
-      <c r="B49" s="306"/>
-      <c r="C49" s="306"/>
-      <c r="D49" s="306"/>
-      <c r="E49" s="306"/>
-      <c r="F49" s="306"/>
-      <c r="G49" s="306"/>
-      <c r="H49" s="306"/>
-      <c r="I49" s="306"/>
-      <c r="J49" s="306"/>
-      <c r="K49" s="306"/>
-      <c r="L49" s="306"/>
-      <c r="M49" s="306"/>
-      <c r="N49" s="306"/>
-      <c r="O49" s="306"/>
-      <c r="P49" s="306"/>
-      <c r="Q49" s="306"/>
-      <c r="R49" s="306"/>
-      <c r="S49" s="306"/>
-      <c r="T49" s="306"/>
-      <c r="U49" s="306"/>
+      <c r="B49" s="315"/>
+      <c r="C49" s="315"/>
+      <c r="D49" s="315"/>
+      <c r="E49" s="315"/>
+      <c r="F49" s="315"/>
+      <c r="G49" s="315"/>
+      <c r="H49" s="315"/>
+      <c r="I49" s="315"/>
+      <c r="J49" s="315"/>
+      <c r="K49" s="315"/>
+      <c r="L49" s="315"/>
+      <c r="M49" s="315"/>
+      <c r="N49" s="315"/>
+      <c r="O49" s="315"/>
+      <c r="P49" s="315"/>
+      <c r="Q49" s="315"/>
+      <c r="R49" s="315"/>
+      <c r="S49" s="315"/>
+      <c r="T49" s="315"/>
+      <c r="U49" s="315"/>
       <c r="V49" s="75"/>
       <c r="W49" s="13"/>
       <c r="X49" s="13"/>
@@ -16919,27 +16955,27 @@
       <c r="AE49" s="13"/>
     </row>
     <row r="50" spans="1:31" ht="15" customHeight="1">
-      <c r="A50" s="306"/>
-      <c r="B50" s="306"/>
-      <c r="C50" s="306"/>
-      <c r="D50" s="306"/>
-      <c r="E50" s="306"/>
-      <c r="F50" s="306"/>
-      <c r="G50" s="306"/>
-      <c r="H50" s="306"/>
-      <c r="I50" s="306"/>
-      <c r="J50" s="306"/>
-      <c r="K50" s="306"/>
-      <c r="L50" s="306"/>
-      <c r="M50" s="306"/>
-      <c r="N50" s="306"/>
-      <c r="O50" s="306"/>
-      <c r="P50" s="306"/>
-      <c r="Q50" s="306"/>
-      <c r="R50" s="306"/>
-      <c r="S50" s="306"/>
-      <c r="T50" s="306"/>
-      <c r="U50" s="306"/>
+      <c r="A50" s="315"/>
+      <c r="B50" s="315"/>
+      <c r="C50" s="315"/>
+      <c r="D50" s="315"/>
+      <c r="E50" s="315"/>
+      <c r="F50" s="315"/>
+      <c r="G50" s="315"/>
+      <c r="H50" s="315"/>
+      <c r="I50" s="315"/>
+      <c r="J50" s="315"/>
+      <c r="K50" s="315"/>
+      <c r="L50" s="315"/>
+      <c r="M50" s="315"/>
+      <c r="N50" s="315"/>
+      <c r="O50" s="315"/>
+      <c r="P50" s="315"/>
+      <c r="Q50" s="315"/>
+      <c r="R50" s="315"/>
+      <c r="S50" s="315"/>
+      <c r="T50" s="315"/>
+      <c r="U50" s="315"/>
       <c r="V50" s="75"/>
       <c r="W50" s="13"/>
       <c r="X50" s="13"/>
@@ -16952,27 +16988,27 @@
       <c r="AE50" s="13"/>
     </row>
     <row r="51" spans="1:31" ht="15" customHeight="1">
-      <c r="A51" s="306"/>
-      <c r="B51" s="306"/>
-      <c r="C51" s="306"/>
-      <c r="D51" s="306"/>
-      <c r="E51" s="306"/>
-      <c r="F51" s="306"/>
-      <c r="G51" s="306"/>
-      <c r="H51" s="306"/>
-      <c r="I51" s="306"/>
-      <c r="J51" s="306"/>
-      <c r="K51" s="306"/>
-      <c r="L51" s="306"/>
-      <c r="M51" s="306"/>
-      <c r="N51" s="306"/>
-      <c r="O51" s="306"/>
-      <c r="P51" s="306"/>
-      <c r="Q51" s="306"/>
-      <c r="R51" s="306"/>
-      <c r="S51" s="306"/>
-      <c r="T51" s="306"/>
-      <c r="U51" s="306"/>
+      <c r="A51" s="315"/>
+      <c r="B51" s="315"/>
+      <c r="C51" s="315"/>
+      <c r="D51" s="315"/>
+      <c r="E51" s="315"/>
+      <c r="F51" s="315"/>
+      <c r="G51" s="315"/>
+      <c r="H51" s="315"/>
+      <c r="I51" s="315"/>
+      <c r="J51" s="315"/>
+      <c r="K51" s="315"/>
+      <c r="L51" s="315"/>
+      <c r="M51" s="315"/>
+      <c r="N51" s="315"/>
+      <c r="O51" s="315"/>
+      <c r="P51" s="315"/>
+      <c r="Q51" s="315"/>
+      <c r="R51" s="315"/>
+      <c r="S51" s="315"/>
+      <c r="T51" s="315"/>
+      <c r="U51" s="315"/>
       <c r="V51" s="75"/>
       <c r="W51" s="13"/>
       <c r="X51" s="13"/>
@@ -17748,35 +17784,35 @@
     </row>
     <row r="4" spans="1:39" ht="15" customHeight="1">
       <c r="A4" s="13"/>
-      <c r="B4" s="316" t="s">
+      <c r="B4" s="325" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="318" t="s">
+      <c r="C4" s="327" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="318"/>
-      <c r="E4" s="318"/>
-      <c r="F4" s="318"/>
-      <c r="G4" s="318"/>
-      <c r="H4" s="318"/>
-      <c r="I4" s="318"/>
-      <c r="J4" s="318"/>
-      <c r="K4" s="318"/>
-      <c r="L4" s="318"/>
-      <c r="M4" s="318"/>
-      <c r="N4" s="318"/>
-      <c r="O4" s="318"/>
-      <c r="P4" s="318"/>
-      <c r="Q4" s="318"/>
-      <c r="R4" s="318"/>
-      <c r="S4" s="318"/>
-      <c r="T4" s="318"/>
-      <c r="U4" s="318"/>
-      <c r="V4" s="318"/>
-      <c r="W4" s="318"/>
-      <c r="X4" s="318"/>
-      <c r="Y4" s="318"/>
-      <c r="Z4" s="318"/>
+      <c r="D4" s="327"/>
+      <c r="E4" s="327"/>
+      <c r="F4" s="327"/>
+      <c r="G4" s="327"/>
+      <c r="H4" s="327"/>
+      <c r="I4" s="327"/>
+      <c r="J4" s="327"/>
+      <c r="K4" s="327"/>
+      <c r="L4" s="327"/>
+      <c r="M4" s="327"/>
+      <c r="N4" s="327"/>
+      <c r="O4" s="327"/>
+      <c r="P4" s="327"/>
+      <c r="Q4" s="327"/>
+      <c r="R4" s="327"/>
+      <c r="S4" s="327"/>
+      <c r="T4" s="327"/>
+      <c r="U4" s="327"/>
+      <c r="V4" s="327"/>
+      <c r="W4" s="327"/>
+      <c r="X4" s="327"/>
+      <c r="Y4" s="327"/>
+      <c r="Z4" s="327"/>
       <c r="AA4" s="13"/>
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
@@ -17793,7 +17829,7 @@
     </row>
     <row r="5" spans="1:39">
       <c r="A5" s="13"/>
-      <c r="B5" s="317"/>
+      <c r="B5" s="326"/>
       <c r="C5" s="82" t="s">
         <v>127</v>
       </c>
@@ -19086,30 +19122,30 @@
       </c>
     </row>
     <row r="25" spans="2:26">
-      <c r="B25" s="319" t="s">
+      <c r="B25" s="328" t="s">
         <v>149</v>
       </c>
-      <c r="C25" s="319"/>
-      <c r="D25" s="319"/>
-      <c r="E25" s="319"/>
-      <c r="F25" s="319"/>
-      <c r="G25" s="319"/>
-      <c r="H25" s="319"/>
-      <c r="I25" s="319"/>
-      <c r="J25" s="319"/>
-      <c r="K25" s="319"/>
-      <c r="L25" s="319"/>
-      <c r="M25" s="319"/>
-      <c r="N25" s="319"/>
-      <c r="O25" s="319"/>
-      <c r="P25" s="319"/>
-      <c r="Q25" s="319"/>
-      <c r="R25" s="319"/>
-      <c r="S25" s="319"/>
-      <c r="T25" s="319"/>
-      <c r="U25" s="319"/>
-      <c r="V25" s="319"/>
-      <c r="W25" s="319"/>
+      <c r="C25" s="328"/>
+      <c r="D25" s="328"/>
+      <c r="E25" s="328"/>
+      <c r="F25" s="328"/>
+      <c r="G25" s="328"/>
+      <c r="H25" s="328"/>
+      <c r="I25" s="328"/>
+      <c r="J25" s="328"/>
+      <c r="K25" s="328"/>
+      <c r="L25" s="328"/>
+      <c r="M25" s="328"/>
+      <c r="N25" s="328"/>
+      <c r="O25" s="328"/>
+      <c r="P25" s="328"/>
+      <c r="Q25" s="328"/>
+      <c r="R25" s="328"/>
+      <c r="S25" s="328"/>
+      <c r="T25" s="328"/>
+      <c r="U25" s="328"/>
+      <c r="V25" s="328"/>
+      <c r="W25" s="328"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -20115,11 +20151,11 @@
         <f>F46/1000</f>
         <v>0</v>
       </c>
-      <c r="H5" s="320" t="s">
+      <c r="H5" s="329" t="s">
         <v>152</v>
       </c>
-      <c r="I5" s="320"/>
-      <c r="J5" s="320"/>
+      <c r="I5" s="329"/>
+      <c r="J5" s="329"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
@@ -20155,9 +20191,9 @@
         <f>F47</f>
         <v>0</v>
       </c>
-      <c r="H6" s="321"/>
-      <c r="I6" s="321"/>
-      <c r="J6" s="321"/>
+      <c r="H6" s="330"/>
+      <c r="I6" s="330"/>
+      <c r="J6" s="330"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -20214,31 +20250,31 @@
       <c r="AE7" s="13"/>
     </row>
     <row r="8" spans="1:31" ht="15" customHeight="1">
-      <c r="A8" s="323" t="s">
+      <c r="A8" s="332" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="323"/>
-      <c r="C8" s="325" t="s">
+      <c r="B8" s="332"/>
+      <c r="C8" s="334" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="325"/>
-      <c r="E8" s="325"/>
-      <c r="F8" s="325"/>
-      <c r="G8" s="325"/>
+      <c r="D8" s="334"/>
+      <c r="E8" s="334"/>
+      <c r="F8" s="334"/>
+      <c r="G8" s="334"/>
       <c r="H8" s="177"/>
-      <c r="I8" s="322" t="s">
+      <c r="I8" s="331" t="s">
         <v>153</v>
       </c>
-      <c r="J8" s="322"/>
-      <c r="K8" s="322"/>
-      <c r="L8" s="322"/>
-      <c r="M8" s="322"/>
-      <c r="N8" s="322"/>
-      <c r="O8" s="322"/>
-      <c r="P8" s="322"/>
-      <c r="Q8" s="322"/>
-      <c r="R8" s="322"/>
-      <c r="S8" s="322"/>
+      <c r="J8" s="331"/>
+      <c r="K8" s="331"/>
+      <c r="L8" s="331"/>
+      <c r="M8" s="331"/>
+      <c r="N8" s="331"/>
+      <c r="O8" s="331"/>
+      <c r="P8" s="331"/>
+      <c r="Q8" s="331"/>
+      <c r="R8" s="331"/>
+      <c r="S8" s="331"/>
       <c r="T8" s="136"/>
       <c r="U8" s="136"/>
       <c r="V8" s="136"/>
@@ -20253,47 +20289,47 @@
       <c r="AE8" s="13"/>
     </row>
     <row r="9" spans="1:31">
-      <c r="A9" s="324" t="s">
+      <c r="A9" s="333" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="324" t="s">
+      <c r="B9" s="333" t="s">
         <v>270</v>
       </c>
-      <c r="C9" s="327" t="s">
+      <c r="C9" s="336" t="s">
         <v>268</v>
       </c>
-      <c r="D9" s="324" t="s">
+      <c r="D9" s="333" t="s">
         <v>269</v>
       </c>
-      <c r="E9" s="327" t="s">
+      <c r="E9" s="336" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="327" t="s">
+      <c r="F9" s="336" t="s">
         <v>84</v>
       </c>
-      <c r="G9" s="324" t="s">
+      <c r="G9" s="333" t="s">
         <v>154</v>
       </c>
       <c r="H9" s="148"/>
-      <c r="I9" s="326" t="s">
+      <c r="I9" s="335" t="s">
         <v>268</v>
       </c>
-      <c r="J9" s="326"/>
+      <c r="J9" s="335"/>
       <c r="K9" s="153"/>
-      <c r="L9" s="326" t="s">
+      <c r="L9" s="335" t="s">
         <v>269</v>
       </c>
-      <c r="M9" s="326"/>
+      <c r="M9" s="335"/>
       <c r="N9" s="153"/>
-      <c r="O9" s="326" t="s">
+      <c r="O9" s="335" t="s">
         <v>84</v>
       </c>
-      <c r="P9" s="326"/>
+      <c r="P9" s="335"/>
       <c r="Q9" s="153"/>
-      <c r="R9" s="326" t="s">
+      <c r="R9" s="335" t="s">
         <v>85</v>
       </c>
-      <c r="S9" s="326"/>
+      <c r="S9" s="335"/>
       <c r="Y9" s="13"/>
       <c r="Z9" s="13"/>
       <c r="AA9" s="13"/>
@@ -20303,13 +20339,13 @@
       <c r="AE9" s="13"/>
     </row>
     <row r="10" spans="1:31">
-      <c r="A10" s="324"/>
-      <c r="B10" s="324"/>
-      <c r="C10" s="327"/>
-      <c r="D10" s="324"/>
-      <c r="E10" s="327"/>
-      <c r="F10" s="327"/>
-      <c r="G10" s="324"/>
+      <c r="A10" s="333"/>
+      <c r="B10" s="333"/>
+      <c r="C10" s="336"/>
+      <c r="D10" s="333"/>
+      <c r="E10" s="336"/>
+      <c r="F10" s="336"/>
+      <c r="G10" s="333"/>
       <c r="H10" s="148"/>
       <c r="I10" s="152">
         <v>2018</v>
@@ -22607,35 +22643,35 @@
     </row>
     <row r="4" spans="1:39" ht="15" customHeight="1">
       <c r="A4" s="13"/>
-      <c r="B4" s="328" t="s">
+      <c r="B4" s="337" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="330" t="s">
+      <c r="C4" s="339" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="330"/>
-      <c r="E4" s="330"/>
-      <c r="F4" s="330"/>
-      <c r="G4" s="330"/>
-      <c r="H4" s="330"/>
-      <c r="I4" s="330"/>
-      <c r="J4" s="330"/>
-      <c r="K4" s="330"/>
-      <c r="L4" s="330"/>
-      <c r="M4" s="330"/>
-      <c r="N4" s="330"/>
-      <c r="O4" s="330"/>
-      <c r="P4" s="330"/>
-      <c r="Q4" s="330"/>
-      <c r="R4" s="330"/>
-      <c r="S4" s="330"/>
-      <c r="T4" s="330"/>
-      <c r="U4" s="330"/>
-      <c r="V4" s="330"/>
-      <c r="W4" s="330"/>
-      <c r="X4" s="330"/>
-      <c r="Y4" s="330"/>
-      <c r="Z4" s="330"/>
+      <c r="D4" s="339"/>
+      <c r="E4" s="339"/>
+      <c r="F4" s="339"/>
+      <c r="G4" s="339"/>
+      <c r="H4" s="339"/>
+      <c r="I4" s="339"/>
+      <c r="J4" s="339"/>
+      <c r="K4" s="339"/>
+      <c r="L4" s="339"/>
+      <c r="M4" s="339"/>
+      <c r="N4" s="339"/>
+      <c r="O4" s="339"/>
+      <c r="P4" s="339"/>
+      <c r="Q4" s="339"/>
+      <c r="R4" s="339"/>
+      <c r="S4" s="339"/>
+      <c r="T4" s="339"/>
+      <c r="U4" s="339"/>
+      <c r="V4" s="339"/>
+      <c r="W4" s="339"/>
+      <c r="X4" s="339"/>
+      <c r="Y4" s="339"/>
+      <c r="Z4" s="339"/>
       <c r="AA4" s="13"/>
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
@@ -22652,7 +22688,7 @@
     </row>
     <row r="5" spans="1:39">
       <c r="A5" s="13"/>
-      <c r="B5" s="329"/>
+      <c r="B5" s="338"/>
       <c r="C5" s="193" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
Try to create a function to modify openxlsx styles rather than creating an infinte amount of them...
</commit_message>
<xml_diff>
--- a/inst/extdata/country_summary_template.xlsx
+++ b/inst/extdata/country_summary_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\documents\WHO\billionaiRe\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12217D3D-DA83-4586-A426-38F12A4DDFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD1B269-BEFC-46B5-A14C-AE8E25E9223C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="26136" windowHeight="16896" tabRatio="942" firstSheet="1" activeTab="4" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
   </bookViews>
@@ -3543,32 +3543,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3646,27 +3646,57 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="34" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="14" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="12" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3675,36 +3705,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3947,19 +3947,19 @@
                     <c:v>#N/A</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>2.7800000000000011</c:v>
+                    <c:v>#N/A</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>1</c:v>
+                    <c:v>#N/A</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>2.4000000000000057</c:v>
+                    <c:v>#N/A</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>#N/A</c:v>
+                    <c:v>1.460000000000008</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>1.9200000000000017</c:v>
+                    <c:v>20.919999999999987</c:v>
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>#N/A</c:v>
@@ -4057,19 +4057,19 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>69.42</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>#N/A</c:v>
+                  <c:v>130.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>100</c:v>
+                  <c:v>172.69</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>#N/A</c:v>
@@ -4156,13 +4156,13 @@
                     <c:v>#N/A</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>#N/A</c:v>
+                    <c:v>1.3900000000000006</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>#N/A</c:v>
+                    <c:v>8.9999999999999858E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>#N/A</c:v>
+                    <c:v>2.3999999999999986</c:v>
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>#N/A</c:v>
@@ -4207,13 +4207,13 @@
                     <c:v>#N/A</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>#N/A</c:v>
+                    <c:v>1.3900000000000006</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>#N/A</c:v>
+                    <c:v>8.9999999999999858E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>#N/A</c:v>
+                    <c:v>2.3999999999999986</c:v>
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>#N/A</c:v>
@@ -4317,13 +4317,13 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>#N/A</c:v>
+                  <c:v>15.29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.03</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>#N/A</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>#N/A</c:v>
@@ -4402,7 +4402,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{158BE1C8-FFCD-4C3C-A457-F765B7FE322A}" type="CELLRANGE">
+                    <a:fld id="{07B4C919-28D1-460D-A9F4-24711E10E795}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4463,7 +4463,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34D849F8-63F2-43D1-8B29-2CA2FD8335A0}" type="CELLRANGE">
+                    <a:fld id="{753C84D4-FF5C-4F9E-A79F-1A2D01F7EDB6}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4524,7 +4524,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE20E833-2A2A-4D9C-AD55-08CC15565EC1}" type="CELLRANGE">
+                    <a:fld id="{10C54F71-A10C-4BDA-96CA-5F5C7550DB9C}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4559,7 +4559,7 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:fld id="{8A09D54B-3435-44E0-871A-BC075AE8AE2B}" type="CELLRANGE">
-                      <a:rPr lang="en-CH"/>
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -4577,7 +4577,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4619,7 +4618,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{281C55F5-5A18-4476-8BE7-56CBFEA7A23C}" type="CELLRANGE">
+                    <a:fld id="{0BE6F7D4-3E9E-487D-91E1-52B281E77368}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4653,7 +4652,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6C2789F-2675-4A70-9801-A4DAFA832B0E}" type="CELLRANGE">
+                    <a:fld id="{53C51393-E944-40EA-A959-68B49F1E18C6}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4687,7 +4686,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E07C3396-83B6-4125-BFDB-D3832AB6D61A}" type="CELLRANGE">
+                    <a:fld id="{2A1744D4-266C-4B42-9B68-1BD1DA0D9BCF}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4721,7 +4720,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF82A87D-3B9D-4E0D-B827-C78B4164D851}" type="CELLRANGE">
+                    <a:fld id="{19110B6E-4EA3-4C5E-9983-9D61108B3D85}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4755,7 +4754,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F3CE9B3-376B-4549-AF64-1B3CF36E778A}" type="CELLRANGE">
+                    <a:fld id="{6C01541C-7589-4237-92CE-0FFAD27B4437}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4789,7 +4788,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5F9D3E8-5A95-4C79-8B58-04DABB08022A}" type="CELLRANGE">
+                    <a:fld id="{C4E1F381-B378-41BC-870E-9B099C954479}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4824,7 +4823,7 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:fld id="{75C064F7-CF27-44E7-8D2D-2BFCF9E60001}" type="CELLRANGE">
-                      <a:rPr lang="en-CH"/>
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -4842,7 +4841,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4984,19 +4982,19 @@
                   <c:v>99.89</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.900000000000006</c:v>
+                  <c:v>17.55</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>95</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>78.099999999999994</c:v>
+                  <c:v>21.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>129.04</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>98.08</c:v>
+                  <c:v>151.77000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>95</c:v>
@@ -6585,7 +6583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B24457E5-FE95-4445-B47B-167F6DC30DAD}" type="CELLRANGE">
+                    <a:fld id="{9F414A5B-A541-482C-A303-5E009BE4F064}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6646,7 +6644,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E806730-1B44-41B9-A029-CD21D2DF10F7}" type="CELLRANGE">
+                    <a:fld id="{5ECDDFBB-F9C0-414B-B4BE-353479261049}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6707,7 +6705,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AEA4F4E2-56C7-4CD6-8225-0FCD7C53CC7E}" type="CELLRANGE">
+                    <a:fld id="{861D3770-F641-4EE8-8059-06186A2A9AC7}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6741,7 +6739,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{862008BD-02E4-451D-ADF3-5A7DCD58CFA1}" type="CELLRANGE">
+                    <a:fld id="{37E4F1DD-67FF-429D-865C-BF1CB57BD797}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6802,7 +6800,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14745543-0347-4E38-8681-545BC6ABC5E5}" type="CELLRANGE">
+                    <a:fld id="{55B08A81-9735-4005-B225-F578711BA721}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6836,7 +6834,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E611814-469D-44FC-ABE1-285256F9C6AE}" type="CELLRANGE">
+                    <a:fld id="{2ABBC1A6-7CF6-4811-95D0-2C24DEFE549C}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6870,7 +6868,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{614B7365-1221-4B26-B12E-4F7C933253AB}" type="CELLRANGE">
+                    <a:fld id="{E0AE85C8-DC59-4374-AD4C-6E90E34CD0F8}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6904,7 +6902,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A3FD486-6772-47D6-A490-55E4B883C93C}" type="CELLRANGE">
+                    <a:fld id="{97893C1C-D81E-461A-8E85-1667DD9B70ED}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6938,7 +6936,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2419BE0F-D9A6-4F03-850A-41C082ABD3C1}" type="CELLRANGE">
+                    <a:fld id="{0A36EE0D-F33A-453D-A5B0-E70E80BE9A8E}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6972,7 +6970,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{809DD890-96D5-4E50-ADC0-6C4FE7EAFF4B}" type="CELLRANGE">
+                    <a:fld id="{D3BAABC5-2473-404C-96A0-A6AFEE56F3CB}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7006,7 +7004,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A152368-3E33-4639-B082-7FB528E87A59}" type="CELLRANGE">
+                    <a:fld id="{B1DAFADE-D64E-48DE-A112-94EE18CF9AB0}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7040,7 +7038,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BACC54FF-4353-4F42-B1E3-A724D0F84C2F}" type="CELLRANGE">
+                    <a:fld id="{17326658-1AFE-4E65-94FF-2889BA86BF18}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7074,7 +7072,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{054FBDC1-983D-4561-8DC5-B84E8E542EFB}" type="CELLRANGE">
+                    <a:fld id="{5D7F56EE-A172-4628-AB21-98CABB306845}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7673,30 +7671,102 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2">
+        <row r="1">
+          <cell r="B1"/>
+          <cell r="C1"/>
+          <cell r="D1"/>
+          <cell r="E1"/>
+          <cell r="I1"/>
+          <cell r="J1"/>
+          <cell r="L1"/>
+          <cell r="M1"/>
+        </row>
+        <row r="2">
+          <cell r="B2"/>
+          <cell r="C2"/>
+          <cell r="D2"/>
+          <cell r="E2"/>
+          <cell r="I2"/>
+          <cell r="J2"/>
+          <cell r="L2"/>
+          <cell r="M2"/>
+        </row>
+        <row r="3">
+          <cell r="B3"/>
+          <cell r="C3"/>
+          <cell r="D3"/>
+          <cell r="E3"/>
+          <cell r="I3"/>
+          <cell r="J3"/>
+          <cell r="L3"/>
+          <cell r="M3"/>
+        </row>
+        <row r="4">
+          <cell r="B4"/>
+          <cell r="C4"/>
+          <cell r="D4"/>
+          <cell r="E4"/>
+          <cell r="I4"/>
+          <cell r="J4"/>
+          <cell r="L4"/>
+          <cell r="M4"/>
+        </row>
         <row r="5">
-          <cell r="E5">
-            <v>1.4020036893157488</v>
-          </cell>
+          <cell r="B5"/>
+          <cell r="C5"/>
+          <cell r="D5"/>
+          <cell r="E5"/>
+          <cell r="I5"/>
+          <cell r="J5"/>
+          <cell r="L5"/>
+          <cell r="M5"/>
         </row>
         <row r="6">
-          <cell r="E6">
-            <v>112.08737916666536</v>
-          </cell>
+          <cell r="B6"/>
+          <cell r="C6"/>
+          <cell r="D6"/>
+          <cell r="E6"/>
+          <cell r="I6"/>
+          <cell r="J6"/>
+          <cell r="L6"/>
+          <cell r="M6"/>
         </row>
         <row r="7">
-          <cell r="E7">
-            <v>125.081316</v>
-          </cell>
+          <cell r="B7"/>
+          <cell r="C7"/>
+          <cell r="D7"/>
+          <cell r="E7"/>
+          <cell r="I7"/>
+          <cell r="J7"/>
+          <cell r="L7"/>
+          <cell r="M7"/>
+        </row>
+        <row r="8">
+          <cell r="B8"/>
+          <cell r="C8"/>
+          <cell r="D8"/>
+          <cell r="E8"/>
+          <cell r="I8"/>
+          <cell r="J8"/>
+          <cell r="L8"/>
+          <cell r="M8"/>
         </row>
         <row r="9">
+          <cell r="B9"/>
           <cell r="C9" t="str">
             <v>Latest Reported/Estimated Data Available</v>
           </cell>
+          <cell r="D9"/>
+          <cell r="E9"/>
           <cell r="I9" t="str">
             <v>2018 Baseline, and 2023 Projection</v>
           </cell>
+          <cell r="J9"/>
+          <cell r="L9"/>
+          <cell r="M9"/>
         </row>
         <row r="10">
+          <cell r="B10"/>
           <cell r="C10" t="str">
             <v>Raw Value</v>
           </cell>
@@ -7723,6 +7793,9 @@
           <cell r="B11" t="str">
             <v>Tracer Indicator</v>
           </cell>
+          <cell r="C11"/>
+          <cell r="D11"/>
+          <cell r="E11"/>
           <cell r="I11" t="str">
             <v>2018</v>
           </cell>
@@ -7735,6 +7808,16 @@
           <cell r="M11" t="str">
             <v>2023</v>
           </cell>
+        </row>
+        <row r="12">
+          <cell r="B12"/>
+          <cell r="C12"/>
+          <cell r="D12"/>
+          <cell r="E12"/>
+          <cell r="I12"/>
+          <cell r="J12"/>
+          <cell r="L12"/>
+          <cell r="M12"/>
         </row>
         <row r="13">
           <cell r="B13" t="str">
@@ -7755,20 +7838,26 @@
           <cell r="J13">
             <v>60.55</v>
           </cell>
+          <cell r="L13"/>
+          <cell r="M13"/>
         </row>
         <row r="14">
           <cell r="B14" t="str">
             <v>Antenatal care coverage (+4 visits) 2</v>
           </cell>
+          <cell r="C14"/>
           <cell r="D14" t="str">
             <v/>
           </cell>
+          <cell r="E14"/>
           <cell r="I14">
             <v>98.58</v>
           </cell>
           <cell r="J14">
             <v>98.46</v>
           </cell>
+          <cell r="L14"/>
+          <cell r="M14"/>
         </row>
         <row r="15">
           <cell r="B15" t="str">
@@ -7789,31 +7878,48 @@
           <cell r="J15">
             <v>98.54</v>
           </cell>
+          <cell r="L15"/>
+          <cell r="M15"/>
         </row>
         <row r="16">
           <cell r="B16" t="str">
             <v>Care seeking for suspected pneumonia</v>
           </cell>
+          <cell r="C16"/>
           <cell r="D16" t="str">
             <v/>
           </cell>
+          <cell r="E16"/>
           <cell r="I16">
             <v>89.91</v>
           </cell>
           <cell r="J16">
             <v>90.82</v>
           </cell>
+          <cell r="L16"/>
+          <cell r="M16"/>
         </row>
         <row r="17">
           <cell r="B17" t="str">
             <v>Average RMNCH</v>
           </cell>
-          <cell r="L17">
-            <v>85.710000000000008</v>
-          </cell>
-          <cell r="M17">
-            <v>87.092500000000001</v>
-          </cell>
+          <cell r="C17"/>
+          <cell r="D17"/>
+          <cell r="E17"/>
+          <cell r="I17"/>
+          <cell r="J17"/>
+          <cell r="L17"/>
+          <cell r="M17"/>
+        </row>
+        <row r="18">
+          <cell r="B18"/>
+          <cell r="C18"/>
+          <cell r="D18"/>
+          <cell r="E18"/>
+          <cell r="I18"/>
+          <cell r="J18"/>
+          <cell r="L18"/>
+          <cell r="M18"/>
         </row>
         <row r="19">
           <cell r="B19" t="str">
@@ -7834,6 +7940,8 @@
           <cell r="J19">
             <v>86.96</v>
           </cell>
+          <cell r="L19"/>
+          <cell r="M19"/>
         </row>
         <row r="20">
           <cell r="B20" t="str">
@@ -7854,14 +7962,22 @@
           <cell r="J20">
             <v>90.99</v>
           </cell>
+          <cell r="L20"/>
+          <cell r="M20"/>
         </row>
         <row r="21">
           <cell r="B21" t="str">
             <v>ITN use 4</v>
           </cell>
+          <cell r="C21"/>
           <cell r="D21" t="str">
             <v/>
           </cell>
+          <cell r="E21"/>
+          <cell r="I21"/>
+          <cell r="J21"/>
+          <cell r="L21"/>
+          <cell r="M21"/>
         </row>
         <row r="22">
           <cell r="B22" t="str">
@@ -7882,17 +7998,30 @@
           <cell r="J22">
             <v>99.9</v>
           </cell>
+          <cell r="L22"/>
+          <cell r="M22"/>
         </row>
         <row r="23">
           <cell r="B23" t="str">
             <v>Average Infectious diseases</v>
           </cell>
-          <cell r="L23">
-            <v>89.956666666666663</v>
-          </cell>
-          <cell r="M23">
-            <v>92.616666666666674</v>
-          </cell>
+          <cell r="C23"/>
+          <cell r="D23"/>
+          <cell r="E23"/>
+          <cell r="I23"/>
+          <cell r="J23"/>
+          <cell r="L23"/>
+          <cell r="M23"/>
+        </row>
+        <row r="24">
+          <cell r="B24"/>
+          <cell r="C24"/>
+          <cell r="D24"/>
+          <cell r="E24"/>
+          <cell r="I24"/>
+          <cell r="J24"/>
+          <cell r="L24"/>
+          <cell r="M24"/>
         </row>
         <row r="25">
           <cell r="B25" t="str">
@@ -7901,9 +8030,7 @@
           <cell r="C25">
             <v>17.55</v>
           </cell>
-          <cell r="D25">
-            <v>64.900000000000006</v>
-          </cell>
+          <cell r="D25"/>
           <cell r="E25">
             <v>2015</v>
           </cell>
@@ -7913,12 +8040,8 @@
           <cell r="J25">
             <v>15.29</v>
           </cell>
-          <cell r="L25">
-            <v>66.64</v>
-          </cell>
-          <cell r="M25">
-            <v>69.42</v>
-          </cell>
+          <cell r="L25"/>
+          <cell r="M25"/>
         </row>
         <row r="26">
           <cell r="B26" t="str">
@@ -7927,9 +8050,7 @@
           <cell r="C26">
             <v>5.2</v>
           </cell>
-          <cell r="D26">
-            <v>95</v>
-          </cell>
+          <cell r="D26"/>
           <cell r="E26">
             <v>2014</v>
           </cell>
@@ -7939,12 +8060,8 @@
           <cell r="J26">
             <v>5.03</v>
           </cell>
-          <cell r="L26">
-            <v>99</v>
-          </cell>
-          <cell r="M26">
-            <v>100</v>
-          </cell>
+          <cell r="L26"/>
+          <cell r="M26"/>
         </row>
         <row r="27">
           <cell r="B27" t="str">
@@ -7953,9 +8070,7 @@
           <cell r="C27">
             <v>21.9</v>
           </cell>
-          <cell r="D27">
-            <v>78.099999999999994</v>
-          </cell>
+          <cell r="D27"/>
           <cell r="E27">
             <v>2018</v>
           </cell>
@@ -7965,23 +8080,30 @@
           <cell r="J27">
             <v>19.5</v>
           </cell>
-          <cell r="L27">
-            <v>78.099999999999994</v>
-          </cell>
-          <cell r="M27">
-            <v>80.5</v>
-          </cell>
+          <cell r="L27"/>
+          <cell r="M27"/>
         </row>
         <row r="28">
           <cell r="B28" t="str">
             <v>Average NCDs</v>
           </cell>
-          <cell r="L28">
-            <v>81.246666666666655</v>
-          </cell>
-          <cell r="M28">
-            <v>81.246666666666655</v>
-          </cell>
+          <cell r="C28"/>
+          <cell r="D28"/>
+          <cell r="E28"/>
+          <cell r="I28"/>
+          <cell r="J28"/>
+          <cell r="L28"/>
+          <cell r="M28"/>
+        </row>
+        <row r="29">
+          <cell r="B29"/>
+          <cell r="C29"/>
+          <cell r="D29"/>
+          <cell r="E29"/>
+          <cell r="I29"/>
+          <cell r="J29"/>
+          <cell r="L29"/>
+          <cell r="M29"/>
         </row>
         <row r="30">
           <cell r="B30" t="str">
@@ -7990,9 +8112,7 @@
           <cell r="C30">
             <v>129.04</v>
           </cell>
-          <cell r="D30">
-            <v>100</v>
-          </cell>
+          <cell r="D30"/>
           <cell r="E30">
             <v>2018</v>
           </cell>
@@ -8002,12 +8122,8 @@
           <cell r="J30">
             <v>130.5</v>
           </cell>
-          <cell r="L30">
-            <v>100</v>
-          </cell>
-          <cell r="M30">
-            <v>100</v>
-          </cell>
+          <cell r="L30"/>
+          <cell r="M30"/>
         </row>
         <row r="31">
           <cell r="B31" t="str">
@@ -8016,9 +8132,7 @@
           <cell r="C31">
             <v>151.77000000000001</v>
           </cell>
-          <cell r="D31">
-            <v>98.08</v>
-          </cell>
+          <cell r="D31"/>
           <cell r="E31">
             <v>2018</v>
           </cell>
@@ -8028,12 +8142,8 @@
           <cell r="J31">
             <v>172.69</v>
           </cell>
-          <cell r="L31">
-            <v>98.08</v>
-          </cell>
-          <cell r="M31">
-            <v>100</v>
-          </cell>
+          <cell r="L31"/>
+          <cell r="M31"/>
         </row>
         <row r="32">
           <cell r="B32" t="str">
@@ -8042,6 +8152,7 @@
           <cell r="C32">
             <v>24.8</v>
           </cell>
+          <cell r="D32"/>
           <cell r="E32">
             <v>2018</v>
           </cell>
@@ -8051,6 +8162,8 @@
           <cell r="J32">
             <v>27.38</v>
           </cell>
+          <cell r="L32"/>
+          <cell r="M32"/>
         </row>
         <row r="33">
           <cell r="B33" t="str">
@@ -8059,6 +8172,7 @@
           <cell r="C33">
             <v>126.98</v>
           </cell>
+          <cell r="D33"/>
           <cell r="E33">
             <v>2018</v>
           </cell>
@@ -8068,6 +8182,8 @@
           <cell r="J33">
             <v>145.31</v>
           </cell>
+          <cell r="L33"/>
+          <cell r="M33"/>
         </row>
         <row r="34">
           <cell r="B34" t="str">
@@ -8076,6 +8192,7 @@
           <cell r="C34">
             <v>95</v>
           </cell>
+          <cell r="D34"/>
           <cell r="E34">
             <v>2020</v>
           </cell>
@@ -8085,25 +8202,30 @@
           <cell r="J34">
             <v>94.99</v>
           </cell>
+          <cell r="L34"/>
+          <cell r="M34"/>
         </row>
         <row r="35">
           <cell r="B35" t="str">
             <v>Average Service capacity and access</v>
           </cell>
-          <cell r="L35">
-            <v>99.039999999999992</v>
-          </cell>
-          <cell r="M35">
-            <v>99.039999999999992</v>
-          </cell>
+          <cell r="C35"/>
+          <cell r="D35"/>
+          <cell r="E35"/>
+          <cell r="I35"/>
+          <cell r="J35"/>
+          <cell r="L35"/>
+          <cell r="M35"/>
         </row>
         <row r="36">
-          <cell r="L36">
-            <v>88.988333333333344</v>
-          </cell>
-          <cell r="M36">
-            <v>89.99895833333332</v>
-          </cell>
+          <cell r="B36"/>
+          <cell r="C36"/>
+          <cell r="D36"/>
+          <cell r="E36"/>
+          <cell r="I36"/>
+          <cell r="J36"/>
+          <cell r="L36"/>
+          <cell r="M36"/>
         </row>
         <row r="37">
           <cell r="B37" t="str">
@@ -8124,55 +8246,342 @@
           <cell r="J37">
             <v>4.0599999999999996</v>
           </cell>
-          <cell r="L37">
-            <v>95.77</v>
-          </cell>
-          <cell r="M37">
-            <v>95.94</v>
-          </cell>
+          <cell r="L37"/>
+          <cell r="M37"/>
         </row>
         <row r="38">
           <cell r="B38" t="str">
             <v>UHC single measure</v>
           </cell>
+          <cell r="C38"/>
+          <cell r="D38"/>
+          <cell r="E38"/>
+          <cell r="I38"/>
+          <cell r="J38"/>
           <cell r="L38">
-            <v>85.224126833333344</v>
+            <v>61.09664039777099</v>
           </cell>
           <cell r="M38">
-            <v>86.345000624999997</v>
+            <v>63.310803650646406</v>
           </cell>
         </row>
         <row r="39">
           <cell r="B39" t="str">
             <v>Change in UHC single measure over 2018-2023</v>
           </cell>
-          <cell r="M39">
-            <v>1.1208737916666536</v>
-          </cell>
+          <cell r="C39"/>
+          <cell r="D39"/>
+          <cell r="E39"/>
+          <cell r="I39"/>
+          <cell r="J39"/>
+          <cell r="L39"/>
+          <cell r="M39"/>
         </row>
         <row r="40">
           <cell r="B40" t="str">
             <v>UN Population 2023 (thousand)</v>
           </cell>
-          <cell r="M40">
-            <v>125081.31600000001</v>
-          </cell>
+          <cell r="C40"/>
+          <cell r="D40"/>
+          <cell r="E40"/>
+          <cell r="I40"/>
+          <cell r="J40"/>
+          <cell r="L40"/>
+          <cell r="M40"/>
         </row>
         <row r="41">
           <cell r="B41" t="str">
             <v>Country contribution to UHC billion target (population - thousand)</v>
           </cell>
-          <cell r="M41">
-            <v>1402.0036893157487</v>
-          </cell>
+          <cell r="C41"/>
+          <cell r="D41"/>
+          <cell r="E41"/>
+          <cell r="I41"/>
+          <cell r="J41"/>
+          <cell r="L41"/>
+          <cell r="M41"/>
         </row>
         <row r="42">
           <cell r="B42" t="str">
             <v>% of country population newly covered by universal healthcare</v>
           </cell>
-          <cell r="M42">
-            <v>1.1208737916666536</v>
-          </cell>
+          <cell r="C42"/>
+          <cell r="D42"/>
+          <cell r="E42"/>
+          <cell r="I42"/>
+          <cell r="J42"/>
+          <cell r="L42"/>
+          <cell r="M42"/>
+        </row>
+        <row r="43">
+          <cell r="B43"/>
+          <cell r="C43"/>
+          <cell r="D43"/>
+          <cell r="E43"/>
+          <cell r="I43"/>
+          <cell r="J43"/>
+          <cell r="L43"/>
+          <cell r="M43"/>
+        </row>
+        <row r="44">
+          <cell r="B44"/>
+          <cell r="C44"/>
+          <cell r="D44"/>
+          <cell r="E44"/>
+          <cell r="I44"/>
+          <cell r="J44"/>
+          <cell r="L44"/>
+          <cell r="M44"/>
+        </row>
+        <row r="45">
+          <cell r="B45"/>
+          <cell r="C45"/>
+          <cell r="D45"/>
+          <cell r="E45"/>
+          <cell r="I45"/>
+          <cell r="J45"/>
+          <cell r="L45"/>
+          <cell r="M45"/>
+        </row>
+        <row r="46">
+          <cell r="B46"/>
+          <cell r="C46"/>
+          <cell r="D46"/>
+          <cell r="E46"/>
+          <cell r="I46"/>
+          <cell r="J46"/>
+          <cell r="L46"/>
+          <cell r="M46"/>
+        </row>
+        <row r="47">
+          <cell r="B47"/>
+          <cell r="C47"/>
+          <cell r="D47"/>
+          <cell r="E47"/>
+          <cell r="I47"/>
+          <cell r="J47"/>
+          <cell r="L47"/>
+          <cell r="M47"/>
+        </row>
+        <row r="48">
+          <cell r="B48"/>
+          <cell r="C48"/>
+          <cell r="D48"/>
+          <cell r="E48"/>
+          <cell r="I48"/>
+          <cell r="J48"/>
+          <cell r="L48"/>
+          <cell r="M48"/>
+        </row>
+        <row r="49">
+          <cell r="B49"/>
+          <cell r="C49"/>
+          <cell r="D49"/>
+          <cell r="E49"/>
+          <cell r="I49"/>
+          <cell r="J49"/>
+          <cell r="L49"/>
+          <cell r="M49"/>
+        </row>
+        <row r="50">
+          <cell r="B50"/>
+          <cell r="C50"/>
+          <cell r="D50"/>
+          <cell r="E50"/>
+          <cell r="I50"/>
+          <cell r="J50"/>
+          <cell r="L50"/>
+          <cell r="M50"/>
+        </row>
+        <row r="51">
+          <cell r="B51"/>
+          <cell r="C51"/>
+          <cell r="D51"/>
+          <cell r="E51"/>
+          <cell r="I51"/>
+          <cell r="J51"/>
+          <cell r="L51"/>
+          <cell r="M51"/>
+        </row>
+        <row r="52">
+          <cell r="B52"/>
+          <cell r="C52"/>
+          <cell r="D52"/>
+          <cell r="E52"/>
+          <cell r="I52"/>
+          <cell r="J52"/>
+          <cell r="L52"/>
+          <cell r="M52"/>
+        </row>
+        <row r="53">
+          <cell r="B53"/>
+          <cell r="C53"/>
+          <cell r="D53"/>
+          <cell r="E53"/>
+          <cell r="I53"/>
+          <cell r="J53"/>
+          <cell r="L53"/>
+          <cell r="M53"/>
+        </row>
+        <row r="54">
+          <cell r="B54"/>
+          <cell r="C54"/>
+          <cell r="D54"/>
+          <cell r="E54"/>
+          <cell r="I54"/>
+          <cell r="J54"/>
+          <cell r="L54"/>
+          <cell r="M54"/>
+        </row>
+        <row r="55">
+          <cell r="B55"/>
+          <cell r="C55"/>
+          <cell r="D55"/>
+          <cell r="E55"/>
+          <cell r="I55"/>
+          <cell r="J55"/>
+          <cell r="L55"/>
+          <cell r="M55"/>
+        </row>
+        <row r="56">
+          <cell r="B56"/>
+          <cell r="C56"/>
+          <cell r="D56"/>
+          <cell r="E56"/>
+          <cell r="I56"/>
+          <cell r="J56"/>
+          <cell r="L56"/>
+          <cell r="M56"/>
+        </row>
+        <row r="57">
+          <cell r="B57"/>
+          <cell r="C57"/>
+          <cell r="D57"/>
+          <cell r="E57"/>
+          <cell r="I57"/>
+          <cell r="J57"/>
+          <cell r="L57"/>
+          <cell r="M57"/>
+        </row>
+        <row r="58">
+          <cell r="B58"/>
+          <cell r="C58"/>
+          <cell r="D58"/>
+          <cell r="E58"/>
+          <cell r="I58"/>
+          <cell r="J58"/>
+          <cell r="L58"/>
+          <cell r="M58"/>
+        </row>
+        <row r="59">
+          <cell r="B59"/>
+          <cell r="C59"/>
+          <cell r="D59"/>
+          <cell r="E59"/>
+          <cell r="I59"/>
+          <cell r="J59"/>
+          <cell r="L59"/>
+          <cell r="M59"/>
+        </row>
+        <row r="60">
+          <cell r="B60"/>
+          <cell r="C60"/>
+          <cell r="D60"/>
+          <cell r="E60"/>
+          <cell r="I60"/>
+          <cell r="J60"/>
+          <cell r="L60"/>
+          <cell r="M60"/>
+        </row>
+        <row r="61">
+          <cell r="B61"/>
+          <cell r="C61"/>
+          <cell r="D61"/>
+          <cell r="E61"/>
+          <cell r="I61"/>
+          <cell r="J61"/>
+          <cell r="L61"/>
+          <cell r="M61"/>
+        </row>
+        <row r="62">
+          <cell r="B62"/>
+          <cell r="C62"/>
+          <cell r="D62"/>
+          <cell r="E62"/>
+          <cell r="I62"/>
+          <cell r="J62"/>
+          <cell r="L62"/>
+          <cell r="M62"/>
+        </row>
+        <row r="63">
+          <cell r="B63"/>
+          <cell r="C63"/>
+          <cell r="D63"/>
+          <cell r="E63"/>
+          <cell r="I63"/>
+          <cell r="J63"/>
+          <cell r="L63"/>
+          <cell r="M63"/>
+        </row>
+        <row r="64">
+          <cell r="B64"/>
+          <cell r="C64"/>
+          <cell r="D64"/>
+          <cell r="E64"/>
+          <cell r="I64"/>
+          <cell r="J64"/>
+          <cell r="L64"/>
+          <cell r="M64"/>
+        </row>
+        <row r="65">
+          <cell r="B65"/>
+          <cell r="C65"/>
+          <cell r="D65"/>
+          <cell r="E65"/>
+          <cell r="I65"/>
+          <cell r="J65"/>
+          <cell r="L65"/>
+          <cell r="M65"/>
+        </row>
+        <row r="66">
+          <cell r="B66"/>
+          <cell r="C66"/>
+          <cell r="D66"/>
+          <cell r="E66"/>
+          <cell r="I66"/>
+          <cell r="J66"/>
+          <cell r="L66"/>
+          <cell r="M66"/>
+        </row>
+        <row r="67">
+          <cell r="B67"/>
+          <cell r="C67"/>
+          <cell r="D67"/>
+          <cell r="E67"/>
+          <cell r="I67"/>
+          <cell r="J67"/>
+          <cell r="L67"/>
+          <cell r="M67"/>
+        </row>
+        <row r="68">
+          <cell r="B68"/>
+          <cell r="C68"/>
+          <cell r="D68"/>
+          <cell r="E68"/>
+          <cell r="I68"/>
+          <cell r="J68"/>
+          <cell r="L68"/>
+          <cell r="M68"/>
+        </row>
+        <row r="69">
+          <cell r="B69"/>
+          <cell r="C69"/>
+          <cell r="D69"/>
+          <cell r="E69"/>
+          <cell r="I69"/>
+          <cell r="J69"/>
+          <cell r="L69"/>
+          <cell r="M69"/>
         </row>
       </sheetData>
       <sheetData sheetId="3"/>
@@ -8242,6 +8651,9 @@
           <cell r="A15" t="str">
             <v>IHR core capacity index*</v>
           </cell>
+        </row>
+        <row r="16">
+          <cell r="A16"/>
         </row>
       </sheetData>
     </sheetDataSet>
@@ -8565,664 +8977,664 @@
   <sheetData>
     <row r="1" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315" t="s">
+      <c r="B2" s="318" t="s">
         <v>339</v>
       </c>
-      <c r="C2" s="315"/>
-      <c r="D2" s="315"/>
-      <c r="E2" s="315"/>
-      <c r="F2" s="315"/>
-      <c r="G2" s="315"/>
-      <c r="H2" s="315"/>
-      <c r="I2" s="315"/>
-      <c r="J2" s="315"/>
-      <c r="K2" s="315"/>
-      <c r="L2" s="315"/>
-      <c r="M2" s="315"/>
+      <c r="C2" s="318"/>
+      <c r="D2" s="318"/>
+      <c r="E2" s="318"/>
+      <c r="F2" s="318"/>
+      <c r="G2" s="318"/>
+      <c r="H2" s="318"/>
+      <c r="I2" s="318"/>
+      <c r="J2" s="318"/>
+      <c r="K2" s="318"/>
+      <c r="L2" s="318"/>
+      <c r="M2" s="318"/>
       <c r="N2" s="68"/>
       <c r="O2" s="68"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="316" t="s">
+      <c r="B3" s="319" t="s">
         <v>437</v>
       </c>
-      <c r="C3" s="316"/>
-      <c r="D3" s="316"/>
-      <c r="E3" s="316"/>
-      <c r="F3" s="316"/>
-      <c r="G3" s="316"/>
-      <c r="H3" s="316"/>
-      <c r="I3" s="316"/>
-      <c r="J3" s="316"/>
-      <c r="K3" s="316"/>
-      <c r="L3" s="316"/>
-      <c r="M3" s="316"/>
+      <c r="C3" s="319"/>
+      <c r="D3" s="319"/>
+      <c r="E3" s="319"/>
+      <c r="F3" s="319"/>
+      <c r="G3" s="319"/>
+      <c r="H3" s="319"/>
+      <c r="I3" s="319"/>
+      <c r="J3" s="319"/>
+      <c r="K3" s="319"/>
+      <c r="L3" s="319"/>
+      <c r="M3" s="319"/>
       <c r="N3" s="210"/>
       <c r="O3" s="210"/>
     </row>
     <row r="4" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="312" t="s">
+      <c r="B4" s="315" t="s">
         <v>340</v>
       </c>
-      <c r="C4" s="312"/>
-      <c r="D4" s="312"/>
-      <c r="E4" s="312"/>
-      <c r="F4" s="312"/>
-      <c r="G4" s="312"/>
-      <c r="H4" s="312"/>
-      <c r="I4" s="312"/>
-      <c r="J4" s="312"/>
-      <c r="K4" s="312"/>
-      <c r="L4" s="312"/>
-      <c r="M4" s="312"/>
+      <c r="C4" s="315"/>
+      <c r="D4" s="315"/>
+      <c r="E4" s="315"/>
+      <c r="F4" s="315"/>
+      <c r="G4" s="315"/>
+      <c r="H4" s="315"/>
+      <c r="I4" s="315"/>
+      <c r="J4" s="315"/>
+      <c r="K4" s="315"/>
+      <c r="L4" s="315"/>
+      <c r="M4" s="315"/>
       <c r="N4" s="211"/>
       <c r="O4" s="211"/>
     </row>
     <row r="5" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="313" t="s">
+      <c r="B5" s="312" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="313"/>
-      <c r="D5" s="313"/>
-      <c r="E5" s="313"/>
-      <c r="F5" s="313"/>
-      <c r="G5" s="313"/>
-      <c r="H5" s="313"/>
-      <c r="I5" s="313"/>
-      <c r="J5" s="313"/>
-      <c r="K5" s="313"/>
-      <c r="L5" s="313"/>
-      <c r="M5" s="313"/>
+      <c r="C5" s="312"/>
+      <c r="D5" s="312"/>
+      <c r="E5" s="312"/>
+      <c r="F5" s="312"/>
+      <c r="G5" s="312"/>
+      <c r="H5" s="312"/>
+      <c r="I5" s="312"/>
+      <c r="J5" s="312"/>
+      <c r="K5" s="312"/>
+      <c r="L5" s="312"/>
+      <c r="M5" s="312"/>
       <c r="N5" s="210"/>
       <c r="O5" s="210"/>
     </row>
     <row r="6" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="311" t="s">
+      <c r="B6" s="317" t="s">
         <v>361</v>
       </c>
-      <c r="C6" s="311"/>
-      <c r="D6" s="311"/>
-      <c r="E6" s="311"/>
-      <c r="F6" s="311"/>
-      <c r="G6" s="311"/>
-      <c r="H6" s="311"/>
-      <c r="I6" s="311"/>
-      <c r="J6" s="311"/>
-      <c r="K6" s="311"/>
-      <c r="L6" s="311"/>
-      <c r="M6" s="311"/>
+      <c r="C6" s="317"/>
+      <c r="D6" s="317"/>
+      <c r="E6" s="317"/>
+      <c r="F6" s="317"/>
+      <c r="G6" s="317"/>
+      <c r="H6" s="317"/>
+      <c r="I6" s="317"/>
+      <c r="J6" s="317"/>
+      <c r="K6" s="317"/>
+      <c r="L6" s="317"/>
+      <c r="M6" s="317"/>
       <c r="N6" s="212"/>
       <c r="O6" s="212"/>
     </row>
     <row r="7" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="311" t="s">
+      <c r="B7" s="317" t="s">
         <v>362</v>
       </c>
-      <c r="C7" s="311"/>
-      <c r="D7" s="311"/>
-      <c r="E7" s="311"/>
-      <c r="F7" s="311"/>
-      <c r="G7" s="311"/>
-      <c r="H7" s="311"/>
-      <c r="I7" s="311"/>
-      <c r="J7" s="311"/>
-      <c r="K7" s="311"/>
-      <c r="L7" s="311"/>
-      <c r="M7" s="311"/>
+      <c r="C7" s="317"/>
+      <c r="D7" s="317"/>
+      <c r="E7" s="317"/>
+      <c r="F7" s="317"/>
+      <c r="G7" s="317"/>
+      <c r="H7" s="317"/>
+      <c r="I7" s="317"/>
+      <c r="J7" s="317"/>
+      <c r="K7" s="317"/>
+      <c r="L7" s="317"/>
+      <c r="M7" s="317"/>
       <c r="N7" s="212"/>
       <c r="O7" s="212"/>
     </row>
     <row r="8" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="311" t="s">
+      <c r="B8" s="317" t="s">
         <v>363</v>
       </c>
-      <c r="C8" s="311"/>
-      <c r="D8" s="311"/>
-      <c r="E8" s="311"/>
-      <c r="F8" s="311"/>
-      <c r="G8" s="311"/>
-      <c r="H8" s="311"/>
-      <c r="I8" s="311"/>
-      <c r="J8" s="311"/>
-      <c r="K8" s="311"/>
-      <c r="L8" s="311"/>
-      <c r="M8" s="311"/>
+      <c r="C8" s="317"/>
+      <c r="D8" s="317"/>
+      <c r="E8" s="317"/>
+      <c r="F8" s="317"/>
+      <c r="G8" s="317"/>
+      <c r="H8" s="317"/>
+      <c r="I8" s="317"/>
+      <c r="J8" s="317"/>
+      <c r="K8" s="317"/>
+      <c r="L8" s="317"/>
+      <c r="M8" s="317"/>
       <c r="N8" s="212"/>
       <c r="O8" s="212"/>
     </row>
     <row r="9" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="313" t="s">
+      <c r="B9" s="312" t="s">
         <v>341</v>
       </c>
-      <c r="C9" s="313"/>
-      <c r="D9" s="313"/>
-      <c r="E9" s="313"/>
-      <c r="F9" s="313"/>
-      <c r="G9" s="313"/>
-      <c r="H9" s="313"/>
-      <c r="I9" s="313"/>
-      <c r="J9" s="313"/>
-      <c r="K9" s="313"/>
-      <c r="L9" s="313"/>
+      <c r="C9" s="312"/>
+      <c r="D9" s="312"/>
+      <c r="E9" s="312"/>
+      <c r="F9" s="312"/>
+      <c r="G9" s="312"/>
+      <c r="H9" s="312"/>
+      <c r="I9" s="312"/>
+      <c r="J9" s="312"/>
+      <c r="K9" s="312"/>
+      <c r="L9" s="312"/>
     </row>
     <row r="10" spans="2:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="313" t="s">
+      <c r="B10" s="312" t="s">
         <v>342</v>
       </c>
-      <c r="C10" s="313"/>
-      <c r="D10" s="313"/>
-      <c r="E10" s="313"/>
-      <c r="F10" s="313"/>
-      <c r="G10" s="313"/>
-      <c r="H10" s="313"/>
-      <c r="I10" s="313"/>
-      <c r="J10" s="313"/>
-      <c r="K10" s="313"/>
-      <c r="L10" s="313"/>
+      <c r="C10" s="312"/>
+      <c r="D10" s="312"/>
+      <c r="E10" s="312"/>
+      <c r="F10" s="312"/>
+      <c r="G10" s="312"/>
+      <c r="H10" s="312"/>
+      <c r="I10" s="312"/>
+      <c r="J10" s="312"/>
+      <c r="K10" s="312"/>
+      <c r="L10" s="312"/>
     </row>
     <row r="11" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="312" t="s">
+      <c r="B11" s="315" t="s">
         <v>343</v>
       </c>
-      <c r="C11" s="312"/>
-      <c r="D11" s="312"/>
-      <c r="E11" s="312"/>
-      <c r="F11" s="312"/>
-      <c r="G11" s="312"/>
-      <c r="H11" s="312"/>
-      <c r="I11" s="312"/>
-      <c r="J11" s="312"/>
-      <c r="K11" s="312"/>
-      <c r="L11" s="312"/>
-      <c r="M11" s="312"/>
+      <c r="C11" s="315"/>
+      <c r="D11" s="315"/>
+      <c r="E11" s="315"/>
+      <c r="F11" s="315"/>
+      <c r="G11" s="315"/>
+      <c r="H11" s="315"/>
+      <c r="I11" s="315"/>
+      <c r="J11" s="315"/>
+      <c r="K11" s="315"/>
+      <c r="L11" s="315"/>
+      <c r="M11" s="315"/>
       <c r="N11" s="69"/>
       <c r="O11" s="69"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="313" t="s">
+      <c r="B12" s="312" t="s">
         <v>344</v>
       </c>
-      <c r="C12" s="313"/>
-      <c r="D12" s="313"/>
-      <c r="E12" s="313"/>
-      <c r="F12" s="313"/>
-      <c r="G12" s="313"/>
-      <c r="H12" s="313"/>
-      <c r="I12" s="313"/>
-      <c r="J12" s="313"/>
-      <c r="K12" s="313"/>
-      <c r="L12" s="313"/>
-      <c r="M12" s="313"/>
+      <c r="C12" s="312"/>
+      <c r="D12" s="312"/>
+      <c r="E12" s="312"/>
+      <c r="F12" s="312"/>
+      <c r="G12" s="312"/>
+      <c r="H12" s="312"/>
+      <c r="I12" s="312"/>
+      <c r="J12" s="312"/>
+      <c r="K12" s="312"/>
+      <c r="L12" s="312"/>
+      <c r="M12" s="312"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="314" t="s">
+      <c r="B13" s="316" t="s">
         <v>369</v>
       </c>
-      <c r="C13" s="311"/>
-      <c r="D13" s="311"/>
-      <c r="E13" s="311"/>
-      <c r="F13" s="311"/>
-      <c r="G13" s="311"/>
-      <c r="H13" s="311"/>
-      <c r="I13" s="311"/>
-      <c r="J13" s="311"/>
-      <c r="K13" s="311"/>
-      <c r="L13" s="311"/>
-      <c r="M13" s="311"/>
+      <c r="C13" s="317"/>
+      <c r="D13" s="317"/>
+      <c r="E13" s="317"/>
+      <c r="F13" s="317"/>
+      <c r="G13" s="317"/>
+      <c r="H13" s="317"/>
+      <c r="I13" s="317"/>
+      <c r="J13" s="317"/>
+      <c r="K13" s="317"/>
+      <c r="L13" s="317"/>
+      <c r="M13" s="317"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="314" t="s">
+      <c r="B14" s="316" t="s">
         <v>370</v>
       </c>
-      <c r="C14" s="311"/>
-      <c r="D14" s="311"/>
-      <c r="E14" s="311"/>
-      <c r="F14" s="311"/>
-      <c r="G14" s="311"/>
-      <c r="H14" s="311"/>
-      <c r="I14" s="311"/>
-      <c r="J14" s="311"/>
-      <c r="K14" s="311"/>
-      <c r="L14" s="311"/>
-      <c r="M14" s="311"/>
+      <c r="C14" s="317"/>
+      <c r="D14" s="317"/>
+      <c r="E14" s="317"/>
+      <c r="F14" s="317"/>
+      <c r="G14" s="317"/>
+      <c r="H14" s="317"/>
+      <c r="I14" s="317"/>
+      <c r="J14" s="317"/>
+      <c r="K14" s="317"/>
+      <c r="L14" s="317"/>
+      <c r="M14" s="317"/>
     </row>
     <row r="15" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="314" t="s">
+      <c r="B15" s="316" t="s">
         <v>371</v>
       </c>
-      <c r="C15" s="311"/>
-      <c r="D15" s="311"/>
-      <c r="E15" s="311"/>
-      <c r="F15" s="311"/>
-      <c r="G15" s="311"/>
-      <c r="H15" s="311"/>
-      <c r="I15" s="311"/>
-      <c r="J15" s="311"/>
-      <c r="K15" s="311"/>
-      <c r="L15" s="311"/>
-      <c r="M15" s="311"/>
+      <c r="C15" s="317"/>
+      <c r="D15" s="317"/>
+      <c r="E15" s="317"/>
+      <c r="F15" s="317"/>
+      <c r="G15" s="317"/>
+      <c r="H15" s="317"/>
+      <c r="I15" s="317"/>
+      <c r="J15" s="317"/>
+      <c r="K15" s="317"/>
+      <c r="L15" s="317"/>
+      <c r="M15" s="317"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="313" t="s">
+      <c r="B16" s="312" t="s">
         <v>368</v>
       </c>
-      <c r="C16" s="313"/>
-      <c r="D16" s="313"/>
-      <c r="E16" s="313"/>
-      <c r="F16" s="313"/>
-      <c r="G16" s="313"/>
-      <c r="H16" s="313"/>
-      <c r="I16" s="313"/>
-      <c r="J16" s="313"/>
-      <c r="K16" s="313"/>
-      <c r="L16" s="313"/>
-      <c r="M16" s="313"/>
+      <c r="C16" s="312"/>
+      <c r="D16" s="312"/>
+      <c r="E16" s="312"/>
+      <c r="F16" s="312"/>
+      <c r="G16" s="312"/>
+      <c r="H16" s="312"/>
+      <c r="I16" s="312"/>
+      <c r="J16" s="312"/>
+      <c r="K16" s="312"/>
+      <c r="L16" s="312"/>
+      <c r="M16" s="312"/>
     </row>
     <row r="17" spans="2:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="B17" s="312" t="s">
+      <c r="B17" s="315" t="s">
         <v>345</v>
       </c>
-      <c r="C17" s="312"/>
-      <c r="D17" s="312"/>
-      <c r="E17" s="312"/>
-      <c r="F17" s="312"/>
-      <c r="G17" s="312"/>
-      <c r="H17" s="312"/>
-      <c r="I17" s="312"/>
-      <c r="J17" s="312"/>
-      <c r="K17" s="312"/>
-      <c r="L17" s="312"/>
-      <c r="M17" s="312"/>
+      <c r="C17" s="315"/>
+      <c r="D17" s="315"/>
+      <c r="E17" s="315"/>
+      <c r="F17" s="315"/>
+      <c r="G17" s="315"/>
+      <c r="H17" s="315"/>
+      <c r="I17" s="315"/>
+      <c r="J17" s="315"/>
+      <c r="K17" s="315"/>
+      <c r="L17" s="315"/>
+      <c r="M17" s="315"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="313" t="s">
+      <c r="B18" s="312" t="s">
         <v>346</v>
       </c>
-      <c r="C18" s="313"/>
-      <c r="D18" s="313"/>
-      <c r="E18" s="313"/>
-      <c r="F18" s="313"/>
-      <c r="G18" s="313"/>
-      <c r="H18" s="313"/>
-      <c r="I18" s="313"/>
-      <c r="J18" s="313"/>
-      <c r="K18" s="313"/>
-      <c r="L18" s="313"/>
-      <c r="M18" s="313"/>
+      <c r="C18" s="312"/>
+      <c r="D18" s="312"/>
+      <c r="E18" s="312"/>
+      <c r="F18" s="312"/>
+      <c r="G18" s="312"/>
+      <c r="H18" s="312"/>
+      <c r="I18" s="312"/>
+      <c r="J18" s="312"/>
+      <c r="K18" s="312"/>
+      <c r="L18" s="312"/>
+      <c r="M18" s="312"/>
     </row>
     <row r="19" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="280"/>
-      <c r="C19" s="317" t="s">
+      <c r="C19" s="311" t="s">
         <v>364</v>
       </c>
-      <c r="D19" s="317"/>
-      <c r="E19" s="317"/>
-      <c r="F19" s="317"/>
-      <c r="G19" s="317"/>
-      <c r="H19" s="317"/>
-      <c r="I19" s="317"/>
-      <c r="J19" s="317"/>
-      <c r="K19" s="317"/>
-      <c r="L19" s="317"/>
-      <c r="M19" s="317"/>
+      <c r="D19" s="311"/>
+      <c r="E19" s="311"/>
+      <c r="F19" s="311"/>
+      <c r="G19" s="311"/>
+      <c r="H19" s="311"/>
+      <c r="I19" s="311"/>
+      <c r="J19" s="311"/>
+      <c r="K19" s="311"/>
+      <c r="L19" s="311"/>
+      <c r="M19" s="311"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="280"/>
-      <c r="C20" s="317" t="s">
+      <c r="C20" s="311" t="s">
         <v>365</v>
       </c>
-      <c r="D20" s="317"/>
-      <c r="E20" s="317"/>
-      <c r="F20" s="317"/>
-      <c r="G20" s="317"/>
-      <c r="H20" s="317"/>
-      <c r="I20" s="317"/>
-      <c r="J20" s="317"/>
-      <c r="K20" s="317"/>
-      <c r="L20" s="317"/>
-      <c r="M20" s="317"/>
+      <c r="D20" s="311"/>
+      <c r="E20" s="311"/>
+      <c r="F20" s="311"/>
+      <c r="G20" s="311"/>
+      <c r="H20" s="311"/>
+      <c r="I20" s="311"/>
+      <c r="J20" s="311"/>
+      <c r="K20" s="311"/>
+      <c r="L20" s="311"/>
+      <c r="M20" s="311"/>
     </row>
     <row r="21" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="280"/>
-      <c r="C21" s="317" t="s">
+      <c r="C21" s="311" t="s">
         <v>464</v>
       </c>
-      <c r="D21" s="317"/>
-      <c r="E21" s="317"/>
-      <c r="F21" s="317"/>
-      <c r="G21" s="317"/>
-      <c r="H21" s="317"/>
-      <c r="I21" s="317"/>
-      <c r="J21" s="317"/>
-      <c r="K21" s="317"/>
-      <c r="L21" s="317"/>
-      <c r="M21" s="317"/>
+      <c r="D21" s="311"/>
+      <c r="E21" s="311"/>
+      <c r="F21" s="311"/>
+      <c r="G21" s="311"/>
+      <c r="H21" s="311"/>
+      <c r="I21" s="311"/>
+      <c r="J21" s="311"/>
+      <c r="K21" s="311"/>
+      <c r="L21" s="311"/>
+      <c r="M21" s="311"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="280"/>
-      <c r="C22" s="317" t="s">
+      <c r="C22" s="311" t="s">
         <v>460</v>
       </c>
-      <c r="D22" s="317"/>
-      <c r="E22" s="317"/>
-      <c r="F22" s="317"/>
-      <c r="G22" s="317"/>
-      <c r="H22" s="317"/>
-      <c r="I22" s="317"/>
-      <c r="J22" s="317"/>
-      <c r="K22" s="317"/>
-      <c r="L22" s="317"/>
-      <c r="M22" s="317"/>
+      <c r="D22" s="311"/>
+      <c r="E22" s="311"/>
+      <c r="F22" s="311"/>
+      <c r="G22" s="311"/>
+      <c r="H22" s="311"/>
+      <c r="I22" s="311"/>
+      <c r="J22" s="311"/>
+      <c r="K22" s="311"/>
+      <c r="L22" s="311"/>
+      <c r="M22" s="311"/>
     </row>
     <row r="23" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="280"/>
       <c r="C23" s="280"/>
-      <c r="D23" s="317" t="s">
+      <c r="D23" s="311" t="s">
         <v>456</v>
       </c>
-      <c r="E23" s="317"/>
-      <c r="F23" s="317"/>
-      <c r="G23" s="317"/>
-      <c r="H23" s="317"/>
-      <c r="I23" s="317"/>
-      <c r="J23" s="317"/>
-      <c r="K23" s="317"/>
-      <c r="L23" s="317"/>
-      <c r="M23" s="317"/>
+      <c r="E23" s="311"/>
+      <c r="F23" s="311"/>
+      <c r="G23" s="311"/>
+      <c r="H23" s="311"/>
+      <c r="I23" s="311"/>
+      <c r="J23" s="311"/>
+      <c r="K23" s="311"/>
+      <c r="L23" s="311"/>
+      <c r="M23" s="311"/>
     </row>
     <row r="24" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="280"/>
       <c r="C24" s="280"/>
-      <c r="D24" s="317" t="s">
+      <c r="D24" s="311" t="s">
         <v>457</v>
       </c>
-      <c r="E24" s="317"/>
-      <c r="F24" s="317"/>
-      <c r="G24" s="317"/>
-      <c r="H24" s="317"/>
-      <c r="I24" s="317"/>
-      <c r="J24" s="317"/>
-      <c r="K24" s="317"/>
-      <c r="L24" s="317"/>
-      <c r="M24" s="317"/>
+      <c r="E24" s="311"/>
+      <c r="F24" s="311"/>
+      <c r="G24" s="311"/>
+      <c r="H24" s="311"/>
+      <c r="I24" s="311"/>
+      <c r="J24" s="311"/>
+      <c r="K24" s="311"/>
+      <c r="L24" s="311"/>
+      <c r="M24" s="311"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="277"/>
       <c r="C25" s="278"/>
-      <c r="D25" s="313" t="s">
+      <c r="D25" s="312" t="s">
         <v>458</v>
       </c>
-      <c r="E25" s="313"/>
-      <c r="F25" s="313"/>
-      <c r="G25" s="313"/>
-      <c r="H25" s="313"/>
-      <c r="I25" s="313"/>
-      <c r="J25" s="313"/>
-      <c r="K25" s="313"/>
-      <c r="L25" s="313"/>
-      <c r="M25" s="313"/>
+      <c r="E25" s="312"/>
+      <c r="F25" s="312"/>
+      <c r="G25" s="312"/>
+      <c r="H25" s="312"/>
+      <c r="I25" s="312"/>
+      <c r="J25" s="312"/>
+      <c r="K25" s="312"/>
+      <c r="L25" s="312"/>
+      <c r="M25" s="312"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="277"/>
       <c r="C26" s="278"/>
-      <c r="D26" s="317" t="s">
+      <c r="D26" s="311" t="s">
         <v>459</v>
       </c>
-      <c r="E26" s="317"/>
-      <c r="F26" s="317"/>
-      <c r="G26" s="317"/>
-      <c r="H26" s="317"/>
-      <c r="I26" s="317"/>
-      <c r="J26" s="317"/>
-      <c r="K26" s="317"/>
-      <c r="L26" s="317"/>
-      <c r="M26" s="317"/>
+      <c r="E26" s="311"/>
+      <c r="F26" s="311"/>
+      <c r="G26" s="311"/>
+      <c r="H26" s="311"/>
+      <c r="I26" s="311"/>
+      <c r="J26" s="311"/>
+      <c r="K26" s="311"/>
+      <c r="L26" s="311"/>
+      <c r="M26" s="311"/>
     </row>
     <row r="27" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="314" t="s">
+      <c r="B27" s="316" t="s">
         <v>366</v>
       </c>
-      <c r="C27" s="311"/>
-      <c r="D27" s="311"/>
-      <c r="E27" s="311"/>
-      <c r="F27" s="311"/>
-      <c r="G27" s="311"/>
-      <c r="H27" s="311"/>
-      <c r="I27" s="311"/>
-      <c r="J27" s="311"/>
-      <c r="K27" s="311"/>
-      <c r="L27" s="311"/>
-      <c r="M27" s="311"/>
+      <c r="C27" s="317"/>
+      <c r="D27" s="317"/>
+      <c r="E27" s="317"/>
+      <c r="F27" s="317"/>
+      <c r="G27" s="317"/>
+      <c r="H27" s="317"/>
+      <c r="I27" s="317"/>
+      <c r="J27" s="317"/>
+      <c r="K27" s="317"/>
+      <c r="L27" s="317"/>
+      <c r="M27" s="317"/>
     </row>
     <row r="28" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="314" t="s">
+      <c r="B28" s="316" t="s">
         <v>367</v>
       </c>
-      <c r="C28" s="311"/>
-      <c r="D28" s="311"/>
-      <c r="E28" s="311"/>
-      <c r="F28" s="311"/>
-      <c r="G28" s="311"/>
-      <c r="H28" s="311"/>
-      <c r="I28" s="311"/>
-      <c r="J28" s="311"/>
-      <c r="K28" s="311"/>
-      <c r="L28" s="311"/>
-      <c r="M28" s="311"/>
+      <c r="C28" s="317"/>
+      <c r="D28" s="317"/>
+      <c r="E28" s="317"/>
+      <c r="F28" s="317"/>
+      <c r="G28" s="317"/>
+      <c r="H28" s="317"/>
+      <c r="I28" s="317"/>
+      <c r="J28" s="317"/>
+      <c r="K28" s="317"/>
+      <c r="L28" s="317"/>
+      <c r="M28" s="317"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="209"/>
     </row>
     <row r="30" spans="2:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="B30" s="312" t="s">
+      <c r="B30" s="315" t="s">
         <v>347</v>
       </c>
-      <c r="C30" s="312"/>
-      <c r="D30" s="312"/>
-      <c r="E30" s="312"/>
-      <c r="F30" s="312"/>
-      <c r="G30" s="312"/>
-      <c r="H30" s="312"/>
-      <c r="I30" s="312"/>
-      <c r="J30" s="312"/>
-      <c r="K30" s="312"/>
-      <c r="L30" s="312"/>
-      <c r="M30" s="312"/>
+      <c r="C30" s="315"/>
+      <c r="D30" s="315"/>
+      <c r="E30" s="315"/>
+      <c r="F30" s="315"/>
+      <c r="G30" s="315"/>
+      <c r="H30" s="315"/>
+      <c r="I30" s="315"/>
+      <c r="J30" s="315"/>
+      <c r="K30" s="315"/>
+      <c r="L30" s="315"/>
+      <c r="M30" s="315"/>
     </row>
     <row r="31" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="313" t="s">
+      <c r="B31" s="312" t="s">
         <v>372</v>
       </c>
-      <c r="C31" s="313"/>
-      <c r="D31" s="313"/>
-      <c r="E31" s="313"/>
-      <c r="F31" s="313"/>
-      <c r="G31" s="313"/>
-      <c r="H31" s="313"/>
-      <c r="I31" s="313"/>
-      <c r="J31" s="313"/>
-      <c r="K31" s="313"/>
-      <c r="L31" s="313"/>
-      <c r="M31" s="313"/>
+      <c r="C31" s="312"/>
+      <c r="D31" s="312"/>
+      <c r="E31" s="312"/>
+      <c r="F31" s="312"/>
+      <c r="G31" s="312"/>
+      <c r="H31" s="312"/>
+      <c r="I31" s="312"/>
+      <c r="J31" s="312"/>
+      <c r="K31" s="312"/>
+      <c r="L31" s="312"/>
+      <c r="M31" s="312"/>
     </row>
     <row r="32" spans="2:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="313" t="s">
+      <c r="B32" s="312" t="s">
         <v>348</v>
       </c>
-      <c r="C32" s="313"/>
-      <c r="D32" s="313"/>
-      <c r="E32" s="313"/>
-      <c r="F32" s="313"/>
-      <c r="G32" s="313"/>
-      <c r="H32" s="313"/>
-      <c r="I32" s="313"/>
-      <c r="J32" s="313"/>
-      <c r="K32" s="313"/>
-      <c r="L32" s="313"/>
-      <c r="M32" s="313"/>
+      <c r="C32" s="312"/>
+      <c r="D32" s="312"/>
+      <c r="E32" s="312"/>
+      <c r="F32" s="312"/>
+      <c r="G32" s="312"/>
+      <c r="H32" s="312"/>
+      <c r="I32" s="312"/>
+      <c r="J32" s="312"/>
+      <c r="K32" s="312"/>
+      <c r="L32" s="312"/>
+      <c r="M32" s="312"/>
     </row>
     <row r="33" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="313" t="s">
+      <c r="B33" s="312" t="s">
         <v>349</v>
       </c>
-      <c r="C33" s="313"/>
-      <c r="D33" s="313"/>
-      <c r="E33" s="313"/>
-      <c r="F33" s="313"/>
-      <c r="G33" s="313"/>
-      <c r="H33" s="313"/>
-      <c r="I33" s="313"/>
-      <c r="J33" s="313"/>
-      <c r="K33" s="313"/>
-      <c r="L33" s="313"/>
-      <c r="M33" s="313"/>
+      <c r="C33" s="312"/>
+      <c r="D33" s="312"/>
+      <c r="E33" s="312"/>
+      <c r="F33" s="312"/>
+      <c r="G33" s="312"/>
+      <c r="H33" s="312"/>
+      <c r="I33" s="312"/>
+      <c r="J33" s="312"/>
+      <c r="K33" s="312"/>
+      <c r="L33" s="312"/>
+      <c r="M33" s="312"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B34" s="313" t="s">
+      <c r="B34" s="312" t="s">
         <v>350</v>
       </c>
-      <c r="C34" s="313"/>
-      <c r="D34" s="313"/>
-      <c r="E34" s="313"/>
-      <c r="F34" s="313"/>
-      <c r="G34" s="313"/>
-      <c r="H34" s="313"/>
-      <c r="I34" s="313"/>
-      <c r="J34" s="313"/>
-      <c r="K34" s="313"/>
-      <c r="L34" s="313"/>
-      <c r="M34" s="313"/>
+      <c r="C34" s="312"/>
+      <c r="D34" s="312"/>
+      <c r="E34" s="312"/>
+      <c r="F34" s="312"/>
+      <c r="G34" s="312"/>
+      <c r="H34" s="312"/>
+      <c r="I34" s="312"/>
+      <c r="J34" s="312"/>
+      <c r="K34" s="312"/>
+      <c r="L34" s="312"/>
+      <c r="M34" s="312"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B35" s="313" t="s">
+      <c r="B35" s="312" t="s">
         <v>351</v>
       </c>
-      <c r="C35" s="313"/>
-      <c r="D35" s="313"/>
-      <c r="E35" s="313"/>
-      <c r="F35" s="313"/>
-      <c r="G35" s="313"/>
-      <c r="H35" s="313"/>
-      <c r="I35" s="313"/>
-      <c r="J35" s="313"/>
-      <c r="K35" s="313"/>
-      <c r="L35" s="313"/>
-      <c r="M35" s="313"/>
+      <c r="C35" s="312"/>
+      <c r="D35" s="312"/>
+      <c r="E35" s="312"/>
+      <c r="F35" s="312"/>
+      <c r="G35" s="312"/>
+      <c r="H35" s="312"/>
+      <c r="I35" s="312"/>
+      <c r="J35" s="312"/>
+      <c r="K35" s="312"/>
+      <c r="L35" s="312"/>
+      <c r="M35" s="312"/>
     </row>
     <row r="36" spans="2:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="B36" s="312" t="s">
+      <c r="B36" s="315" t="s">
         <v>352</v>
       </c>
-      <c r="C36" s="312"/>
-      <c r="D36" s="312"/>
-      <c r="E36" s="312"/>
-      <c r="F36" s="312"/>
-      <c r="G36" s="312"/>
-      <c r="H36" s="312"/>
-      <c r="I36" s="312"/>
-      <c r="J36" s="312"/>
-      <c r="K36" s="312"/>
-      <c r="L36" s="312"/>
-      <c r="M36" s="312"/>
+      <c r="C36" s="315"/>
+      <c r="D36" s="315"/>
+      <c r="E36" s="315"/>
+      <c r="F36" s="315"/>
+      <c r="G36" s="315"/>
+      <c r="H36" s="315"/>
+      <c r="I36" s="315"/>
+      <c r="J36" s="315"/>
+      <c r="K36" s="315"/>
+      <c r="L36" s="315"/>
+      <c r="M36" s="315"/>
     </row>
     <row r="37" spans="2:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="313" t="s">
+      <c r="B37" s="312" t="s">
         <v>353</v>
       </c>
-      <c r="C37" s="313"/>
-      <c r="D37" s="313"/>
-      <c r="E37" s="313"/>
-      <c r="F37" s="313"/>
-      <c r="G37" s="313"/>
-      <c r="H37" s="313"/>
-      <c r="I37" s="313"/>
-      <c r="J37" s="313"/>
-      <c r="K37" s="313"/>
-      <c r="L37" s="313"/>
-      <c r="M37" s="313"/>
+      <c r="C37" s="312"/>
+      <c r="D37" s="312"/>
+      <c r="E37" s="312"/>
+      <c r="F37" s="312"/>
+      <c r="G37" s="312"/>
+      <c r="H37" s="312"/>
+      <c r="I37" s="312"/>
+      <c r="J37" s="312"/>
+      <c r="K37" s="312"/>
+      <c r="L37" s="312"/>
+      <c r="M37" s="312"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B38" s="313" t="s">
+      <c r="B38" s="312" t="s">
         <v>354</v>
       </c>
-      <c r="C38" s="313"/>
-      <c r="D38" s="313"/>
-      <c r="E38" s="313"/>
-      <c r="F38" s="313"/>
-      <c r="G38" s="313"/>
-      <c r="H38" s="313"/>
-      <c r="I38" s="313"/>
-      <c r="J38" s="313"/>
-      <c r="K38" s="313"/>
-      <c r="L38" s="313"/>
-      <c r="M38" s="313"/>
+      <c r="C38" s="312"/>
+      <c r="D38" s="312"/>
+      <c r="E38" s="312"/>
+      <c r="F38" s="312"/>
+      <c r="G38" s="312"/>
+      <c r="H38" s="312"/>
+      <c r="I38" s="312"/>
+      <c r="J38" s="312"/>
+      <c r="K38" s="312"/>
+      <c r="L38" s="312"/>
+      <c r="M38" s="312"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39" s="209"/>
     </row>
     <row r="40" spans="2:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="B40" s="312" t="s">
+      <c r="B40" s="315" t="s">
         <v>355</v>
       </c>
-      <c r="C40" s="312"/>
-      <c r="D40" s="312"/>
-      <c r="E40" s="312"/>
-      <c r="F40" s="312"/>
-      <c r="G40" s="312"/>
-      <c r="H40" s="312"/>
-      <c r="I40" s="312"/>
-      <c r="J40" s="312"/>
-      <c r="K40" s="312"/>
-      <c r="L40" s="312"/>
-      <c r="M40" s="312"/>
+      <c r="C40" s="315"/>
+      <c r="D40" s="315"/>
+      <c r="E40" s="315"/>
+      <c r="F40" s="315"/>
+      <c r="G40" s="315"/>
+      <c r="H40" s="315"/>
+      <c r="I40" s="315"/>
+      <c r="J40" s="315"/>
+      <c r="K40" s="315"/>
+      <c r="L40" s="315"/>
+      <c r="M40" s="315"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B41" s="319" t="s">
+      <c r="B41" s="314" t="s">
         <v>356</v>
       </c>
-      <c r="C41" s="319"/>
-      <c r="D41" s="319"/>
-      <c r="E41" s="319"/>
-      <c r="F41" s="319"/>
-      <c r="G41" s="319"/>
-      <c r="H41" s="319"/>
-      <c r="I41" s="319"/>
-      <c r="J41" s="319"/>
-      <c r="K41" s="319"/>
-      <c r="L41" s="319"/>
-      <c r="M41" s="319"/>
+      <c r="C41" s="314"/>
+      <c r="D41" s="314"/>
+      <c r="E41" s="314"/>
+      <c r="F41" s="314"/>
+      <c r="G41" s="314"/>
+      <c r="H41" s="314"/>
+      <c r="I41" s="314"/>
+      <c r="J41" s="314"/>
+      <c r="K41" s="314"/>
+      <c r="L41" s="314"/>
+      <c r="M41" s="314"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B42" s="319" t="s">
+      <c r="B42" s="314" t="s">
         <v>357</v>
       </c>
-      <c r="C42" s="319"/>
-      <c r="D42" s="319"/>
-      <c r="E42" s="319"/>
-      <c r="F42" s="319"/>
-      <c r="G42" s="319"/>
-      <c r="H42" s="319"/>
-      <c r="I42" s="319"/>
-      <c r="J42" s="319"/>
-      <c r="K42" s="319"/>
-      <c r="L42" s="319"/>
-      <c r="M42" s="319"/>
+      <c r="C42" s="314"/>
+      <c r="D42" s="314"/>
+      <c r="E42" s="314"/>
+      <c r="F42" s="314"/>
+      <c r="G42" s="314"/>
+      <c r="H42" s="314"/>
+      <c r="I42" s="314"/>
+      <c r="J42" s="314"/>
+      <c r="K42" s="314"/>
+      <c r="L42" s="314"/>
+      <c r="M42" s="314"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B43" s="319" t="s">
+      <c r="B43" s="314" t="s">
         <v>358</v>
       </c>
-      <c r="C43" s="319"/>
-      <c r="D43" s="319"/>
-      <c r="E43" s="319"/>
-      <c r="F43" s="319"/>
-      <c r="G43" s="319"/>
-      <c r="H43" s="319"/>
-      <c r="I43" s="319"/>
-      <c r="J43" s="319"/>
-      <c r="K43" s="319"/>
-      <c r="L43" s="319"/>
-      <c r="M43" s="319"/>
+      <c r="C43" s="314"/>
+      <c r="D43" s="314"/>
+      <c r="E43" s="314"/>
+      <c r="F43" s="314"/>
+      <c r="G43" s="314"/>
+      <c r="H43" s="314"/>
+      <c r="I43" s="314"/>
+      <c r="J43" s="314"/>
+      <c r="K43" s="314"/>
+      <c r="L43" s="314"/>
+      <c r="M43" s="314"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44" s="270" t="s">
@@ -9241,55 +9653,82 @@
       <c r="M44" s="268"/>
     </row>
     <row r="45" spans="2:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="B45" s="312" t="s">
+      <c r="B45" s="315" t="s">
         <v>359</v>
       </c>
-      <c r="C45" s="312"/>
-      <c r="D45" s="312"/>
-      <c r="E45" s="312"/>
-      <c r="F45" s="312"/>
-      <c r="G45" s="312"/>
-      <c r="H45" s="312"/>
-      <c r="I45" s="312"/>
-      <c r="J45" s="312"/>
-      <c r="K45" s="312"/>
-      <c r="L45" s="312"/>
-      <c r="M45" s="312"/>
+      <c r="C45" s="315"/>
+      <c r="D45" s="315"/>
+      <c r="E45" s="315"/>
+      <c r="F45" s="315"/>
+      <c r="G45" s="315"/>
+      <c r="H45" s="315"/>
+      <c r="I45" s="315"/>
+      <c r="J45" s="315"/>
+      <c r="K45" s="315"/>
+      <c r="L45" s="315"/>
+      <c r="M45" s="315"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B46" s="313" t="s">
+      <c r="B46" s="312" t="s">
         <v>463</v>
       </c>
-      <c r="C46" s="313"/>
-      <c r="D46" s="313"/>
-      <c r="E46" s="313"/>
-      <c r="F46" s="313"/>
-      <c r="G46" s="313"/>
-      <c r="H46" s="313"/>
-      <c r="I46" s="313"/>
-      <c r="J46" s="313"/>
-      <c r="K46" s="313"/>
-      <c r="L46" s="313"/>
-      <c r="M46" s="313"/>
+      <c r="C46" s="312"/>
+      <c r="D46" s="312"/>
+      <c r="E46" s="312"/>
+      <c r="F46" s="312"/>
+      <c r="G46" s="312"/>
+      <c r="H46" s="312"/>
+      <c r="I46" s="312"/>
+      <c r="J46" s="312"/>
+      <c r="K46" s="312"/>
+      <c r="L46" s="312"/>
+      <c r="M46" s="312"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B47" s="318" t="s">
+      <c r="B47" s="313" t="s">
         <v>449</v>
       </c>
-      <c r="C47" s="318"/>
-      <c r="D47" s="318"/>
-      <c r="E47" s="318"/>
-      <c r="F47" s="318"/>
-      <c r="G47" s="318"/>
-      <c r="H47" s="318"/>
-      <c r="I47" s="318"/>
-      <c r="J47" s="318"/>
-      <c r="K47" s="318"/>
-      <c r="L47" s="318"/>
-      <c r="M47" s="318"/>
+      <c r="C47" s="313"/>
+      <c r="D47" s="313"/>
+      <c r="E47" s="313"/>
+      <c r="F47" s="313"/>
+      <c r="G47" s="313"/>
+      <c r="H47" s="313"/>
+      <c r="I47" s="313"/>
+      <c r="J47" s="313"/>
+      <c r="K47" s="313"/>
+      <c r="L47" s="313"/>
+      <c r="M47" s="313"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B12:M12"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="C21:M21"/>
+    <mergeCell ref="C22:M22"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="C19:M19"/>
+    <mergeCell ref="C20:M20"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="B27:M27"/>
+    <mergeCell ref="B28:M28"/>
+    <mergeCell ref="B30:M30"/>
     <mergeCell ref="D23:M23"/>
     <mergeCell ref="D24:M24"/>
     <mergeCell ref="D25:M25"/>
@@ -9306,33 +9745,6 @@
     <mergeCell ref="B41:M41"/>
     <mergeCell ref="B31:M31"/>
     <mergeCell ref="B32:M32"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B35:M35"/>
-    <mergeCell ref="B27:M27"/>
-    <mergeCell ref="B28:M28"/>
-    <mergeCell ref="B30:M30"/>
-    <mergeCell ref="C21:M21"/>
-    <mergeCell ref="C22:M22"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="B16:M16"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="B18:M18"/>
-    <mergeCell ref="C19:M19"/>
-    <mergeCell ref="C20:M20"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B8:M8"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B12:M12"/>
-    <mergeCell ref="B13:M13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B41" r:id="rId1" display="https://cdn.who.int/media/docs/default-source/documents/about-us/thirteenth-general-programme/gpw13_methodology_nov9_online-version1b3170f8-98ea-4fcc-aa3a-059ede7e51ad.pdf?sfvrsn=12dfeb0d_1&amp;download=true" xr:uid="{5B1AD3AB-AC30-4E70-9D4E-7E9B49DF39DD}"/>
@@ -10024,121 +10436,121 @@
       <c r="Z8" s="13"/>
     </row>
     <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="365" t="s">
+      <c r="A9" s="351" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="365"/>
-      <c r="C9" s="363" t="s">
+      <c r="B9" s="351"/>
+      <c r="C9" s="346" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="363"/>
-      <c r="E9" s="363"/>
-      <c r="F9" s="363"/>
-      <c r="G9" s="363"/>
-      <c r="H9" s="363"/>
-      <c r="I9" s="363"/>
+      <c r="D9" s="346"/>
+      <c r="E9" s="346"/>
+      <c r="F9" s="346"/>
+      <c r="G9" s="346"/>
+      <c r="H9" s="346"/>
+      <c r="I9" s="346"/>
       <c r="J9" s="30"/>
-      <c r="K9" s="364" t="s">
+      <c r="K9" s="347" t="s">
         <v>78</v>
       </c>
-      <c r="L9" s="364"/>
-      <c r="M9" s="364"/>
-      <c r="N9" s="364"/>
-      <c r="O9" s="364"/>
-      <c r="P9" s="364"/>
-      <c r="Q9" s="364"/>
-      <c r="R9" s="364"/>
-      <c r="S9" s="364"/>
-      <c r="T9" s="364"/>
-      <c r="U9" s="364"/>
+      <c r="L9" s="347"/>
+      <c r="M9" s="347"/>
+      <c r="N9" s="347"/>
+      <c r="O9" s="347"/>
+      <c r="P9" s="347"/>
+      <c r="Q9" s="347"/>
+      <c r="R9" s="347"/>
+      <c r="S9" s="347"/>
+      <c r="T9" s="347"/>
+      <c r="U9" s="347"/>
       <c r="V9" s="30"/>
-      <c r="W9" s="360" t="s">
+      <c r="W9" s="357" t="s">
         <v>79</v>
       </c>
-      <c r="X9" s="361"/>
-      <c r="Y9" s="361"/>
-      <c r="Z9" s="362"/>
+      <c r="X9" s="358"/>
+      <c r="Y9" s="358"/>
+      <c r="Z9" s="359"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="349" t="s">
+      <c r="A10" s="350" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="349" t="s">
+      <c r="B10" s="350" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="349" t="s">
+      <c r="C10" s="350" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="349" t="s">
+      <c r="D10" s="350" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="349" t="s">
+      <c r="E10" s="350" t="s">
         <v>120</v>
       </c>
-      <c r="F10" s="349" t="s">
+      <c r="F10" s="350" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="349" t="s">
+      <c r="G10" s="350" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="351" t="s">
+      <c r="H10" s="348" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="351" t="s">
+      <c r="I10" s="348" t="s">
         <v>114</v>
       </c>
       <c r="J10" s="31"/>
-      <c r="K10" s="353" t="s">
+      <c r="K10" s="363" t="s">
         <v>81</v>
       </c>
-      <c r="L10" s="353" t="s">
+      <c r="L10" s="363" t="s">
         <v>82</v>
       </c>
       <c r="M10" s="85"/>
-      <c r="N10" s="353" t="s">
+      <c r="N10" s="363" t="s">
         <v>83</v>
       </c>
-      <c r="O10" s="353" t="s">
+      <c r="O10" s="363" t="s">
         <v>82</v>
       </c>
       <c r="P10" s="85"/>
-      <c r="Q10" s="353" t="s">
+      <c r="Q10" s="363" t="s">
         <v>84</v>
       </c>
-      <c r="R10" s="353" t="s">
+      <c r="R10" s="363" t="s">
         <v>82</v>
       </c>
       <c r="S10" s="85"/>
-      <c r="T10" s="353" t="s">
+      <c r="T10" s="363" t="s">
         <v>85</v>
       </c>
-      <c r="U10" s="353" t="s">
+      <c r="U10" s="363" t="s">
         <v>82</v>
       </c>
       <c r="V10" s="31"/>
-      <c r="W10" s="350" t="s">
+      <c r="W10" s="362" t="s">
         <v>118</v>
       </c>
-      <c r="X10" s="349" t="s">
+      <c r="X10" s="350" t="s">
         <v>115</v>
       </c>
-      <c r="Y10" s="349" t="s">
+      <c r="Y10" s="350" t="s">
         <v>116</v>
       </c>
-      <c r="Z10" s="349" t="s">
+      <c r="Z10" s="350" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="349"/>
-      <c r="B11" s="349"/>
-      <c r="C11" s="352"/>
-      <c r="D11" s="352"/>
-      <c r="E11" s="352"/>
-      <c r="F11" s="352"/>
-      <c r="G11" s="352"/>
-      <c r="H11" s="352"/>
-      <c r="I11" s="352"/>
+      <c r="A11" s="350"/>
+      <c r="B11" s="350"/>
+      <c r="C11" s="349"/>
+      <c r="D11" s="349"/>
+      <c r="E11" s="349"/>
+      <c r="F11" s="349"/>
+      <c r="G11" s="349"/>
+      <c r="H11" s="349"/>
+      <c r="I11" s="349"/>
       <c r="J11" s="31"/>
       <c r="K11" s="27">
         <v>2018</v>
@@ -10168,10 +10580,10 @@
         <v>2023</v>
       </c>
       <c r="V11" s="31"/>
-      <c r="W11" s="350"/>
-      <c r="X11" s="349"/>
-      <c r="Y11" s="349"/>
-      <c r="Z11" s="349"/>
+      <c r="W11" s="362"/>
+      <c r="X11" s="350"/>
+      <c r="Y11" s="350"/>
+      <c r="Z11" s="350"/>
     </row>
     <row r="12" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="183" t="s">
@@ -11354,14 +11766,14 @@
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
       <c r="U30" s="13"/>
-      <c r="W30" s="354" t="s">
+      <c r="W30" s="364" t="s">
         <v>104</v>
       </c>
-      <c r="X30" s="355"/>
-      <c r="Y30" s="356" t="s">
+      <c r="X30" s="365"/>
+      <c r="Y30" s="352" t="s">
         <v>105</v>
       </c>
-      <c r="Z30" s="357"/>
+      <c r="Z30" s="353"/>
     </row>
     <row r="31" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="51" t="s">
@@ -11388,10 +11800,10 @@
       <c r="T31" s="13"/>
       <c r="U31" s="13"/>
       <c r="V31" s="26"/>
-      <c r="W31" s="358" t="s">
+      <c r="W31" s="354" t="s">
         <v>107</v>
       </c>
-      <c r="X31" s="359"/>
+      <c r="X31" s="355"/>
       <c r="Y31" s="40" t="s">
         <v>126</v>
       </c>
@@ -11424,10 +11836,10 @@
       <c r="T32" s="13"/>
       <c r="U32" s="13"/>
       <c r="V32" s="26"/>
-      <c r="W32" s="346" t="s">
+      <c r="W32" s="356" t="s">
         <v>109</v>
       </c>
-      <c r="X32" s="346"/>
+      <c r="X32" s="356"/>
       <c r="Y32" s="254">
         <v>1660448.0263009099</v>
       </c>
@@ -11461,10 +11873,10 @@
       <c r="T33" s="13"/>
       <c r="U33" s="13"/>
       <c r="V33" s="26"/>
-      <c r="W33" s="346" t="s">
+      <c r="W33" s="356" t="s">
         <v>111</v>
       </c>
-      <c r="X33" s="346"/>
+      <c r="X33" s="356"/>
       <c r="Y33" s="254">
         <v>-691434.53619569901</v>
       </c>
@@ -11496,10 +11908,10 @@
       <c r="S34" s="13"/>
       <c r="T34" s="13"/>
       <c r="U34" s="13"/>
-      <c r="W34" s="347" t="s">
+      <c r="W34" s="360" t="s">
         <v>444</v>
       </c>
-      <c r="X34" s="348"/>
+      <c r="X34" s="361"/>
       <c r="Y34" s="255">
         <f>Y32+Y33</f>
         <v>969013.49010521092</v>
@@ -11531,10 +11943,10 @@
       <c r="S35" s="13"/>
       <c r="T35" s="13"/>
       <c r="U35" s="13"/>
-      <c r="W35" s="346" t="s">
+      <c r="W35" s="356" t="s">
         <v>112</v>
       </c>
-      <c r="X35" s="346"/>
+      <c r="X35" s="356"/>
       <c r="Y35" s="254">
         <v>3.6784375539831999</v>
       </c>
@@ -11936,18 +12348,6 @@
     <row r="76" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="K9:U9"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="Y30:Z30"/>
-    <mergeCell ref="W31:X31"/>
-    <mergeCell ref="W32:X32"/>
-    <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="W9:Z9"/>
-    <mergeCell ref="Z10:Z11"/>
     <mergeCell ref="W33:X33"/>
     <mergeCell ref="W34:X34"/>
     <mergeCell ref="W35:X35"/>
@@ -11964,6 +12364,18 @@
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
+    <mergeCell ref="Y30:Z30"/>
+    <mergeCell ref="W31:X31"/>
+    <mergeCell ref="W32:X32"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="W9:Z9"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="K9:U9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <conditionalFormatting sqref="E12:E28">
     <cfRule type="expression" dxfId="1" priority="2">
@@ -20243,31 +20655,31 @@
       </c>
       <c r="C10" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>66.64</v>
+        <v>16.68</v>
       </c>
       <c r="D10" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>69.42</v>
-      </c>
-      <c r="E10" s="56">
+        <v>15.29</v>
+      </c>
+      <c r="E10" s="56" t="e">
         <f t="shared" si="0"/>
-        <v>69.42</v>
-      </c>
-      <c r="F10" s="56" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F10" s="56">
         <f t="shared" si="1"/>
+        <v>15.29</v>
+      </c>
+      <c r="G10" s="56" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="G10" s="56">
-        <f t="shared" si="2"/>
-        <v>2.7800000000000011</v>
-      </c>
-      <c r="H10" s="56" t="e">
+      <c r="H10" s="56">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>1.3900000000000006</v>
       </c>
       <c r="I10" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>64.900000000000006</v>
+        <v>17.55</v>
       </c>
       <c r="J10" s="208">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A10,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
@@ -20283,31 +20695,31 @@
       </c>
       <c r="C11" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>99</v>
+        <v>5.12</v>
       </c>
       <c r="D11" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>100</v>
-      </c>
-      <c r="E11" s="56">
+        <v>5.03</v>
+      </c>
+      <c r="E11" s="56" t="e">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F11" s="56" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F11" s="56">
         <f t="shared" si="1"/>
+        <v>5.03</v>
+      </c>
+      <c r="G11" s="56" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="G11" s="56">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H11" s="56" t="e">
+      <c r="H11" s="56">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>8.9999999999999858E-2</v>
       </c>
       <c r="I11" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>95</v>
+        <v>5.2</v>
       </c>
       <c r="J11" s="208">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A11,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
@@ -20323,31 +20735,31 @@
       </c>
       <c r="C12" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>78.099999999999994</v>
+        <v>21.9</v>
       </c>
       <c r="D12" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>80.5</v>
-      </c>
-      <c r="E12" s="56">
+        <v>19.5</v>
+      </c>
+      <c r="E12" s="56" t="e">
         <f t="shared" si="0"/>
-        <v>80.5</v>
-      </c>
-      <c r="F12" s="56" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F12" s="56">
         <f t="shared" si="1"/>
+        <v>19.5</v>
+      </c>
+      <c r="G12" s="56" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="G12" s="56">
-        <f t="shared" si="2"/>
-        <v>2.4000000000000057</v>
-      </c>
-      <c r="H12" s="56" t="e">
+      <c r="H12" s="56">
         <f t="shared" si="3"/>
-        <v>#N/A</v>
+        <v>2.3999999999999986</v>
       </c>
       <c r="I12" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>78.099999999999994</v>
+        <v>21.9</v>
       </c>
       <c r="J12" s="208">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A12,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
@@ -20363,23 +20775,23 @@
       </c>
       <c r="C13" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>100</v>
+        <v>129.04</v>
       </c>
       <c r="D13" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>100</v>
-      </c>
-      <c r="E13" s="56" t="e">
+        <v>130.5</v>
+      </c>
+      <c r="E13" s="56">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>130.5</v>
       </c>
       <c r="F13" s="56" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G13" s="56" t="e">
+      <c r="G13" s="56">
         <f t="shared" si="2"/>
-        <v>#N/A</v>
+        <v>1.460000000000008</v>
       </c>
       <c r="H13" s="56" t="e">
         <f t="shared" si="3"/>
@@ -20387,7 +20799,7 @@
       </c>
       <c r="I13" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>100</v>
+        <v>129.04</v>
       </c>
       <c r="J13" s="208">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A13,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
@@ -20403,15 +20815,15 @@
       </c>
       <c r="C14" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!I$1:I$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!L$1:L$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>98.08</v>
+        <v>151.77000000000001</v>
       </c>
       <c r="D14" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))=0,INDEX([1]UHC_summary!J$1:J$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!M$1:M$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>100</v>
+        <v>172.69</v>
       </c>
       <c r="E14" s="56">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>172.69</v>
       </c>
       <c r="F14" s="56" t="e">
         <f t="shared" si="1"/>
@@ -20419,7 +20831,7 @@
       </c>
       <c r="G14" s="56">
         <f t="shared" si="2"/>
-        <v>1.9200000000000017</v>
+        <v>20.919999999999987</v>
       </c>
       <c r="H14" s="56" t="e">
         <f t="shared" si="3"/>
@@ -20427,7 +20839,7 @@
       </c>
       <c r="I14" s="56">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))="",INDEX([1]UHC_summary!C$1:C$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0)), INDEX([1]UHC_summary!D$1:D$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
-        <v>98.08</v>
+        <v>151.77000000000001</v>
       </c>
       <c r="J14" s="208">
         <f>_xlfn.IFNA(IF(INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))=0,"",INDEX([1]UHC_summary!E$1:E$101,MATCH([1]UHC_Inter!$A14,[1]UHC_summary!$B$1:$B$101,0))),"")</f>
@@ -25330,12 +25742,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FB6FBD5E95BAB542B810C32545CA4E3B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c88f4da8c98e9c6f14dc759bd92b3b9d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f244dd4c-ee25-4b14-a7cd-a89d47e877b9" xmlns:ns4="7d5efbb1-7b5c-4600-961f-d0c91f173691" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11dd0c1a7b4f1799f1daf73497fb7c0" ns3:_="" ns4:_="">
     <xsd:import namespace="f244dd4c-ee25-4b14-a7cd-a89d47e877b9"/>
@@ -25546,6 +25952,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5668EAE9-BE2F-449B-83FE-5638B2ED2DF4}">
   <ds:schemaRefs>
@@ -25555,23 +25967,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C5798F-31D9-455C-A266-3CF2A88C6872}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7d5efbb1-7b5c-4600-961f-d0c91f173691"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f244dd4c-ee25-4b14-a7cd-a89d47e877b9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B491DB35-4E91-4B2D-816E-03001B21F1D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25588,4 +25983,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C5798F-31D9-455C-A266-3CF2A88C6872}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7d5efbb1-7b5c-4600-961f-d0c91f173691"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f244dd4c-ee25-4b14-a7cd-a89d47e877b9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixing bugs with country profiles.
</commit_message>
<xml_diff>
--- a/inst/extdata/country_summary_template.xlsx
+++ b/inst/extdata/country_summary_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E619F946-F12A-4339-88EB-31CFF4E5BCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821865C4-6BCC-40F0-87D8-FEC06A49DF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32280" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="942" activeTab="10" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
   </bookViews>
@@ -3472,33 +3472,51 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="51" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3542,18 +3560,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="54" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3564,6 +3570,18 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3573,39 +3591,39 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3616,24 +3634,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -4320,7 +4320,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96F0638F-1245-47F5-8417-DE53DC2661A6}" type="CELLRANGE">
+                    <a:fld id="{273E43D1-B923-46B6-B3F9-41785F46D2C4}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4381,7 +4381,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B3FDDFC-C16C-4FCC-BDDD-EB2AD621F4DD}" type="CELLRANGE">
+                    <a:fld id="{D8C54C63-C72C-4E18-BBE9-1DCA140C0641}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4442,7 +4442,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D68425C9-9B0A-4A91-9CBA-B8D93EF93917}" type="CELLRANGE">
+                    <a:fld id="{B4AC9CE7-6D59-43AC-8A85-D22BFCE38275}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4476,7 +4476,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{93A84D4D-2BFB-42AC-A453-7B186AB3F110}" type="CELLRANGE">
+                    <a:fld id="{022A63E5-4B81-4FFF-B8AE-7CC705ED2F77}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4537,7 +4537,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2BCE8849-AFBD-4A99-B884-5A061EA80D21}" type="CELLRANGE">
+                    <a:fld id="{E3FD1B56-D120-4286-955A-54FDCB02EC6B}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4571,7 +4571,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA18073F-77C5-4768-A025-E81B44830825}" type="CELLRANGE">
+                    <a:fld id="{2D3DB64D-CED0-4DEC-98BF-A08BB7EFC82D}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4605,7 +4605,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E58FFA3-A599-46CA-9812-E203D746FBC2}" type="CELLRANGE">
+                    <a:fld id="{16453298-2DF1-422F-8023-B860B2353A05}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4639,7 +4639,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{20DBE4C2-C0AB-4F59-8A25-AE9532C093E8}" type="CELLRANGE">
+                    <a:fld id="{7D5E3EB6-56FF-4F57-93BD-959FCF5DBE0A}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4673,7 +4673,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06A83D8D-5650-4230-92C3-2C772433DB8F}" type="CELLRANGE">
+                    <a:fld id="{55A9D060-A8FC-4A88-BC02-B7005EB3744B}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4707,7 +4707,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A83B2B8-FACF-46F5-A056-5A6DC68F243A}" type="CELLRANGE">
+                    <a:fld id="{7C0FD6D9-08E3-4784-884B-E99DA59B2AC4}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4741,7 +4741,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4488E5B4-6324-44EA-A3B6-9C725A858E25}" type="CELLRANGE">
+                    <a:fld id="{87C7436E-1CDF-40D0-B47D-7B00153CDE6C}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6503,7 +6503,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67C29468-A71E-4533-B15A-8359B3C3D8CC}" type="CELLRANGE">
+                    <a:fld id="{051DB302-85CC-4053-94CD-006C252E4151}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6564,7 +6564,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B4C3EE9-E309-469E-9829-E96CB3F7F620}" type="CELLRANGE">
+                    <a:fld id="{1E0761D2-A119-46B7-A314-F866DEDC61C5}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6625,7 +6625,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{952E52CA-64ED-4AF6-99CF-D08E79820FDE}" type="CELLRANGE">
+                    <a:fld id="{094C8B86-3E18-4C78-AFE0-FE5BA96D6244}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6659,7 +6659,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B0F4639-CF87-4C48-8124-79DBDE11B530}" type="CELLRANGE">
+                    <a:fld id="{B3619F6D-1868-494D-BEF5-A0695E6254F6}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6720,7 +6720,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6490242A-4956-4A80-96BF-0036685F0F8A}" type="CELLRANGE">
+                    <a:fld id="{1DA55DDA-3494-4C3E-A3DE-EDBE8D7961CC}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6754,7 +6754,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C6AE29F-9509-4D9B-AB68-4DB77C93C6C8}" type="CELLRANGE">
+                    <a:fld id="{2D7904EB-F7EC-4C04-910B-B0841945A71E}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6788,7 +6788,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3BAACF6-61EF-48BC-AD9C-F14715BAFAAC}" type="CELLRANGE">
+                    <a:fld id="{B4CF9563-58A2-4DBB-A7BF-8173BE1F21DE}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6822,7 +6822,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD401514-8865-416B-99AD-9A2F0FB35517}" type="CELLRANGE">
+                    <a:fld id="{016F2508-3332-4213-BD03-BC7F9D2D07CD}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6856,7 +6856,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1CCE6139-8C4D-4B39-82A2-9D63AB1F8966}" type="CELLRANGE">
+                    <a:fld id="{8D06C226-FE69-45AE-A3C4-D2638C23FD99}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6890,7 +6890,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C26E091-1126-49AC-8A75-C35CEC9A6FE8}" type="CELLRANGE">
+                    <a:fld id="{982B213A-610B-46BB-A32B-9B32ACE254A6}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6924,7 +6924,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{615374FC-BCE5-4906-B8EF-4DD963C844AD}" type="CELLRANGE">
+                    <a:fld id="{10C757B8-BE68-41FE-A230-FA47004B1F47}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6958,7 +6958,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EDC3C98C-AD2D-4EFC-8F1B-7FC87771A82C}" type="CELLRANGE">
+                    <a:fld id="{FC69992C-7E4F-4E75-9975-251B84CACA32}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6992,7 +6992,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6EDBA6FE-F926-4B08-803E-A0AA2177A877}" type="CELLRANGE">
+                    <a:fld id="{E216B47D-39F5-4ABA-8CFA-8927E6F2AC55}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8897,74 +8897,74 @@
   <sheetData>
     <row r="1" spans="2:15" ht="10.5" customHeight="1"/>
     <row r="2" spans="2:15" ht="36" customHeight="1">
-      <c r="B2" s="318" t="s">
+      <c r="B2" s="321" t="s">
         <v>339</v>
       </c>
-      <c r="C2" s="318"/>
-      <c r="D2" s="318"/>
-      <c r="E2" s="318"/>
-      <c r="F2" s="318"/>
-      <c r="G2" s="318"/>
-      <c r="H2" s="318"/>
-      <c r="I2" s="318"/>
-      <c r="J2" s="318"/>
-      <c r="K2" s="318"/>
-      <c r="L2" s="318"/>
-      <c r="M2" s="318"/>
+      <c r="C2" s="321"/>
+      <c r="D2" s="321"/>
+      <c r="E2" s="321"/>
+      <c r="F2" s="321"/>
+      <c r="G2" s="321"/>
+      <c r="H2" s="321"/>
+      <c r="I2" s="321"/>
+      <c r="J2" s="321"/>
+      <c r="K2" s="321"/>
+      <c r="L2" s="321"/>
+      <c r="M2" s="321"/>
       <c r="N2" s="62"/>
       <c r="O2" s="62"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1">
-      <c r="B3" s="319" t="s">
+      <c r="B3" s="322" t="s">
         <v>437</v>
       </c>
-      <c r="C3" s="319"/>
-      <c r="D3" s="319"/>
-      <c r="E3" s="319"/>
-      <c r="F3" s="319"/>
-      <c r="G3" s="319"/>
-      <c r="H3" s="319"/>
-      <c r="I3" s="319"/>
-      <c r="J3" s="319"/>
-      <c r="K3" s="319"/>
-      <c r="L3" s="319"/>
-      <c r="M3" s="319"/>
+      <c r="C3" s="322"/>
+      <c r="D3" s="322"/>
+      <c r="E3" s="322"/>
+      <c r="F3" s="322"/>
+      <c r="G3" s="322"/>
+      <c r="H3" s="322"/>
+      <c r="I3" s="322"/>
+      <c r="J3" s="322"/>
+      <c r="K3" s="322"/>
+      <c r="L3" s="322"/>
+      <c r="M3" s="322"/>
       <c r="N3" s="201"/>
       <c r="O3" s="201"/>
     </row>
     <row r="4" spans="2:15" ht="18.75" customHeight="1">
-      <c r="B4" s="315" t="s">
+      <c r="B4" s="318" t="s">
         <v>340</v>
       </c>
-      <c r="C4" s="315"/>
-      <c r="D4" s="315"/>
-      <c r="E4" s="315"/>
-      <c r="F4" s="315"/>
-      <c r="G4" s="315"/>
-      <c r="H4" s="315"/>
-      <c r="I4" s="315"/>
-      <c r="J4" s="315"/>
-      <c r="K4" s="315"/>
-      <c r="L4" s="315"/>
-      <c r="M4" s="315"/>
+      <c r="C4" s="318"/>
+      <c r="D4" s="318"/>
+      <c r="E4" s="318"/>
+      <c r="F4" s="318"/>
+      <c r="G4" s="318"/>
+      <c r="H4" s="318"/>
+      <c r="I4" s="318"/>
+      <c r="J4" s="318"/>
+      <c r="K4" s="318"/>
+      <c r="L4" s="318"/>
+      <c r="M4" s="318"/>
       <c r="N4" s="202"/>
       <c r="O4" s="202"/>
     </row>
     <row r="5" spans="2:15" ht="15" customHeight="1">
-      <c r="B5" s="312" t="s">
+      <c r="B5" s="319" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="312"/>
-      <c r="D5" s="312"/>
-      <c r="E5" s="312"/>
-      <c r="F5" s="312"/>
-      <c r="G5" s="312"/>
-      <c r="H5" s="312"/>
-      <c r="I5" s="312"/>
-      <c r="J5" s="312"/>
-      <c r="K5" s="312"/>
-      <c r="L5" s="312"/>
-      <c r="M5" s="312"/>
+      <c r="C5" s="319"/>
+      <c r="D5" s="319"/>
+      <c r="E5" s="319"/>
+      <c r="F5" s="319"/>
+      <c r="G5" s="319"/>
+      <c r="H5" s="319"/>
+      <c r="I5" s="319"/>
+      <c r="J5" s="319"/>
+      <c r="K5" s="319"/>
+      <c r="L5" s="319"/>
+      <c r="M5" s="319"/>
       <c r="N5" s="201"/>
       <c r="O5" s="201"/>
     </row>
@@ -9023,71 +9023,71 @@
       <c r="O8" s="203"/>
     </row>
     <row r="9" spans="2:15" ht="30" customHeight="1">
-      <c r="B9" s="312" t="s">
+      <c r="B9" s="319" t="s">
         <v>341</v>
       </c>
-      <c r="C9" s="312"/>
-      <c r="D9" s="312"/>
-      <c r="E9" s="312"/>
-      <c r="F9" s="312"/>
-      <c r="G9" s="312"/>
-      <c r="H9" s="312"/>
-      <c r="I9" s="312"/>
-      <c r="J9" s="312"/>
-      <c r="K9" s="312"/>
-      <c r="L9" s="312"/>
+      <c r="C9" s="319"/>
+      <c r="D9" s="319"/>
+      <c r="E9" s="319"/>
+      <c r="F9" s="319"/>
+      <c r="G9" s="319"/>
+      <c r="H9" s="319"/>
+      <c r="I9" s="319"/>
+      <c r="J9" s="319"/>
+      <c r="K9" s="319"/>
+      <c r="L9" s="319"/>
     </row>
     <row r="10" spans="2:15" ht="33.75" customHeight="1">
-      <c r="B10" s="312" t="s">
+      <c r="B10" s="319" t="s">
         <v>342</v>
       </c>
-      <c r="C10" s="312"/>
-      <c r="D10" s="312"/>
-      <c r="E10" s="312"/>
-      <c r="F10" s="312"/>
-      <c r="G10" s="312"/>
-      <c r="H10" s="312"/>
-      <c r="I10" s="312"/>
-      <c r="J10" s="312"/>
-      <c r="K10" s="312"/>
-      <c r="L10" s="312"/>
+      <c r="C10" s="319"/>
+      <c r="D10" s="319"/>
+      <c r="E10" s="319"/>
+      <c r="F10" s="319"/>
+      <c r="G10" s="319"/>
+      <c r="H10" s="319"/>
+      <c r="I10" s="319"/>
+      <c r="J10" s="319"/>
+      <c r="K10" s="319"/>
+      <c r="L10" s="319"/>
     </row>
     <row r="11" spans="2:15" ht="21" customHeight="1">
-      <c r="B11" s="315" t="s">
+      <c r="B11" s="318" t="s">
         <v>343</v>
       </c>
-      <c r="C11" s="315"/>
-      <c r="D11" s="315"/>
-      <c r="E11" s="315"/>
-      <c r="F11" s="315"/>
-      <c r="G11" s="315"/>
-      <c r="H11" s="315"/>
-      <c r="I11" s="315"/>
-      <c r="J11" s="315"/>
-      <c r="K11" s="315"/>
-      <c r="L11" s="315"/>
-      <c r="M11" s="315"/>
+      <c r="C11" s="318"/>
+      <c r="D11" s="318"/>
+      <c r="E11" s="318"/>
+      <c r="F11" s="318"/>
+      <c r="G11" s="318"/>
+      <c r="H11" s="318"/>
+      <c r="I11" s="318"/>
+      <c r="J11" s="318"/>
+      <c r="K11" s="318"/>
+      <c r="L11" s="318"/>
+      <c r="M11" s="318"/>
       <c r="N11" s="63"/>
       <c r="O11" s="63"/>
     </row>
     <row r="12" spans="2:15">
-      <c r="B12" s="312" t="s">
+      <c r="B12" s="319" t="s">
         <v>344</v>
       </c>
-      <c r="C12" s="312"/>
-      <c r="D12" s="312"/>
-      <c r="E12" s="312"/>
-      <c r="F12" s="312"/>
-      <c r="G12" s="312"/>
-      <c r="H12" s="312"/>
-      <c r="I12" s="312"/>
-      <c r="J12" s="312"/>
-      <c r="K12" s="312"/>
-      <c r="L12" s="312"/>
-      <c r="M12" s="312"/>
+      <c r="C12" s="319"/>
+      <c r="D12" s="319"/>
+      <c r="E12" s="319"/>
+      <c r="F12" s="319"/>
+      <c r="G12" s="319"/>
+      <c r="H12" s="319"/>
+      <c r="I12" s="319"/>
+      <c r="J12" s="319"/>
+      <c r="K12" s="319"/>
+      <c r="L12" s="319"/>
+      <c r="M12" s="319"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="B13" s="316" t="s">
+      <c r="B13" s="320" t="s">
         <v>369</v>
       </c>
       <c r="C13" s="317"/>
@@ -9103,7 +9103,7 @@
       <c r="M13" s="317"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="B14" s="316" t="s">
+      <c r="B14" s="320" t="s">
         <v>370</v>
       </c>
       <c r="C14" s="317"/>
@@ -9119,7 +9119,7 @@
       <c r="M14" s="317"/>
     </row>
     <row r="15" spans="2:15" ht="17.25" customHeight="1">
-      <c r="B15" s="316" t="s">
+      <c r="B15" s="320" t="s">
         <v>371</v>
       </c>
       <c r="C15" s="317"/>
@@ -9135,183 +9135,183 @@
       <c r="M15" s="317"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="B16" s="312" t="s">
+      <c r="B16" s="319" t="s">
         <v>368</v>
       </c>
-      <c r="C16" s="312"/>
-      <c r="D16" s="312"/>
-      <c r="E16" s="312"/>
-      <c r="F16" s="312"/>
-      <c r="G16" s="312"/>
-      <c r="H16" s="312"/>
-      <c r="I16" s="312"/>
-      <c r="J16" s="312"/>
-      <c r="K16" s="312"/>
-      <c r="L16" s="312"/>
-      <c r="M16" s="312"/>
+      <c r="C16" s="319"/>
+      <c r="D16" s="319"/>
+      <c r="E16" s="319"/>
+      <c r="F16" s="319"/>
+      <c r="G16" s="319"/>
+      <c r="H16" s="319"/>
+      <c r="I16" s="319"/>
+      <c r="J16" s="319"/>
+      <c r="K16" s="319"/>
+      <c r="L16" s="319"/>
+      <c r="M16" s="319"/>
     </row>
     <row r="17" spans="2:13" ht="18">
-      <c r="B17" s="315" t="s">
+      <c r="B17" s="318" t="s">
         <v>345</v>
       </c>
-      <c r="C17" s="315"/>
-      <c r="D17" s="315"/>
-      <c r="E17" s="315"/>
-      <c r="F17" s="315"/>
-      <c r="G17" s="315"/>
-      <c r="H17" s="315"/>
-      <c r="I17" s="315"/>
-      <c r="J17" s="315"/>
-      <c r="K17" s="315"/>
-      <c r="L17" s="315"/>
-      <c r="M17" s="315"/>
+      <c r="C17" s="318"/>
+      <c r="D17" s="318"/>
+      <c r="E17" s="318"/>
+      <c r="F17" s="318"/>
+      <c r="G17" s="318"/>
+      <c r="H17" s="318"/>
+      <c r="I17" s="318"/>
+      <c r="J17" s="318"/>
+      <c r="K17" s="318"/>
+      <c r="L17" s="318"/>
+      <c r="M17" s="318"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="312" t="s">
+      <c r="B18" s="319" t="s">
         <v>346</v>
       </c>
-      <c r="C18" s="312"/>
-      <c r="D18" s="312"/>
-      <c r="E18" s="312"/>
-      <c r="F18" s="312"/>
-      <c r="G18" s="312"/>
-      <c r="H18" s="312"/>
-      <c r="I18" s="312"/>
-      <c r="J18" s="312"/>
-      <c r="K18" s="312"/>
-      <c r="L18" s="312"/>
-      <c r="M18" s="312"/>
+      <c r="C18" s="319"/>
+      <c r="D18" s="319"/>
+      <c r="E18" s="319"/>
+      <c r="F18" s="319"/>
+      <c r="G18" s="319"/>
+      <c r="H18" s="319"/>
+      <c r="I18" s="319"/>
+      <c r="J18" s="319"/>
+      <c r="K18" s="319"/>
+      <c r="L18" s="319"/>
+      <c r="M18" s="319"/>
     </row>
     <row r="19" spans="2:13" ht="14.4" customHeight="1">
       <c r="B19" s="259"/>
-      <c r="C19" s="311" t="s">
+      <c r="C19" s="323" t="s">
         <v>364</v>
       </c>
-      <c r="D19" s="311"/>
-      <c r="E19" s="311"/>
-      <c r="F19" s="311"/>
-      <c r="G19" s="311"/>
-      <c r="H19" s="311"/>
-      <c r="I19" s="311"/>
-      <c r="J19" s="311"/>
-      <c r="K19" s="311"/>
-      <c r="L19" s="311"/>
-      <c r="M19" s="311"/>
+      <c r="D19" s="323"/>
+      <c r="E19" s="323"/>
+      <c r="F19" s="323"/>
+      <c r="G19" s="323"/>
+      <c r="H19" s="323"/>
+      <c r="I19" s="323"/>
+      <c r="J19" s="323"/>
+      <c r="K19" s="323"/>
+      <c r="L19" s="323"/>
+      <c r="M19" s="323"/>
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="259"/>
-      <c r="C20" s="311" t="s">
+      <c r="C20" s="323" t="s">
         <v>365</v>
       </c>
-      <c r="D20" s="311"/>
-      <c r="E20" s="311"/>
-      <c r="F20" s="311"/>
-      <c r="G20" s="311"/>
-      <c r="H20" s="311"/>
-      <c r="I20" s="311"/>
-      <c r="J20" s="311"/>
-      <c r="K20" s="311"/>
-      <c r="L20" s="311"/>
-      <c r="M20" s="311"/>
+      <c r="D20" s="323"/>
+      <c r="E20" s="323"/>
+      <c r="F20" s="323"/>
+      <c r="G20" s="323"/>
+      <c r="H20" s="323"/>
+      <c r="I20" s="323"/>
+      <c r="J20" s="323"/>
+      <c r="K20" s="323"/>
+      <c r="L20" s="323"/>
+      <c r="M20" s="323"/>
     </row>
     <row r="21" spans="2:13" ht="14.4" customHeight="1">
       <c r="B21" s="259"/>
-      <c r="C21" s="311" t="s">
+      <c r="C21" s="323" t="s">
         <v>464</v>
       </c>
-      <c r="D21" s="311"/>
-      <c r="E21" s="311"/>
-      <c r="F21" s="311"/>
-      <c r="G21" s="311"/>
-      <c r="H21" s="311"/>
-      <c r="I21" s="311"/>
-      <c r="J21" s="311"/>
-      <c r="K21" s="311"/>
-      <c r="L21" s="311"/>
-      <c r="M21" s="311"/>
+      <c r="D21" s="323"/>
+      <c r="E21" s="323"/>
+      <c r="F21" s="323"/>
+      <c r="G21" s="323"/>
+      <c r="H21" s="323"/>
+      <c r="I21" s="323"/>
+      <c r="J21" s="323"/>
+      <c r="K21" s="323"/>
+      <c r="L21" s="323"/>
+      <c r="M21" s="323"/>
     </row>
     <row r="22" spans="2:13">
       <c r="B22" s="259"/>
-      <c r="C22" s="311" t="s">
+      <c r="C22" s="323" t="s">
         <v>460</v>
       </c>
-      <c r="D22" s="311"/>
-      <c r="E22" s="311"/>
-      <c r="F22" s="311"/>
-      <c r="G22" s="311"/>
-      <c r="H22" s="311"/>
-      <c r="I22" s="311"/>
-      <c r="J22" s="311"/>
-      <c r="K22" s="311"/>
-      <c r="L22" s="311"/>
-      <c r="M22" s="311"/>
+      <c r="D22" s="323"/>
+      <c r="E22" s="323"/>
+      <c r="F22" s="323"/>
+      <c r="G22" s="323"/>
+      <c r="H22" s="323"/>
+      <c r="I22" s="323"/>
+      <c r="J22" s="323"/>
+      <c r="K22" s="323"/>
+      <c r="L22" s="323"/>
+      <c r="M22" s="323"/>
     </row>
     <row r="23" spans="2:13" ht="14.4" customHeight="1">
       <c r="B23" s="259"/>
       <c r="C23" s="259"/>
-      <c r="D23" s="311" t="s">
+      <c r="D23" s="323" t="s">
         <v>456</v>
       </c>
-      <c r="E23" s="311"/>
-      <c r="F23" s="311"/>
-      <c r="G23" s="311"/>
-      <c r="H23" s="311"/>
-      <c r="I23" s="311"/>
-      <c r="J23" s="311"/>
-      <c r="K23" s="311"/>
-      <c r="L23" s="311"/>
-      <c r="M23" s="311"/>
+      <c r="E23" s="323"/>
+      <c r="F23" s="323"/>
+      <c r="G23" s="323"/>
+      <c r="H23" s="323"/>
+      <c r="I23" s="323"/>
+      <c r="J23" s="323"/>
+      <c r="K23" s="323"/>
+      <c r="L23" s="323"/>
+      <c r="M23" s="323"/>
     </row>
     <row r="24" spans="2:13" ht="14.4" customHeight="1">
       <c r="B24" s="259"/>
       <c r="C24" s="259"/>
-      <c r="D24" s="311" t="s">
+      <c r="D24" s="323" t="s">
         <v>457</v>
       </c>
-      <c r="E24" s="311"/>
-      <c r="F24" s="311"/>
-      <c r="G24" s="311"/>
-      <c r="H24" s="311"/>
-      <c r="I24" s="311"/>
-      <c r="J24" s="311"/>
-      <c r="K24" s="311"/>
-      <c r="L24" s="311"/>
-      <c r="M24" s="311"/>
+      <c r="E24" s="323"/>
+      <c r="F24" s="323"/>
+      <c r="G24" s="323"/>
+      <c r="H24" s="323"/>
+      <c r="I24" s="323"/>
+      <c r="J24" s="323"/>
+      <c r="K24" s="323"/>
+      <c r="L24" s="323"/>
+      <c r="M24" s="323"/>
     </row>
     <row r="25" spans="2:13">
       <c r="B25" s="256"/>
       <c r="C25" s="257"/>
-      <c r="D25" s="312" t="s">
+      <c r="D25" s="319" t="s">
         <v>458</v>
       </c>
-      <c r="E25" s="312"/>
-      <c r="F25" s="312"/>
-      <c r="G25" s="312"/>
-      <c r="H25" s="312"/>
-      <c r="I25" s="312"/>
-      <c r="J25" s="312"/>
-      <c r="K25" s="312"/>
-      <c r="L25" s="312"/>
-      <c r="M25" s="312"/>
+      <c r="E25" s="319"/>
+      <c r="F25" s="319"/>
+      <c r="G25" s="319"/>
+      <c r="H25" s="319"/>
+      <c r="I25" s="319"/>
+      <c r="J25" s="319"/>
+      <c r="K25" s="319"/>
+      <c r="L25" s="319"/>
+      <c r="M25" s="319"/>
     </row>
     <row r="26" spans="2:13">
       <c r="B26" s="256"/>
       <c r="C26" s="257"/>
-      <c r="D26" s="311" t="s">
+      <c r="D26" s="323" t="s">
         <v>459</v>
       </c>
-      <c r="E26" s="311"/>
-      <c r="F26" s="311"/>
-      <c r="G26" s="311"/>
-      <c r="H26" s="311"/>
-      <c r="I26" s="311"/>
-      <c r="J26" s="311"/>
-      <c r="K26" s="311"/>
-      <c r="L26" s="311"/>
-      <c r="M26" s="311"/>
+      <c r="E26" s="323"/>
+      <c r="F26" s="323"/>
+      <c r="G26" s="323"/>
+      <c r="H26" s="323"/>
+      <c r="I26" s="323"/>
+      <c r="J26" s="323"/>
+      <c r="K26" s="323"/>
+      <c r="L26" s="323"/>
+      <c r="M26" s="323"/>
     </row>
     <row r="27" spans="2:13" ht="15" customHeight="1">
-      <c r="B27" s="316" t="s">
+      <c r="B27" s="320" t="s">
         <v>366</v>
       </c>
       <c r="C27" s="317"/>
@@ -9327,7 +9327,7 @@
       <c r="M27" s="317"/>
     </row>
     <row r="28" spans="2:13" ht="15" customHeight="1">
-      <c r="B28" s="316" t="s">
+      <c r="B28" s="320" t="s">
         <v>367</v>
       </c>
       <c r="C28" s="317"/>
@@ -9346,215 +9346,215 @@
       <c r="B29" s="200"/>
     </row>
     <row r="30" spans="2:13" ht="18">
-      <c r="B30" s="315" t="s">
+      <c r="B30" s="318" t="s">
         <v>347</v>
       </c>
-      <c r="C30" s="315"/>
-      <c r="D30" s="315"/>
-      <c r="E30" s="315"/>
-      <c r="F30" s="315"/>
-      <c r="G30" s="315"/>
-      <c r="H30" s="315"/>
-      <c r="I30" s="315"/>
-      <c r="J30" s="315"/>
-      <c r="K30" s="315"/>
-      <c r="L30" s="315"/>
-      <c r="M30" s="315"/>
+      <c r="C30" s="318"/>
+      <c r="D30" s="318"/>
+      <c r="E30" s="318"/>
+      <c r="F30" s="318"/>
+      <c r="G30" s="318"/>
+      <c r="H30" s="318"/>
+      <c r="I30" s="318"/>
+      <c r="J30" s="318"/>
+      <c r="K30" s="318"/>
+      <c r="L30" s="318"/>
+      <c r="M30" s="318"/>
     </row>
     <row r="31" spans="2:13" ht="15" customHeight="1">
-      <c r="B31" s="312" t="s">
+      <c r="B31" s="319" t="s">
         <v>372</v>
       </c>
-      <c r="C31" s="312"/>
-      <c r="D31" s="312"/>
-      <c r="E31" s="312"/>
-      <c r="F31" s="312"/>
-      <c r="G31" s="312"/>
-      <c r="H31" s="312"/>
-      <c r="I31" s="312"/>
-      <c r="J31" s="312"/>
-      <c r="K31" s="312"/>
-      <c r="L31" s="312"/>
-      <c r="M31" s="312"/>
+      <c r="C31" s="319"/>
+      <c r="D31" s="319"/>
+      <c r="E31" s="319"/>
+      <c r="F31" s="319"/>
+      <c r="G31" s="319"/>
+      <c r="H31" s="319"/>
+      <c r="I31" s="319"/>
+      <c r="J31" s="319"/>
+      <c r="K31" s="319"/>
+      <c r="L31" s="319"/>
+      <c r="M31" s="319"/>
     </row>
     <row r="32" spans="2:13" ht="31.5" customHeight="1">
-      <c r="B32" s="312" t="s">
+      <c r="B32" s="319" t="s">
         <v>348</v>
       </c>
-      <c r="C32" s="312"/>
-      <c r="D32" s="312"/>
-      <c r="E32" s="312"/>
-      <c r="F32" s="312"/>
-      <c r="G32" s="312"/>
-      <c r="H32" s="312"/>
-      <c r="I32" s="312"/>
-      <c r="J32" s="312"/>
-      <c r="K32" s="312"/>
-      <c r="L32" s="312"/>
-      <c r="M32" s="312"/>
+      <c r="C32" s="319"/>
+      <c r="D32" s="319"/>
+      <c r="E32" s="319"/>
+      <c r="F32" s="319"/>
+      <c r="G32" s="319"/>
+      <c r="H32" s="319"/>
+      <c r="I32" s="319"/>
+      <c r="J32" s="319"/>
+      <c r="K32" s="319"/>
+      <c r="L32" s="319"/>
+      <c r="M32" s="319"/>
     </row>
     <row r="33" spans="2:13" ht="28.5" customHeight="1">
-      <c r="B33" s="312" t="s">
+      <c r="B33" s="319" t="s">
         <v>349</v>
       </c>
-      <c r="C33" s="312"/>
-      <c r="D33" s="312"/>
-      <c r="E33" s="312"/>
-      <c r="F33" s="312"/>
-      <c r="G33" s="312"/>
-      <c r="H33" s="312"/>
-      <c r="I33" s="312"/>
-      <c r="J33" s="312"/>
-      <c r="K33" s="312"/>
-      <c r="L33" s="312"/>
-      <c r="M33" s="312"/>
+      <c r="C33" s="319"/>
+      <c r="D33" s="319"/>
+      <c r="E33" s="319"/>
+      <c r="F33" s="319"/>
+      <c r="G33" s="319"/>
+      <c r="H33" s="319"/>
+      <c r="I33" s="319"/>
+      <c r="J33" s="319"/>
+      <c r="K33" s="319"/>
+      <c r="L33" s="319"/>
+      <c r="M33" s="319"/>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="312" t="s">
+      <c r="B34" s="319" t="s">
         <v>350</v>
       </c>
-      <c r="C34" s="312"/>
-      <c r="D34" s="312"/>
-      <c r="E34" s="312"/>
-      <c r="F34" s="312"/>
-      <c r="G34" s="312"/>
-      <c r="H34" s="312"/>
-      <c r="I34" s="312"/>
-      <c r="J34" s="312"/>
-      <c r="K34" s="312"/>
-      <c r="L34" s="312"/>
-      <c r="M34" s="312"/>
+      <c r="C34" s="319"/>
+      <c r="D34" s="319"/>
+      <c r="E34" s="319"/>
+      <c r="F34" s="319"/>
+      <c r="G34" s="319"/>
+      <c r="H34" s="319"/>
+      <c r="I34" s="319"/>
+      <c r="J34" s="319"/>
+      <c r="K34" s="319"/>
+      <c r="L34" s="319"/>
+      <c r="M34" s="319"/>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="312" t="s">
+      <c r="B35" s="319" t="s">
         <v>351</v>
       </c>
-      <c r="C35" s="312"/>
-      <c r="D35" s="312"/>
-      <c r="E35" s="312"/>
-      <c r="F35" s="312"/>
-      <c r="G35" s="312"/>
-      <c r="H35" s="312"/>
-      <c r="I35" s="312"/>
-      <c r="J35" s="312"/>
-      <c r="K35" s="312"/>
-      <c r="L35" s="312"/>
-      <c r="M35" s="312"/>
+      <c r="C35" s="319"/>
+      <c r="D35" s="319"/>
+      <c r="E35" s="319"/>
+      <c r="F35" s="319"/>
+      <c r="G35" s="319"/>
+      <c r="H35" s="319"/>
+      <c r="I35" s="319"/>
+      <c r="J35" s="319"/>
+      <c r="K35" s="319"/>
+      <c r="L35" s="319"/>
+      <c r="M35" s="319"/>
     </row>
     <row r="36" spans="2:13" ht="18">
-      <c r="B36" s="315" t="s">
+      <c r="B36" s="318" t="s">
         <v>352</v>
       </c>
-      <c r="C36" s="315"/>
-      <c r="D36" s="315"/>
-      <c r="E36" s="315"/>
-      <c r="F36" s="315"/>
-      <c r="G36" s="315"/>
-      <c r="H36" s="315"/>
-      <c r="I36" s="315"/>
-      <c r="J36" s="315"/>
-      <c r="K36" s="315"/>
-      <c r="L36" s="315"/>
-      <c r="M36" s="315"/>
+      <c r="C36" s="318"/>
+      <c r="D36" s="318"/>
+      <c r="E36" s="318"/>
+      <c r="F36" s="318"/>
+      <c r="G36" s="318"/>
+      <c r="H36" s="318"/>
+      <c r="I36" s="318"/>
+      <c r="J36" s="318"/>
+      <c r="K36" s="318"/>
+      <c r="L36" s="318"/>
+      <c r="M36" s="318"/>
     </row>
     <row r="37" spans="2:13" ht="30.75" customHeight="1">
-      <c r="B37" s="312" t="s">
+      <c r="B37" s="319" t="s">
         <v>353</v>
       </c>
-      <c r="C37" s="312"/>
-      <c r="D37" s="312"/>
-      <c r="E37" s="312"/>
-      <c r="F37" s="312"/>
-      <c r="G37" s="312"/>
-      <c r="H37" s="312"/>
-      <c r="I37" s="312"/>
-      <c r="J37" s="312"/>
-      <c r="K37" s="312"/>
-      <c r="L37" s="312"/>
-      <c r="M37" s="312"/>
+      <c r="C37" s="319"/>
+      <c r="D37" s="319"/>
+      <c r="E37" s="319"/>
+      <c r="F37" s="319"/>
+      <c r="G37" s="319"/>
+      <c r="H37" s="319"/>
+      <c r="I37" s="319"/>
+      <c r="J37" s="319"/>
+      <c r="K37" s="319"/>
+      <c r="L37" s="319"/>
+      <c r="M37" s="319"/>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="312" t="s">
+      <c r="B38" s="319" t="s">
         <v>354</v>
       </c>
-      <c r="C38" s="312"/>
-      <c r="D38" s="312"/>
-      <c r="E38" s="312"/>
-      <c r="F38" s="312"/>
-      <c r="G38" s="312"/>
-      <c r="H38" s="312"/>
-      <c r="I38" s="312"/>
-      <c r="J38" s="312"/>
-      <c r="K38" s="312"/>
-      <c r="L38" s="312"/>
-      <c r="M38" s="312"/>
+      <c r="C38" s="319"/>
+      <c r="D38" s="319"/>
+      <c r="E38" s="319"/>
+      <c r="F38" s="319"/>
+      <c r="G38" s="319"/>
+      <c r="H38" s="319"/>
+      <c r="I38" s="319"/>
+      <c r="J38" s="319"/>
+      <c r="K38" s="319"/>
+      <c r="L38" s="319"/>
+      <c r="M38" s="319"/>
     </row>
     <row r="39" spans="2:13">
       <c r="B39" s="200"/>
     </row>
     <row r="40" spans="2:13" ht="18">
-      <c r="B40" s="315" t="s">
+      <c r="B40" s="318" t="s">
         <v>355</v>
       </c>
-      <c r="C40" s="315"/>
-      <c r="D40" s="315"/>
-      <c r="E40" s="315"/>
-      <c r="F40" s="315"/>
-      <c r="G40" s="315"/>
-      <c r="H40" s="315"/>
-      <c r="I40" s="315"/>
-      <c r="J40" s="315"/>
-      <c r="K40" s="315"/>
-      <c r="L40" s="315"/>
-      <c r="M40" s="315"/>
+      <c r="C40" s="318"/>
+      <c r="D40" s="318"/>
+      <c r="E40" s="318"/>
+      <c r="F40" s="318"/>
+      <c r="G40" s="318"/>
+      <c r="H40" s="318"/>
+      <c r="I40" s="318"/>
+      <c r="J40" s="318"/>
+      <c r="K40" s="318"/>
+      <c r="L40" s="318"/>
+      <c r="M40" s="318"/>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="314" t="s">
+      <c r="B41" s="325" t="s">
         <v>356</v>
       </c>
-      <c r="C41" s="314"/>
-      <c r="D41" s="314"/>
-      <c r="E41" s="314"/>
-      <c r="F41" s="314"/>
-      <c r="G41" s="314"/>
-      <c r="H41" s="314"/>
-      <c r="I41" s="314"/>
-      <c r="J41" s="314"/>
-      <c r="K41" s="314"/>
-      <c r="L41" s="314"/>
-      <c r="M41" s="314"/>
+      <c r="C41" s="325"/>
+      <c r="D41" s="325"/>
+      <c r="E41" s="325"/>
+      <c r="F41" s="325"/>
+      <c r="G41" s="325"/>
+      <c r="H41" s="325"/>
+      <c r="I41" s="325"/>
+      <c r="J41" s="325"/>
+      <c r="K41" s="325"/>
+      <c r="L41" s="325"/>
+      <c r="M41" s="325"/>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="314" t="s">
+      <c r="B42" s="325" t="s">
         <v>357</v>
       </c>
-      <c r="C42" s="314"/>
-      <c r="D42" s="314"/>
-      <c r="E42" s="314"/>
-      <c r="F42" s="314"/>
-      <c r="G42" s="314"/>
-      <c r="H42" s="314"/>
-      <c r="I42" s="314"/>
-      <c r="J42" s="314"/>
-      <c r="K42" s="314"/>
-      <c r="L42" s="314"/>
-      <c r="M42" s="314"/>
+      <c r="C42" s="325"/>
+      <c r="D42" s="325"/>
+      <c r="E42" s="325"/>
+      <c r="F42" s="325"/>
+      <c r="G42" s="325"/>
+      <c r="H42" s="325"/>
+      <c r="I42" s="325"/>
+      <c r="J42" s="325"/>
+      <c r="K42" s="325"/>
+      <c r="L42" s="325"/>
+      <c r="M42" s="325"/>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="314" t="s">
+      <c r="B43" s="325" t="s">
         <v>358</v>
       </c>
-      <c r="C43" s="314"/>
-      <c r="D43" s="314"/>
-      <c r="E43" s="314"/>
-      <c r="F43" s="314"/>
-      <c r="G43" s="314"/>
-      <c r="H43" s="314"/>
-      <c r="I43" s="314"/>
-      <c r="J43" s="314"/>
-      <c r="K43" s="314"/>
-      <c r="L43" s="314"/>
-      <c r="M43" s="314"/>
+      <c r="C43" s="325"/>
+      <c r="D43" s="325"/>
+      <c r="E43" s="325"/>
+      <c r="F43" s="325"/>
+      <c r="G43" s="325"/>
+      <c r="H43" s="325"/>
+      <c r="I43" s="325"/>
+      <c r="J43" s="325"/>
+      <c r="K43" s="325"/>
+      <c r="L43" s="325"/>
+      <c r="M43" s="325"/>
     </row>
     <row r="44" spans="2:13">
       <c r="B44" s="250" t="s">
@@ -9573,82 +9573,55 @@
       <c r="M44" s="248"/>
     </row>
     <row r="45" spans="2:13" ht="18">
-      <c r="B45" s="315" t="s">
+      <c r="B45" s="318" t="s">
         <v>359</v>
       </c>
-      <c r="C45" s="315"/>
-      <c r="D45" s="315"/>
-      <c r="E45" s="315"/>
-      <c r="F45" s="315"/>
-      <c r="G45" s="315"/>
-      <c r="H45" s="315"/>
-      <c r="I45" s="315"/>
-      <c r="J45" s="315"/>
-      <c r="K45" s="315"/>
-      <c r="L45" s="315"/>
-      <c r="M45" s="315"/>
+      <c r="C45" s="318"/>
+      <c r="D45" s="318"/>
+      <c r="E45" s="318"/>
+      <c r="F45" s="318"/>
+      <c r="G45" s="318"/>
+      <c r="H45" s="318"/>
+      <c r="I45" s="318"/>
+      <c r="J45" s="318"/>
+      <c r="K45" s="318"/>
+      <c r="L45" s="318"/>
+      <c r="M45" s="318"/>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="312" t="s">
+      <c r="B46" s="319" t="s">
         <v>463</v>
       </c>
-      <c r="C46" s="312"/>
-      <c r="D46" s="312"/>
-      <c r="E46" s="312"/>
-      <c r="F46" s="312"/>
-      <c r="G46" s="312"/>
-      <c r="H46" s="312"/>
-      <c r="I46" s="312"/>
-      <c r="J46" s="312"/>
-      <c r="K46" s="312"/>
-      <c r="L46" s="312"/>
-      <c r="M46" s="312"/>
+      <c r="C46" s="319"/>
+      <c r="D46" s="319"/>
+      <c r="E46" s="319"/>
+      <c r="F46" s="319"/>
+      <c r="G46" s="319"/>
+      <c r="H46" s="319"/>
+      <c r="I46" s="319"/>
+      <c r="J46" s="319"/>
+      <c r="K46" s="319"/>
+      <c r="L46" s="319"/>
+      <c r="M46" s="319"/>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="313" t="s">
+      <c r="B47" s="324" t="s">
         <v>449</v>
       </c>
-      <c r="C47" s="313"/>
-      <c r="D47" s="313"/>
-      <c r="E47" s="313"/>
-      <c r="F47" s="313"/>
-      <c r="G47" s="313"/>
-      <c r="H47" s="313"/>
-      <c r="I47" s="313"/>
-      <c r="J47" s="313"/>
-      <c r="K47" s="313"/>
-      <c r="L47" s="313"/>
-      <c r="M47" s="313"/>
+      <c r="C47" s="324"/>
+      <c r="D47" s="324"/>
+      <c r="E47" s="324"/>
+      <c r="F47" s="324"/>
+      <c r="G47" s="324"/>
+      <c r="H47" s="324"/>
+      <c r="I47" s="324"/>
+      <c r="J47" s="324"/>
+      <c r="K47" s="324"/>
+      <c r="L47" s="324"/>
+      <c r="M47" s="324"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B8:M8"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B12:M12"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="C21:M21"/>
-    <mergeCell ref="C22:M22"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="B16:M16"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="B18:M18"/>
-    <mergeCell ref="C19:M19"/>
-    <mergeCell ref="C20:M20"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B35:M35"/>
-    <mergeCell ref="B27:M27"/>
-    <mergeCell ref="B28:M28"/>
-    <mergeCell ref="B30:M30"/>
     <mergeCell ref="D23:M23"/>
     <mergeCell ref="D24:M24"/>
     <mergeCell ref="D25:M25"/>
@@ -9665,6 +9638,33 @@
     <mergeCell ref="B41:M41"/>
     <mergeCell ref="B31:M31"/>
     <mergeCell ref="B32:M32"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="B27:M27"/>
+    <mergeCell ref="B28:M28"/>
+    <mergeCell ref="B30:M30"/>
+    <mergeCell ref="C21:M21"/>
+    <mergeCell ref="C22:M22"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="C19:M19"/>
+    <mergeCell ref="C20:M20"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B12:M12"/>
+    <mergeCell ref="B13:M13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B41" r:id="rId1" display="https://cdn.who.int/media/docs/default-source/documents/about-us/thirteenth-general-programme/gpw13_methodology_nov9_online-version1b3170f8-98ea-4fcc-aa3a-059ede7e51ad.pdf?sfvrsn=12dfeb0d_1&amp;download=true" xr:uid="{5B1AD3AB-AC30-4E70-9D4E-7E9B49DF39DD}"/>
@@ -10090,7 +10090,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z35" sqref="Z35"/>
+      <selection pane="topRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -10357,67 +10357,67 @@
       <c r="Z8" s="13"/>
     </row>
     <row r="9" spans="1:32" ht="15" customHeight="1">
-      <c r="A9" s="351" t="s">
+      <c r="A9" s="362" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="351"/>
-      <c r="C9" s="346" t="s">
+      <c r="B9" s="362"/>
+      <c r="C9" s="360" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="346"/>
-      <c r="E9" s="346"/>
-      <c r="F9" s="346"/>
-      <c r="G9" s="346"/>
-      <c r="H9" s="346"/>
-      <c r="I9" s="346"/>
+      <c r="D9" s="360"/>
+      <c r="E9" s="360"/>
+      <c r="F9" s="360"/>
+      <c r="G9" s="360"/>
+      <c r="H9" s="360"/>
+      <c r="I9" s="360"/>
       <c r="J9" s="29"/>
-      <c r="K9" s="347" t="s">
+      <c r="K9" s="361" t="s">
         <v>78</v>
       </c>
-      <c r="L9" s="347"/>
-      <c r="M9" s="347"/>
-      <c r="N9" s="347"/>
-      <c r="O9" s="347"/>
-      <c r="P9" s="347"/>
-      <c r="Q9" s="347"/>
-      <c r="R9" s="347"/>
-      <c r="S9" s="347"/>
-      <c r="T9" s="347"/>
-      <c r="U9" s="347"/>
+      <c r="L9" s="361"/>
+      <c r="M9" s="361"/>
+      <c r="N9" s="361"/>
+      <c r="O9" s="361"/>
+      <c r="P9" s="361"/>
+      <c r="Q9" s="361"/>
+      <c r="R9" s="361"/>
+      <c r="S9" s="361"/>
+      <c r="T9" s="361"/>
+      <c r="U9" s="361"/>
       <c r="V9" s="29"/>
-      <c r="W9" s="353" t="s">
+      <c r="W9" s="357" t="s">
         <v>79</v>
       </c>
-      <c r="X9" s="354"/>
-      <c r="Y9" s="354"/>
-      <c r="Z9" s="355"/>
+      <c r="X9" s="358"/>
+      <c r="Y9" s="358"/>
+      <c r="Z9" s="359"/>
     </row>
     <row r="10" spans="1:32">
-      <c r="A10" s="350" t="s">
+      <c r="A10" s="352" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="350" t="s">
+      <c r="B10" s="352" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="350" t="s">
+      <c r="C10" s="352" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="350" t="s">
+      <c r="D10" s="352" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="350" t="s">
+      <c r="E10" s="352" t="s">
         <v>120</v>
       </c>
-      <c r="F10" s="350" t="s">
+      <c r="F10" s="352" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="350" t="s">
+      <c r="G10" s="352" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="348" t="s">
+      <c r="H10" s="355" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="348" t="s">
+      <c r="I10" s="355" t="s">
         <v>114</v>
       </c>
       <c r="J10" s="30"/>
@@ -10449,29 +10449,29 @@
         <v>82</v>
       </c>
       <c r="V10" s="30"/>
-      <c r="W10" s="352" t="s">
+      <c r="W10" s="354" t="s">
         <v>118</v>
       </c>
-      <c r="X10" s="352" t="s">
+      <c r="X10" s="354" t="s">
         <v>115</v>
       </c>
-      <c r="Y10" s="352" t="s">
+      <c r="Y10" s="354" t="s">
         <v>116</v>
       </c>
-      <c r="Z10" s="350" t="s">
+      <c r="Z10" s="352" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="15" customHeight="1">
-      <c r="A11" s="349"/>
-      <c r="B11" s="349"/>
-      <c r="C11" s="349"/>
-      <c r="D11" s="349"/>
-      <c r="E11" s="349"/>
-      <c r="F11" s="349"/>
-      <c r="G11" s="349"/>
-      <c r="H11" s="349"/>
-      <c r="I11" s="349"/>
+      <c r="A11" s="353"/>
+      <c r="B11" s="353"/>
+      <c r="C11" s="353"/>
+      <c r="D11" s="353"/>
+      <c r="E11" s="353"/>
+      <c r="F11" s="353"/>
+      <c r="G11" s="353"/>
+      <c r="H11" s="353"/>
+      <c r="I11" s="353"/>
       <c r="J11" s="30"/>
       <c r="K11" s="288">
         <v>2018</v>
@@ -10501,10 +10501,10 @@
         <v>2023</v>
       </c>
       <c r="V11" s="30"/>
-      <c r="W11" s="349"/>
-      <c r="X11" s="349"/>
-      <c r="Y11" s="349"/>
-      <c r="Z11" s="349"/>
+      <c r="W11" s="353"/>
+      <c r="X11" s="353"/>
+      <c r="Y11" s="353"/>
+      <c r="Z11" s="353"/>
     </row>
     <row r="12" spans="1:32" s="3" customFormat="1" ht="22.05" customHeight="1">
       <c r="A12" s="289" t="s">
@@ -11687,14 +11687,14 @@
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
       <c r="U30" s="13"/>
-      <c r="W30" s="363" t="s">
+      <c r="W30" s="313" t="s">
         <v>104</v>
       </c>
-      <c r="X30" s="364"/>
-      <c r="Y30" s="361" t="s">
+      <c r="X30" s="314"/>
+      <c r="Y30" s="311" t="s">
         <v>105</v>
       </c>
-      <c r="Z30" s="362"/>
+      <c r="Z30" s="312"/>
     </row>
     <row r="31" spans="1:32" ht="15" customHeight="1">
       <c r="A31" s="45" t="s">
@@ -11721,10 +11721,10 @@
       <c r="T31" s="13"/>
       <c r="U31" s="13"/>
       <c r="V31" s="26"/>
-      <c r="W31" s="365" t="s">
+      <c r="W31" s="315" t="s">
         <v>107</v>
       </c>
-      <c r="X31" s="366"/>
+      <c r="X31" s="316"/>
       <c r="Y31" s="310" t="s">
         <v>126</v>
       </c>
@@ -12269,6 +12269,15 @@
     <row r="76" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="W9:Z9"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="K9:U9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="W10:W11"/>
     <mergeCell ref="X10:X11"/>
@@ -12281,15 +12290,6 @@
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="W9:Z9"/>
-    <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="K9:U9"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <conditionalFormatting sqref="E12:E28">
     <cfRule type="expression" dxfId="1" priority="2">
@@ -12408,35 +12408,35 @@
     </row>
     <row r="4" spans="1:39" ht="15" customHeight="1">
       <c r="A4" s="13"/>
-      <c r="B4" s="358" t="s">
+      <c r="B4" s="364" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="357" t="s">
+      <c r="C4" s="363" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="357"/>
-      <c r="E4" s="357"/>
-      <c r="F4" s="357"/>
-      <c r="G4" s="357"/>
-      <c r="H4" s="357"/>
-      <c r="I4" s="357"/>
-      <c r="J4" s="357"/>
-      <c r="K4" s="357"/>
-      <c r="L4" s="357"/>
-      <c r="M4" s="357"/>
-      <c r="N4" s="357"/>
-      <c r="O4" s="357"/>
-      <c r="P4" s="357"/>
-      <c r="Q4" s="357"/>
-      <c r="R4" s="357"/>
-      <c r="S4" s="357"/>
-      <c r="T4" s="357"/>
-      <c r="U4" s="357"/>
-      <c r="V4" s="357"/>
-      <c r="W4" s="357"/>
-      <c r="X4" s="357"/>
-      <c r="Y4" s="357"/>
-      <c r="Z4" s="357"/>
+      <c r="D4" s="363"/>
+      <c r="E4" s="363"/>
+      <c r="F4" s="363"/>
+      <c r="G4" s="363"/>
+      <c r="H4" s="363"/>
+      <c r="I4" s="363"/>
+      <c r="J4" s="363"/>
+      <c r="K4" s="363"/>
+      <c r="L4" s="363"/>
+      <c r="M4" s="363"/>
+      <c r="N4" s="363"/>
+      <c r="O4" s="363"/>
+      <c r="P4" s="363"/>
+      <c r="Q4" s="363"/>
+      <c r="R4" s="363"/>
+      <c r="S4" s="363"/>
+      <c r="T4" s="363"/>
+      <c r="U4" s="363"/>
+      <c r="V4" s="363"/>
+      <c r="W4" s="363"/>
+      <c r="X4" s="363"/>
+      <c r="Y4" s="363"/>
+      <c r="Z4" s="363"/>
       <c r="AA4" s="13"/>
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
@@ -12453,7 +12453,7 @@
     </row>
     <row r="5" spans="1:39">
       <c r="A5" s="13"/>
-      <c r="B5" s="359"/>
+      <c r="B5" s="365"/>
       <c r="C5" s="241" t="s">
         <v>127</v>
       </c>
@@ -13592,28 +13592,28 @@
       <c r="Z22" s="242"/>
     </row>
     <row r="23" spans="2:26">
-      <c r="B23" s="360"/>
-      <c r="C23" s="360"/>
-      <c r="D23" s="360"/>
-      <c r="E23" s="360"/>
-      <c r="F23" s="360"/>
-      <c r="G23" s="360"/>
-      <c r="H23" s="360"/>
-      <c r="I23" s="360"/>
-      <c r="J23" s="360"/>
-      <c r="K23" s="360"/>
-      <c r="L23" s="360"/>
-      <c r="M23" s="360"/>
-      <c r="N23" s="360"/>
-      <c r="O23" s="360"/>
-      <c r="P23" s="360"/>
-      <c r="Q23" s="360"/>
-      <c r="R23" s="360"/>
-      <c r="S23" s="360"/>
-      <c r="T23" s="360"/>
-      <c r="U23" s="360"/>
-      <c r="V23" s="360"/>
-      <c r="W23" s="360"/>
+      <c r="B23" s="366"/>
+      <c r="C23" s="366"/>
+      <c r="D23" s="366"/>
+      <c r="E23" s="366"/>
+      <c r="F23" s="366"/>
+      <c r="G23" s="366"/>
+      <c r="H23" s="366"/>
+      <c r="I23" s="366"/>
+      <c r="J23" s="366"/>
+      <c r="K23" s="366"/>
+      <c r="L23" s="366"/>
+      <c r="M23" s="366"/>
+      <c r="N23" s="366"/>
+      <c r="O23" s="366"/>
+      <c r="P23" s="366"/>
+      <c r="Q23" s="366"/>
+      <c r="R23" s="366"/>
+      <c r="S23" s="366"/>
+      <c r="T23" s="366"/>
+      <c r="U23" s="366"/>
+      <c r="V23" s="366"/>
+      <c r="W23" s="366"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -15926,29 +15926,29 @@
     <row r="9" spans="1:31" ht="18">
       <c r="A9" s="77"/>
       <c r="B9" s="267"/>
-      <c r="C9" s="325" t="s">
+      <c r="C9" s="331" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="325"/>
-      <c r="E9" s="325"/>
-      <c r="F9" s="325"/>
-      <c r="G9" s="325"/>
+      <c r="D9" s="331"/>
+      <c r="E9" s="331"/>
+      <c r="F9" s="331"/>
+      <c r="G9" s="331"/>
       <c r="H9" s="28"/>
-      <c r="I9" s="325" t="s">
+      <c r="I9" s="331" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="325"/>
-      <c r="K9" s="325"/>
-      <c r="L9" s="325"/>
-      <c r="M9" s="325"/>
-      <c r="N9" s="325"/>
-      <c r="O9" s="325"/>
-      <c r="P9" s="325"/>
-      <c r="Q9" s="325"/>
-      <c r="R9" s="325"/>
-      <c r="S9" s="325"/>
-      <c r="T9" s="325"/>
-      <c r="U9" s="325"/>
+      <c r="J9" s="331"/>
+      <c r="K9" s="331"/>
+      <c r="L9" s="331"/>
+      <c r="M9" s="331"/>
+      <c r="N9" s="331"/>
+      <c r="O9" s="331"/>
+      <c r="P9" s="331"/>
+      <c r="Q9" s="331"/>
+      <c r="R9" s="331"/>
+      <c r="S9" s="331"/>
+      <c r="T9" s="331"/>
+      <c r="U9" s="331"/>
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
       <c r="X9" s="13"/>
@@ -15963,45 +15963,45 @@
     <row r="10" spans="1:31" ht="14.55" customHeight="1">
       <c r="A10" s="78"/>
       <c r="B10" s="78"/>
-      <c r="C10" s="326" t="s">
+      <c r="C10" s="332" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="326" t="s">
+      <c r="D10" s="332" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="320" t="s">
+      <c r="E10" s="326" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="320" t="s">
+      <c r="F10" s="326" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="320" t="s">
+      <c r="G10" s="326" t="s">
         <v>85</v>
       </c>
       <c r="H10" s="54"/>
-      <c r="I10" s="320" t="s">
+      <c r="I10" s="326" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="320"/>
+      <c r="J10" s="326"/>
       <c r="K10" s="258"/>
-      <c r="L10" s="320" t="s">
+      <c r="L10" s="326" t="s">
         <v>228</v>
       </c>
-      <c r="M10" s="320"/>
+      <c r="M10" s="326"/>
       <c r="N10" s="258"/>
-      <c r="O10" s="329" t="s">
+      <c r="O10" s="335" t="s">
         <v>455</v>
       </c>
       <c r="P10" s="258"/>
-      <c r="Q10" s="320" t="s">
+      <c r="Q10" s="326" t="s">
         <v>84</v>
       </c>
-      <c r="R10" s="320"/>
+      <c r="R10" s="326"/>
       <c r="S10" s="258"/>
-      <c r="T10" s="320" t="s">
+      <c r="T10" s="326" t="s">
         <v>85</v>
       </c>
-      <c r="U10" s="320"/>
+      <c r="U10" s="326"/>
       <c r="V10" s="45"/>
       <c r="W10" s="45"/>
       <c r="X10" s="45"/>
@@ -16020,11 +16020,11 @@
       <c r="B11" s="78" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="327"/>
-      <c r="D11" s="327"/>
-      <c r="E11" s="328"/>
-      <c r="F11" s="328"/>
-      <c r="G11" s="328"/>
+      <c r="C11" s="333"/>
+      <c r="D11" s="333"/>
+      <c r="E11" s="334"/>
+      <c r="F11" s="334"/>
+      <c r="G11" s="334"/>
       <c r="H11" s="29"/>
       <c r="I11" s="100">
         <v>2018</v>
@@ -16040,7 +16040,7 @@
         <v>2023</v>
       </c>
       <c r="N11" s="101"/>
-      <c r="O11" s="330"/>
+      <c r="O11" s="336"/>
       <c r="P11" s="101"/>
       <c r="Q11" s="100">
         <v>2018</v>
@@ -17066,7 +17066,7 @@
       <c r="AE30" s="13"/>
     </row>
     <row r="31" spans="1:31" ht="25.5" customHeight="1">
-      <c r="A31" s="322" t="s">
+      <c r="A31" s="328" t="s">
         <v>199</v>
       </c>
       <c r="B31" s="83" t="s">
@@ -17127,7 +17127,7 @@
       <c r="AE31" s="13"/>
     </row>
     <row r="32" spans="1:31" ht="25.5" customHeight="1">
-      <c r="A32" s="323"/>
+      <c r="A32" s="329"/>
       <c r="B32" s="83" t="s">
         <v>201</v>
       </c>
@@ -17185,7 +17185,7 @@
       <c r="AE32" s="13"/>
     </row>
     <row r="33" spans="1:31" ht="25.5" customHeight="1">
-      <c r="A33" s="324"/>
+      <c r="A33" s="330"/>
       <c r="B33" s="83" t="s">
         <v>204</v>
       </c>
@@ -17874,29 +17874,29 @@
       <c r="AE49" s="13"/>
     </row>
     <row r="50" spans="1:31" ht="15" customHeight="1">
-      <c r="A50" s="321" t="s">
+      <c r="A50" s="327" t="s">
         <v>263</v>
       </c>
-      <c r="B50" s="321"/>
-      <c r="C50" s="321"/>
-      <c r="D50" s="321"/>
-      <c r="E50" s="321"/>
-      <c r="F50" s="321"/>
-      <c r="G50" s="321"/>
-      <c r="H50" s="321"/>
-      <c r="I50" s="321"/>
-      <c r="J50" s="321"/>
-      <c r="K50" s="321"/>
-      <c r="L50" s="321"/>
-      <c r="M50" s="321"/>
-      <c r="N50" s="321"/>
-      <c r="O50" s="321"/>
-      <c r="P50" s="321"/>
-      <c r="Q50" s="321"/>
-      <c r="R50" s="321"/>
-      <c r="S50" s="321"/>
-      <c r="T50" s="321"/>
-      <c r="U50" s="321"/>
+      <c r="B50" s="327"/>
+      <c r="C50" s="327"/>
+      <c r="D50" s="327"/>
+      <c r="E50" s="327"/>
+      <c r="F50" s="327"/>
+      <c r="G50" s="327"/>
+      <c r="H50" s="327"/>
+      <c r="I50" s="327"/>
+      <c r="J50" s="327"/>
+      <c r="K50" s="327"/>
+      <c r="L50" s="327"/>
+      <c r="M50" s="327"/>
+      <c r="N50" s="327"/>
+      <c r="O50" s="327"/>
+      <c r="P50" s="327"/>
+      <c r="Q50" s="327"/>
+      <c r="R50" s="327"/>
+      <c r="S50" s="327"/>
+      <c r="T50" s="327"/>
+      <c r="U50" s="327"/>
       <c r="V50" s="69"/>
       <c r="W50" s="13"/>
       <c r="X50" s="13"/>
@@ -17909,27 +17909,27 @@
       <c r="AE50" s="13"/>
     </row>
     <row r="51" spans="1:31" ht="15" customHeight="1">
-      <c r="A51" s="321"/>
-      <c r="B51" s="321"/>
-      <c r="C51" s="321"/>
-      <c r="D51" s="321"/>
-      <c r="E51" s="321"/>
-      <c r="F51" s="321"/>
-      <c r="G51" s="321"/>
-      <c r="H51" s="321"/>
-      <c r="I51" s="321"/>
-      <c r="J51" s="321"/>
-      <c r="K51" s="321"/>
-      <c r="L51" s="321"/>
-      <c r="M51" s="321"/>
-      <c r="N51" s="321"/>
-      <c r="O51" s="321"/>
-      <c r="P51" s="321"/>
-      <c r="Q51" s="321"/>
-      <c r="R51" s="321"/>
-      <c r="S51" s="321"/>
-      <c r="T51" s="321"/>
-      <c r="U51" s="321"/>
+      <c r="A51" s="327"/>
+      <c r="B51" s="327"/>
+      <c r="C51" s="327"/>
+      <c r="D51" s="327"/>
+      <c r="E51" s="327"/>
+      <c r="F51" s="327"/>
+      <c r="G51" s="327"/>
+      <c r="H51" s="327"/>
+      <c r="I51" s="327"/>
+      <c r="J51" s="327"/>
+      <c r="K51" s="327"/>
+      <c r="L51" s="327"/>
+      <c r="M51" s="327"/>
+      <c r="N51" s="327"/>
+      <c r="O51" s="327"/>
+      <c r="P51" s="327"/>
+      <c r="Q51" s="327"/>
+      <c r="R51" s="327"/>
+      <c r="S51" s="327"/>
+      <c r="T51" s="327"/>
+      <c r="U51" s="327"/>
       <c r="V51" s="69"/>
       <c r="W51" s="13"/>
       <c r="X51" s="13"/>
@@ -17942,27 +17942,27 @@
       <c r="AE51" s="13"/>
     </row>
     <row r="52" spans="1:31" ht="15" customHeight="1">
-      <c r="A52" s="321"/>
-      <c r="B52" s="321"/>
-      <c r="C52" s="321"/>
-      <c r="D52" s="321"/>
-      <c r="E52" s="321"/>
-      <c r="F52" s="321"/>
-      <c r="G52" s="321"/>
-      <c r="H52" s="321"/>
-      <c r="I52" s="321"/>
-      <c r="J52" s="321"/>
-      <c r="K52" s="321"/>
-      <c r="L52" s="321"/>
-      <c r="M52" s="321"/>
-      <c r="N52" s="321"/>
-      <c r="O52" s="321"/>
-      <c r="P52" s="321"/>
-      <c r="Q52" s="321"/>
-      <c r="R52" s="321"/>
-      <c r="S52" s="321"/>
-      <c r="T52" s="321"/>
-      <c r="U52" s="321"/>
+      <c r="A52" s="327"/>
+      <c r="B52" s="327"/>
+      <c r="C52" s="327"/>
+      <c r="D52" s="327"/>
+      <c r="E52" s="327"/>
+      <c r="F52" s="327"/>
+      <c r="G52" s="327"/>
+      <c r="H52" s="327"/>
+      <c r="I52" s="327"/>
+      <c r="J52" s="327"/>
+      <c r="K52" s="327"/>
+      <c r="L52" s="327"/>
+      <c r="M52" s="327"/>
+      <c r="N52" s="327"/>
+      <c r="O52" s="327"/>
+      <c r="P52" s="327"/>
+      <c r="Q52" s="327"/>
+      <c r="R52" s="327"/>
+      <c r="S52" s="327"/>
+      <c r="T52" s="327"/>
+      <c r="U52" s="327"/>
       <c r="V52" s="69"/>
       <c r="W52" s="13"/>
       <c r="X52" s="13"/>
@@ -18814,35 +18814,35 @@
     </row>
     <row r="4" spans="1:39" ht="15" customHeight="1">
       <c r="A4" s="13"/>
-      <c r="B4" s="331" t="s">
+      <c r="B4" s="337" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="333" t="s">
+      <c r="C4" s="339" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="333"/>
-      <c r="E4" s="333"/>
-      <c r="F4" s="333"/>
-      <c r="G4" s="333"/>
-      <c r="H4" s="333"/>
-      <c r="I4" s="333"/>
-      <c r="J4" s="333"/>
-      <c r="K4" s="333"/>
-      <c r="L4" s="333"/>
-      <c r="M4" s="333"/>
-      <c r="N4" s="333"/>
-      <c r="O4" s="333"/>
-      <c r="P4" s="333"/>
-      <c r="Q4" s="333"/>
-      <c r="R4" s="333"/>
-      <c r="S4" s="333"/>
-      <c r="T4" s="333"/>
-      <c r="U4" s="333"/>
-      <c r="V4" s="333"/>
-      <c r="W4" s="333"/>
-      <c r="X4" s="333"/>
-      <c r="Y4" s="333"/>
-      <c r="Z4" s="333"/>
+      <c r="D4" s="339"/>
+      <c r="E4" s="339"/>
+      <c r="F4" s="339"/>
+      <c r="G4" s="339"/>
+      <c r="H4" s="339"/>
+      <c r="I4" s="339"/>
+      <c r="J4" s="339"/>
+      <c r="K4" s="339"/>
+      <c r="L4" s="339"/>
+      <c r="M4" s="339"/>
+      <c r="N4" s="339"/>
+      <c r="O4" s="339"/>
+      <c r="P4" s="339"/>
+      <c r="Q4" s="339"/>
+      <c r="R4" s="339"/>
+      <c r="S4" s="339"/>
+      <c r="T4" s="339"/>
+      <c r="U4" s="339"/>
+      <c r="V4" s="339"/>
+      <c r="W4" s="339"/>
+      <c r="X4" s="339"/>
+      <c r="Y4" s="339"/>
+      <c r="Z4" s="339"/>
       <c r="AA4" s="13"/>
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
@@ -18859,7 +18859,7 @@
     </row>
     <row r="5" spans="1:39">
       <c r="A5" s="13"/>
-      <c r="B5" s="332"/>
+      <c r="B5" s="338"/>
       <c r="C5" s="76" t="s">
         <v>127</v>
       </c>
@@ -20152,30 +20152,30 @@
       </c>
     </row>
     <row r="25" spans="2:26">
-      <c r="B25" s="334" t="s">
+      <c r="B25" s="340" t="s">
         <v>149</v>
       </c>
-      <c r="C25" s="334"/>
-      <c r="D25" s="334"/>
-      <c r="E25" s="334"/>
-      <c r="F25" s="334"/>
-      <c r="G25" s="334"/>
-      <c r="H25" s="334"/>
-      <c r="I25" s="334"/>
-      <c r="J25" s="334"/>
-      <c r="K25" s="334"/>
-      <c r="L25" s="334"/>
-      <c r="M25" s="334"/>
-      <c r="N25" s="334"/>
-      <c r="O25" s="334"/>
-      <c r="P25" s="334"/>
-      <c r="Q25" s="334"/>
-      <c r="R25" s="334"/>
-      <c r="S25" s="334"/>
-      <c r="T25" s="334"/>
-      <c r="U25" s="334"/>
-      <c r="V25" s="334"/>
-      <c r="W25" s="334"/>
+      <c r="C25" s="340"/>
+      <c r="D25" s="340"/>
+      <c r="E25" s="340"/>
+      <c r="F25" s="340"/>
+      <c r="G25" s="340"/>
+      <c r="H25" s="340"/>
+      <c r="I25" s="340"/>
+      <c r="J25" s="340"/>
+      <c r="K25" s="340"/>
+      <c r="L25" s="340"/>
+      <c r="M25" s="340"/>
+      <c r="N25" s="340"/>
+      <c r="O25" s="340"/>
+      <c r="P25" s="340"/>
+      <c r="Q25" s="340"/>
+      <c r="R25" s="340"/>
+      <c r="S25" s="340"/>
+      <c r="T25" s="340"/>
+      <c r="U25" s="340"/>
+      <c r="V25" s="340"/>
+      <c r="W25" s="340"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -21186,11 +21186,11 @@
         <f>F47/1000</f>
         <v>0</v>
       </c>
-      <c r="H5" s="339" t="s">
+      <c r="H5" s="341" t="s">
         <v>152</v>
       </c>
-      <c r="I5" s="340"/>
-      <c r="J5" s="340"/>
+      <c r="I5" s="342"/>
+      <c r="J5" s="342"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
@@ -21226,11 +21226,11 @@
         <f>F48</f>
         <v>0</v>
       </c>
-      <c r="H6" s="339" t="s">
+      <c r="H6" s="341" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="340"/>
-      <c r="J6" s="340"/>
+      <c r="I6" s="342"/>
+      <c r="J6" s="342"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -21266,11 +21266,11 @@
         <f>F49/1000</f>
         <v>0</v>
       </c>
-      <c r="H7" s="339" t="s">
+      <c r="H7" s="341" t="s">
         <v>152</v>
       </c>
-      <c r="I7" s="340"/>
-      <c r="J7" s="340"/>
+      <c r="I7" s="342"/>
+      <c r="J7" s="342"/>
       <c r="K7" s="67"/>
       <c r="L7" s="67"/>
       <c r="M7" s="67"/>
@@ -21327,31 +21327,31 @@
       <c r="AE8" s="13"/>
     </row>
     <row r="9" spans="1:31" ht="15" customHeight="1">
-      <c r="A9" s="342" t="s">
+      <c r="A9" s="344" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="342"/>
-      <c r="C9" s="338" t="s">
+      <c r="B9" s="344"/>
+      <c r="C9" s="346" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="338"/>
-      <c r="E9" s="338"/>
-      <c r="F9" s="338"/>
-      <c r="G9" s="338"/>
+      <c r="D9" s="346"/>
+      <c r="E9" s="346"/>
+      <c r="F9" s="346"/>
+      <c r="G9" s="346"/>
       <c r="H9" s="157"/>
-      <c r="I9" s="341" t="s">
+      <c r="I9" s="343" t="s">
         <v>153</v>
       </c>
-      <c r="J9" s="341"/>
-      <c r="K9" s="341"/>
-      <c r="L9" s="341"/>
-      <c r="M9" s="341"/>
-      <c r="N9" s="341"/>
-      <c r="O9" s="341"/>
-      <c r="P9" s="341"/>
-      <c r="Q9" s="341"/>
-      <c r="R9" s="341"/>
-      <c r="S9" s="341"/>
+      <c r="J9" s="343"/>
+      <c r="K9" s="343"/>
+      <c r="L9" s="343"/>
+      <c r="M9" s="343"/>
+      <c r="N9" s="343"/>
+      <c r="O9" s="343"/>
+      <c r="P9" s="343"/>
+      <c r="Q9" s="343"/>
+      <c r="R9" s="343"/>
+      <c r="S9" s="343"/>
       <c r="T9" s="116"/>
       <c r="U9" s="116"/>
       <c r="V9" s="116"/>
@@ -21366,47 +21366,47 @@
       <c r="AE9" s="13"/>
     </row>
     <row r="10" spans="1:31">
-      <c r="A10" s="336" t="s">
+      <c r="A10" s="345" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="336" t="s">
+      <c r="B10" s="345" t="s">
         <v>270</v>
       </c>
-      <c r="C10" s="337" t="s">
+      <c r="C10" s="348" t="s">
         <v>268</v>
       </c>
-      <c r="D10" s="336" t="s">
+      <c r="D10" s="345" t="s">
         <v>269</v>
       </c>
-      <c r="E10" s="337" t="s">
+      <c r="E10" s="348" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="337" t="s">
+      <c r="F10" s="348" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="336" t="s">
+      <c r="G10" s="345" t="s">
         <v>154</v>
       </c>
       <c r="H10" s="128"/>
-      <c r="I10" s="335" t="s">
+      <c r="I10" s="347" t="s">
         <v>268</v>
       </c>
-      <c r="J10" s="335"/>
+      <c r="J10" s="347"/>
       <c r="K10" s="133"/>
-      <c r="L10" s="335" t="s">
+      <c r="L10" s="347" t="s">
         <v>269</v>
       </c>
-      <c r="M10" s="335"/>
+      <c r="M10" s="347"/>
       <c r="N10" s="133"/>
-      <c r="O10" s="335" t="s">
+      <c r="O10" s="347" t="s">
         <v>84</v>
       </c>
-      <c r="P10" s="335"/>
+      <c r="P10" s="347"/>
       <c r="Q10" s="133"/>
-      <c r="R10" s="335" t="s">
+      <c r="R10" s="347" t="s">
         <v>85</v>
       </c>
-      <c r="S10" s="335"/>
+      <c r="S10" s="347"/>
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
       <c r="AA10" s="13"/>
@@ -21416,13 +21416,13 @@
       <c r="AE10" s="13"/>
     </row>
     <row r="11" spans="1:31">
-      <c r="A11" s="336"/>
-      <c r="B11" s="336"/>
-      <c r="C11" s="337"/>
-      <c r="D11" s="336"/>
-      <c r="E11" s="337"/>
-      <c r="F11" s="337"/>
-      <c r="G11" s="336"/>
+      <c r="A11" s="345"/>
+      <c r="B11" s="345"/>
+      <c r="C11" s="348"/>
+      <c r="D11" s="345"/>
+      <c r="E11" s="348"/>
+      <c r="F11" s="348"/>
+      <c r="G11" s="345"/>
       <c r="H11" s="128"/>
       <c r="I11" s="132">
         <v>2018</v>
@@ -23579,16 +23579,6 @@
     <row r="83" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="I9:S9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="O10:P10"/>
     <mergeCell ref="R10:S10"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="B10:B11"/>
@@ -23596,6 +23586,16 @@
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="I9:S9"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="D13:D25 L13:M25">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
@@ -23721,35 +23721,35 @@
     </row>
     <row r="4" spans="1:39" ht="15" customHeight="1">
       <c r="A4" s="13"/>
-      <c r="B4" s="343" t="s">
+      <c r="B4" s="349" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="345" t="s">
+      <c r="C4" s="351" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="345"/>
-      <c r="E4" s="345"/>
-      <c r="F4" s="345"/>
-      <c r="G4" s="345"/>
-      <c r="H4" s="345"/>
-      <c r="I4" s="345"/>
-      <c r="J4" s="345"/>
-      <c r="K4" s="345"/>
-      <c r="L4" s="345"/>
-      <c r="M4" s="345"/>
-      <c r="N4" s="345"/>
-      <c r="O4" s="345"/>
-      <c r="P4" s="345"/>
-      <c r="Q4" s="345"/>
-      <c r="R4" s="345"/>
-      <c r="S4" s="345"/>
-      <c r="T4" s="345"/>
-      <c r="U4" s="345"/>
-      <c r="V4" s="345"/>
-      <c r="W4" s="345"/>
-      <c r="X4" s="345"/>
-      <c r="Y4" s="345"/>
-      <c r="Z4" s="345"/>
+      <c r="D4" s="351"/>
+      <c r="E4" s="351"/>
+      <c r="F4" s="351"/>
+      <c r="G4" s="351"/>
+      <c r="H4" s="351"/>
+      <c r="I4" s="351"/>
+      <c r="J4" s="351"/>
+      <c r="K4" s="351"/>
+      <c r="L4" s="351"/>
+      <c r="M4" s="351"/>
+      <c r="N4" s="351"/>
+      <c r="O4" s="351"/>
+      <c r="P4" s="351"/>
+      <c r="Q4" s="351"/>
+      <c r="R4" s="351"/>
+      <c r="S4" s="351"/>
+      <c r="T4" s="351"/>
+      <c r="U4" s="351"/>
+      <c r="V4" s="351"/>
+      <c r="W4" s="351"/>
+      <c r="X4" s="351"/>
+      <c r="Y4" s="351"/>
+      <c r="Z4" s="351"/>
       <c r="AA4" s="13"/>
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
@@ -23766,7 +23766,7 @@
     </row>
     <row r="5" spans="1:39">
       <c r="A5" s="13"/>
-      <c r="B5" s="344"/>
+      <c r="B5" s="350"/>
       <c r="C5" s="173" t="s">
         <v>127</v>
       </c>
@@ -25776,6 +25776,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FB6FBD5E95BAB542B810C32545CA4E3B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c88f4da8c98e9c6f14dc759bd92b3b9d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f244dd4c-ee25-4b14-a7cd-a89d47e877b9" xmlns:ns4="7d5efbb1-7b5c-4600-961f-d0c91f173691" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11dd0c1a7b4f1799f1daf73497fb7c0" ns3:_="" ns4:_="">
     <xsd:import namespace="f244dd4c-ee25-4b14-a7cd-a89d47e877b9"/>
@@ -25986,12 +25992,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5668EAE9-BE2F-449B-83FE-5638B2ED2DF4}">
   <ds:schemaRefs>
@@ -26001,6 +26001,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C5798F-31D9-455C-A266-3CF2A88C6872}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7d5efbb1-7b5c-4600-961f-d0c91f173691"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f244dd4c-ee25-4b14-a7cd-a89d47e877b9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B491DB35-4E91-4B2D-816E-03001B21F1D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26017,21 +26034,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C5798F-31D9-455C-A266-3CF2A88C6872}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7d5efbb1-7b5c-4600-961f-d0c91f173691"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f244dd4c-ee25-4b14-a7cd-a89d47e877b9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>